<commit_message>
added game display requirement to the excel
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyncthingServiceAcct\school work\2025\Spring 2025\CSE 3310 FUNDAMENTALS OF SOFTWARE ENGR\cse3310-sp25-004\FinalRequirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15176dbdb68e5a3b/Desktop/CSE3310/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE3C0BA-C38D-42CB-BB42-145B56C6D64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{7AE3C0BA-C38D-42CB-BB42-145B56C6D64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C73C20-20AA-41CF-8CF6-30C58CAD13C3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="13170" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="642">
   <si>
     <t>Tested By</t>
   </si>
@@ -1863,6 +1863,96 @@
   </si>
   <si>
     <t>PG - 37</t>
+  </si>
+  <si>
+    <t>GD - 1</t>
+  </si>
+  <si>
+    <t>Game Display - 3</t>
+  </si>
+  <si>
+    <t>Game Display shall display board with appropriate places</t>
+  </si>
+  <si>
+    <t>createBoard()</t>
+  </si>
+  <si>
+    <t>GD - 2</t>
+  </si>
+  <si>
+    <t>Game display shall communicate with Page Manager through web sockets</t>
+  </si>
+  <si>
+    <t>socket.js</t>
+  </si>
+  <si>
+    <t>GD - 3</t>
+  </si>
+  <si>
+    <t>Game Display shall display the piece movement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">handleClick(clickedId), movePiece(fromId, toId), </t>
+  </si>
+  <si>
+    <t>GD - 4</t>
+  </si>
+  <si>
+    <t>Game Display shall display the current players of the game</t>
+  </si>
+  <si>
+    <t>updatePlayerTurn(), switchPlayer()</t>
+  </si>
+  <si>
+    <t>GD - 5</t>
+  </si>
+  <si>
+    <t>game Display shall have a log that dislays the history of moves as well as status of the game</t>
+  </si>
+  <si>
+    <t>addLog(message, type='info')</t>
+  </si>
+  <si>
+    <t>GD - 6</t>
+  </si>
+  <si>
+    <t>Game Display shall allow users to quit and request draw with buttons</t>
+  </si>
+  <si>
+    <t>quitGame(), sendDrawRequest()</t>
+  </si>
+  <si>
+    <t>GD - 7</t>
+  </si>
+  <si>
+    <t>Game Display shall allow users to move pieces</t>
+  </si>
+  <si>
+    <t>movePiece(fromId, toId), handleClick(clickedId), sendGameMove(fromId, toId)</t>
+  </si>
+  <si>
+    <t>GD - 8</t>
+  </si>
+  <si>
+    <t>Game Display shall show whose turn it is</t>
+  </si>
+  <si>
+    <t>GD - 9</t>
+  </si>
+  <si>
+    <t>Game Display Shall validate if a move is legal with backend before executing</t>
+  </si>
+  <si>
+    <t>sendGameMove(fromtId, toId)</t>
+  </si>
+  <si>
+    <t>GD - 10</t>
+  </si>
+  <si>
+    <t>Game Display shall remove caputred pieces from the board upon successful jump</t>
+  </si>
+  <si>
+    <t>handleMoveResult(moveData)</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2089,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2036,19 +2126,20 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Neutral" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2311,33 +2402,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S211"/>
+  <dimension ref="A1:S221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView tabSelected="1" topLeftCell="C209" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="36.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="123.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="2" customWidth="1"/>
-    <col min="7" max="16" width="8.6640625" style="1"/>
-    <col min="17" max="17" width="8.6640625" style="3"/>
-    <col min="18" max="18" width="8.6640625" style="1"/>
-    <col min="19" max="19" width="36.44140625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="123.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
+    <col min="7" max="16" width="8.7109375" style="1"/>
+    <col min="17" max="17" width="8.7109375" style="3"/>
+    <col min="18" max="18" width="8.7109375" style="1"/>
+    <col min="19" max="19" width="36.42578125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2375,7 +2466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2395,7 +2486,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2418,7 +2509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2426,27 +2517,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -2460,7 +2551,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -2474,7 +2565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2488,7 +2579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2502,7 +2593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
@@ -2516,7 +2607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -2530,7 +2621,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>41</v>
       </c>
@@ -2544,7 +2635,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -2558,7 +2649,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>46</v>
       </c>
@@ -2572,7 +2663,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2586,7 +2677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
@@ -2600,7 +2691,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>54</v>
       </c>
@@ -2614,7 +2705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>57</v>
       </c>
@@ -2628,7 +2719,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>59</v>
       </c>
@@ -2642,7 +2733,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -2657,7 +2748,7 @@
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2672,7 +2763,7 @@
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -2687,7 +2778,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -2702,7 +2793,7 @@
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
@@ -2719,7 +2810,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -2734,7 +2825,7 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -2750,7 +2841,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>85</v>
       </c>
@@ -2767,7 +2858,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
@@ -2784,7 +2875,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -2798,7 +2889,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -2812,7 +2903,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>98</v>
       </c>
@@ -2826,7 +2917,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>101</v>
       </c>
@@ -2840,7 +2931,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -2854,7 +2945,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>107</v>
       </c>
@@ -2868,7 +2959,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
@@ -2882,7 +2973,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>112</v>
       </c>
@@ -2896,7 +2987,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -2910,7 +3001,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>118</v>
       </c>
@@ -2924,7 +3015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>121</v>
       </c>
@@ -2938,7 +3029,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -2952,7 +3043,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
@@ -2966,7 +3057,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>131</v>
       </c>
@@ -2980,7 +3071,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>134</v>
       </c>
@@ -2994,7 +3085,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -3008,7 +3099,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
@@ -3022,7 +3113,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>143</v>
       </c>
@@ -3036,7 +3127,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>146</v>
       </c>
@@ -3050,7 +3141,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>149</v>
       </c>
@@ -3064,7 +3155,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>151</v>
       </c>
@@ -3078,7 +3169,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>153</v>
       </c>
@@ -3092,7 +3183,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>155</v>
       </c>
@@ -3106,7 +3197,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>157</v>
       </c>
@@ -3120,7 +3211,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>159</v>
       </c>
@@ -3137,7 +3228,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -3151,7 +3242,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>168</v>
       </c>
@@ -3165,7 +3256,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>172</v>
       </c>
@@ -3179,7 +3270,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -3193,7 +3284,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>180</v>
       </c>
@@ -3207,7 +3298,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
@@ -3221,7 +3312,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>188</v>
       </c>
@@ -3235,7 +3326,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>192</v>
       </c>
@@ -3249,7 +3340,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>196</v>
       </c>
@@ -3263,7 +3354,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>199</v>
       </c>
@@ -3277,7 +3368,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>202</v>
       </c>
@@ -3291,7 +3382,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>205</v>
       </c>
@@ -3305,7 +3396,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>208</v>
       </c>
@@ -3319,7 +3410,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>211</v>
       </c>
@@ -3333,7 +3424,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>214</v>
       </c>
@@ -3347,7 +3438,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>217</v>
       </c>
@@ -3361,7 +3452,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>221</v>
       </c>
@@ -3375,7 +3466,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>225</v>
       </c>
@@ -3389,7 +3480,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>229</v>
       </c>
@@ -3403,7 +3494,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>232</v>
       </c>
@@ -3417,7 +3508,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>235</v>
       </c>
@@ -3431,7 +3522,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>238</v>
       </c>
@@ -3445,7 +3536,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>242</v>
       </c>
@@ -3459,7 +3550,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>245</v>
       </c>
@@ -3473,7 +3564,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>248</v>
       </c>
@@ -3487,7 +3578,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>251</v>
       </c>
@@ -3501,7 +3592,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>254</v>
       </c>
@@ -3515,7 +3606,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>257</v>
       </c>
@@ -3529,7 +3620,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>260</v>
       </c>
@@ -3543,7 +3634,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>263</v>
       </c>
@@ -3557,7 +3648,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>266</v>
       </c>
@@ -3571,7 +3662,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>269</v>
       </c>
@@ -3585,7 +3676,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>272</v>
       </c>
@@ -3599,7 +3690,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>275</v>
       </c>
@@ -3613,7 +3704,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>279</v>
       </c>
@@ -3627,7 +3718,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>281</v>
       </c>
@@ -3641,7 +3732,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>285</v>
       </c>
@@ -3655,7 +3746,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>287</v>
       </c>
@@ -3669,7 +3760,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>290</v>
       </c>
@@ -3683,7 +3774,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>293</v>
       </c>
@@ -3697,7 +3788,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>296</v>
       </c>
@@ -3711,7 +3802,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>299</v>
       </c>
@@ -3725,7 +3816,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>302</v>
       </c>
@@ -3739,7 +3830,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>305</v>
       </c>
@@ -3753,7 +3844,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>307</v>
       </c>
@@ -3767,7 +3858,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>309</v>
       </c>
@@ -3781,7 +3872,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>312</v>
       </c>
@@ -3795,7 +3886,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>315</v>
       </c>
@@ -3809,7 +3900,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>318</v>
       </c>
@@ -3823,7 +3914,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>320</v>
       </c>
@@ -3837,7 +3928,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>324</v>
       </c>
@@ -3851,7 +3942,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>326</v>
       </c>
@@ -3865,7 +3956,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>329</v>
       </c>
@@ -3879,7 +3970,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>331</v>
       </c>
@@ -3893,7 +3984,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>333</v>
       </c>
@@ -3907,7 +3998,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>335</v>
       </c>
@@ -3921,7 +4012,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>338</v>
       </c>
@@ -3935,7 +4026,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>340</v>
       </c>
@@ -3949,7 +4040,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>342</v>
       </c>
@@ -3963,7 +4054,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>345</v>
       </c>
@@ -3977,7 +4068,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>347</v>
       </c>
@@ -3991,7 +4082,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>349</v>
       </c>
@@ -4005,7 +4096,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>351</v>
       </c>
@@ -4019,7 +4110,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>353</v>
       </c>
@@ -4033,7 +4124,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>356</v>
       </c>
@@ -4047,7 +4138,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>358</v>
       </c>
@@ -4061,7 +4152,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>360</v>
       </c>
@@ -4075,7 +4166,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>362</v>
       </c>
@@ -4089,7 +4180,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>364</v>
       </c>
@@ -4103,7 +4194,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
         <v>366</v>
       </c>
@@ -4117,7 +4208,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
         <v>370</v>
       </c>
@@ -4131,7 +4222,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>373</v>
       </c>
@@ -4145,7 +4236,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>376</v>
       </c>
@@ -4159,7 +4250,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>378</v>
       </c>
@@ -4173,7 +4264,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>381</v>
       </c>
@@ -4187,7 +4278,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>384</v>
       </c>
@@ -4201,7 +4292,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>387</v>
       </c>
@@ -4215,7 +4306,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>390</v>
       </c>
@@ -4229,7 +4320,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>393</v>
       </c>
@@ -4243,7 +4334,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>396</v>
       </c>
@@ -4257,7 +4348,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>399</v>
       </c>
@@ -4271,7 +4362,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>402</v>
       </c>
@@ -4285,7 +4376,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>406</v>
       </c>
@@ -4299,7 +4390,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="16" t="s">
         <v>409</v>
       </c>
@@ -4313,7 +4404,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="16" t="s">
         <v>411</v>
       </c>
@@ -4327,7 +4418,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="16" t="s">
         <v>412</v>
       </c>
@@ -4341,7 +4432,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="16" t="s">
         <v>413</v>
       </c>
@@ -4355,7 +4446,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="16" t="s">
         <v>414</v>
       </c>
@@ -4369,7 +4460,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="16" t="s">
         <v>415</v>
       </c>
@@ -4383,7 +4474,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="16" t="s">
         <v>416</v>
       </c>
@@ -4397,7 +4488,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="16" t="s">
         <v>417</v>
       </c>
@@ -4411,7 +4502,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="16" t="s">
         <v>418</v>
       </c>
@@ -4425,7 +4516,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
         <v>419</v>
       </c>
@@ -4439,7 +4530,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="16" t="s">
         <v>442</v>
       </c>
@@ -4453,7 +4544,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
         <v>443</v>
       </c>
@@ -4467,7 +4558,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>483</v>
       </c>
@@ -4481,7 +4572,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>484</v>
       </c>
@@ -4495,7 +4586,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>485</v>
       </c>
@@ -4509,7 +4600,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>486</v>
       </c>
@@ -4523,7 +4614,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>487</v>
       </c>
@@ -4537,7 +4628,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>488</v>
       </c>
@@ -4551,7 +4642,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>489</v>
       </c>
@@ -4565,7 +4656,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>490</v>
       </c>
@@ -4579,7 +4670,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>491</v>
       </c>
@@ -4593,7 +4684,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>492</v>
       </c>
@@ -4607,7 +4698,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>493</v>
       </c>
@@ -4621,7 +4712,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>494</v>
       </c>
@@ -4635,7 +4726,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>495</v>
       </c>
@@ -4649,7 +4740,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>496</v>
       </c>
@@ -4663,7 +4754,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>497</v>
       </c>
@@ -4677,7 +4768,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>498</v>
       </c>
@@ -4691,7 +4782,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>499</v>
       </c>
@@ -4705,7 +4796,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>500</v>
       </c>
@@ -4719,7 +4810,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>501</v>
       </c>
@@ -4733,7 +4824,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>502</v>
       </c>
@@ -4747,7 +4838,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>503</v>
       </c>
@@ -4761,7 +4852,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A175" s="22" t="s">
         <v>575</v>
       </c>
@@ -4775,7 +4866,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A176" s="22" t="s">
         <v>576</v>
       </c>
@@ -4789,7 +4880,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A177" s="22" t="s">
         <v>577</v>
       </c>
@@ -4803,7 +4894,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A178" s="22" t="s">
         <v>578</v>
       </c>
@@ -4817,7 +4908,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A179" s="22" t="s">
         <v>579</v>
       </c>
@@ -4831,7 +4922,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A180" s="22" t="s">
         <v>580</v>
       </c>
@@ -4845,7 +4936,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="22" t="s">
         <v>581</v>
       </c>
@@ -4859,7 +4950,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="22" t="s">
         <v>582</v>
       </c>
@@ -4873,7 +4964,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="22" t="s">
         <v>583</v>
       </c>
@@ -4887,7 +4978,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="22" t="s">
         <v>584</v>
       </c>
@@ -4901,7 +4992,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="22" t="s">
         <v>585</v>
       </c>
@@ -4915,7 +5006,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A186" s="22" t="s">
         <v>586</v>
       </c>
@@ -4929,7 +5020,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A187" s="22" t="s">
         <v>587</v>
       </c>
@@ -4943,7 +5034,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A188" s="22" t="s">
         <v>588</v>
       </c>
@@ -4957,7 +5048,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A189" s="22" t="s">
         <v>589</v>
       </c>
@@ -4971,7 +5062,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="22" t="s">
         <v>590</v>
       </c>
@@ -4985,7 +5076,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A191" s="22" t="s">
         <v>591</v>
       </c>
@@ -4999,7 +5090,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="22" t="s">
         <v>592</v>
       </c>
@@ -5013,7 +5104,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A193" s="22" t="s">
         <v>593</v>
       </c>
@@ -5027,7 +5118,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A194" s="22" t="s">
         <v>594</v>
       </c>
@@ -5041,7 +5132,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="22" t="s">
         <v>595</v>
       </c>
@@ -5055,7 +5146,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A196" s="22" t="s">
         <v>596</v>
       </c>
@@ -5069,7 +5160,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="22" t="s">
         <v>597</v>
       </c>
@@ -5083,7 +5174,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="22" t="s">
         <v>598</v>
       </c>
@@ -5097,7 +5188,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="22" t="s">
         <v>599</v>
       </c>
@@ -5111,7 +5202,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A200" s="22" t="s">
         <v>600</v>
       </c>
@@ -5125,7 +5216,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="22" t="s">
         <v>601</v>
       </c>
@@ -5139,7 +5230,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A202" s="22" t="s">
         <v>602</v>
       </c>
@@ -5153,7 +5244,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="22" t="s">
         <v>603</v>
       </c>
@@ -5167,7 +5258,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A204" s="22" t="s">
         <v>604</v>
       </c>
@@ -5181,7 +5272,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="22" t="s">
         <v>605</v>
       </c>
@@ -5195,7 +5286,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="22" t="s">
         <v>606</v>
       </c>
@@ -5209,7 +5300,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A207" s="22" t="s">
         <v>607</v>
       </c>
@@ -5223,7 +5314,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="22" t="s">
         <v>608</v>
       </c>
@@ -5237,7 +5328,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A209" s="22" t="s">
         <v>609</v>
       </c>
@@ -5251,7 +5342,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A210" s="22" t="s">
         <v>610</v>
       </c>
@@ -5265,7 +5356,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="22" t="s">
         <v>611</v>
       </c>
@@ -5277,6 +5368,146 @@
       </c>
       <c r="D211" s="18" t="s">
         <v>573</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C212" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADDED MORE requirments for game display
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a314dec4b6146c21/Desktop/school/spring2025/cse3310/cse3310-sp25-004/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15176dbdb68e5a3b/Desktop/CSE3310/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F63872B2-2440-446F-8C73-0073951D60A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{F63872B2-2440-446F-8C73-0073951D60A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{342078CC-4055-47C1-8794-2B9F8C87EF82}"/>
   <bookViews>
-    <workbookView xWindow="5950" yWindow="2990" windowWidth="19200" windowHeight="11170" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="1485" windowWidth="24945" windowHeight="14010" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,60 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="4">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="4">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="655">
   <si>
     <t>Tested By</t>
   </si>
@@ -1971,6 +2023,27 @@
   </si>
   <si>
     <t>index.html</t>
+  </si>
+  <si>
+    <t>UI_001</t>
+  </si>
+  <si>
+    <t>UI_002</t>
+  </si>
+  <si>
+    <t>UI_004</t>
+  </si>
+  <si>
+    <t>UI_005</t>
+  </si>
+  <si>
+    <t>UI_006</t>
+  </si>
+  <si>
+    <t>UI_007</t>
+  </si>
+  <si>
+    <t>UI_003</t>
   </si>
 </sst>
 </file>
@@ -2244,6 +2317,85 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+</richValueRels>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2422,31 +2574,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C217" sqref="C217"/>
+    <sheetView tabSelected="1" topLeftCell="C210" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R220" sqref="R220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="36.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="123.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" style="2" customWidth="1"/>
-    <col min="7" max="16" width="8.7265625" style="1"/>
-    <col min="17" max="17" width="8.7265625" style="3"/>
-    <col min="18" max="18" width="8.7265625" style="1"/>
-    <col min="19" max="19" width="36.453125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="123.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
+    <col min="7" max="16" width="8.7109375" style="1"/>
+    <col min="17" max="17" width="8.7109375" style="3"/>
+    <col min="18" max="18" width="26.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="36.42578125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2484,7 +2636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2504,7 +2656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2527,7 +2679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2535,27 +2687,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -2569,7 +2721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
@@ -2583,7 +2735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2597,7 +2749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
@@ -2611,7 +2763,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>35</v>
       </c>
@@ -2625,7 +2777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -2639,7 +2791,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>41</v>
       </c>
@@ -2653,7 +2805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
@@ -2667,7 +2819,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>46</v>
       </c>
@@ -2681,7 +2833,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2695,7 +2847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>52</v>
       </c>
@@ -2709,7 +2861,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>54</v>
       </c>
@@ -2723,7 +2875,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>57</v>
       </c>
@@ -2737,7 +2889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>59</v>
       </c>
@@ -2751,7 +2903,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -2766,7 +2918,7 @@
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2781,7 +2933,7 @@
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -2796,7 +2948,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -2811,7 +2963,7 @@
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
@@ -2828,7 +2980,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -2843,7 +2995,7 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -2859,7 +3011,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>85</v>
       </c>
@@ -2876,7 +3028,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
@@ -2893,7 +3045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>91</v>
       </c>
@@ -2907,7 +3059,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -2921,7 +3073,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>98</v>
       </c>
@@ -2935,7 +3087,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>101</v>
       </c>
@@ -2949,7 +3101,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -2963,7 +3115,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>107</v>
       </c>
@@ -2977,7 +3129,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
@@ -2991,7 +3143,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>112</v>
       </c>
@@ -3005,7 +3157,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -3019,7 +3171,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>118</v>
       </c>
@@ -3033,7 +3185,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>121</v>
       </c>
@@ -3047,7 +3199,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -3061,7 +3213,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
@@ -3075,7 +3227,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>131</v>
       </c>
@@ -3089,7 +3241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>134</v>
       </c>
@@ -3103,7 +3255,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -3117,7 +3269,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
@@ -3131,7 +3283,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>143</v>
       </c>
@@ -3145,7 +3297,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>146</v>
       </c>
@@ -3159,7 +3311,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>149</v>
       </c>
@@ -3173,7 +3325,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>151</v>
       </c>
@@ -3187,7 +3339,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>153</v>
       </c>
@@ -3201,7 +3353,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>155</v>
       </c>
@@ -3215,7 +3367,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>157</v>
       </c>
@@ -3229,7 +3381,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>159</v>
       </c>
@@ -3246,7 +3398,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>164</v>
       </c>
@@ -3260,7 +3412,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>168</v>
       </c>
@@ -3274,7 +3426,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>172</v>
       </c>
@@ -3288,7 +3440,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>176</v>
       </c>
@@ -3302,7 +3454,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>180</v>
       </c>
@@ -3316,7 +3468,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>184</v>
       </c>
@@ -3330,7 +3482,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>188</v>
       </c>
@@ -3344,7 +3496,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>192</v>
       </c>
@@ -3358,7 +3510,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>196</v>
       </c>
@@ -3372,7 +3524,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>199</v>
       </c>
@@ -3386,7 +3538,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>202</v>
       </c>
@@ -3400,7 +3552,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>205</v>
       </c>
@@ -3414,7 +3566,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>208</v>
       </c>
@@ -3428,7 +3580,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>211</v>
       </c>
@@ -3442,7 +3594,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>214</v>
       </c>
@@ -3456,7 +3608,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>217</v>
       </c>
@@ -3470,7 +3622,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>221</v>
       </c>
@@ -3484,7 +3636,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>225</v>
       </c>
@@ -3498,7 +3650,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>229</v>
       </c>
@@ -3512,7 +3664,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>232</v>
       </c>
@@ -3526,7 +3678,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>235</v>
       </c>
@@ -3540,7 +3692,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>238</v>
       </c>
@@ -3554,7 +3706,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>242</v>
       </c>
@@ -3568,7 +3720,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>245</v>
       </c>
@@ -3582,7 +3734,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>248</v>
       </c>
@@ -3596,7 +3748,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>251</v>
       </c>
@@ -3610,7 +3762,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>254</v>
       </c>
@@ -3624,7 +3776,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>257</v>
       </c>
@@ -3638,7 +3790,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>260</v>
       </c>
@@ -3652,7 +3804,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>263</v>
       </c>
@@ -3666,7 +3818,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>266</v>
       </c>
@@ -3680,7 +3832,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>269</v>
       </c>
@@ -3694,7 +3846,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>272</v>
       </c>
@@ -3708,7 +3860,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>275</v>
       </c>
@@ -3722,7 +3874,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>279</v>
       </c>
@@ -3736,7 +3888,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>281</v>
       </c>
@@ -3750,7 +3902,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>285</v>
       </c>
@@ -3764,7 +3916,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>287</v>
       </c>
@@ -3778,7 +3930,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>290</v>
       </c>
@@ -3792,7 +3944,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>293</v>
       </c>
@@ -3806,7 +3958,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>296</v>
       </c>
@@ -3820,7 +3972,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>299</v>
       </c>
@@ -3834,7 +3986,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>302</v>
       </c>
@@ -3848,7 +4000,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>305</v>
       </c>
@@ -3862,7 +4014,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>307</v>
       </c>
@@ -3876,7 +4028,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>309</v>
       </c>
@@ -3890,7 +4042,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>312</v>
       </c>
@@ -3904,7 +4056,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>315</v>
       </c>
@@ -3918,7 +4070,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>318</v>
       </c>
@@ -3932,7 +4084,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>320</v>
       </c>
@@ -3946,7 +4098,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>324</v>
       </c>
@@ -3960,7 +4112,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>326</v>
       </c>
@@ -3974,7 +4126,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>329</v>
       </c>
@@ -3988,7 +4140,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>331</v>
       </c>
@@ -4002,7 +4154,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>333</v>
       </c>
@@ -4016,7 +4168,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>335</v>
       </c>
@@ -4030,7 +4182,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>338</v>
       </c>
@@ -4044,7 +4196,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>340</v>
       </c>
@@ -4058,7 +4210,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>342</v>
       </c>
@@ -4072,7 +4224,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>345</v>
       </c>
@@ -4086,7 +4238,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>347</v>
       </c>
@@ -4100,7 +4252,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>349</v>
       </c>
@@ -4114,7 +4266,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>351</v>
       </c>
@@ -4128,7 +4280,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>353</v>
       </c>
@@ -4142,7 +4294,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>356</v>
       </c>
@@ -4156,7 +4308,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>358</v>
       </c>
@@ -4170,7 +4322,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>360</v>
       </c>
@@ -4184,7 +4336,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>362</v>
       </c>
@@ -4198,7 +4350,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>364</v>
       </c>
@@ -4212,7 +4364,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
         <v>366</v>
       </c>
@@ -4226,7 +4378,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
         <v>370</v>
       </c>
@@ -4240,7 +4392,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>373</v>
       </c>
@@ -4254,7 +4406,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>376</v>
       </c>
@@ -4268,7 +4420,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>378</v>
       </c>
@@ -4282,7 +4434,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>381</v>
       </c>
@@ -4296,7 +4448,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>384</v>
       </c>
@@ -4310,7 +4462,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>387</v>
       </c>
@@ -4324,7 +4476,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>390</v>
       </c>
@@ -4338,7 +4490,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>393</v>
       </c>
@@ -4352,7 +4504,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>396</v>
       </c>
@@ -4366,7 +4518,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>399</v>
       </c>
@@ -4380,7 +4532,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>402</v>
       </c>
@@ -4394,7 +4546,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>406</v>
       </c>
@@ -4408,7 +4560,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="16" t="s">
         <v>409</v>
       </c>
@@ -4422,7 +4574,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="16" t="s">
         <v>411</v>
       </c>
@@ -4436,7 +4588,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="16" t="s">
         <v>412</v>
       </c>
@@ -4450,7 +4602,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="23.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="16" t="s">
         <v>413</v>
       </c>
@@ -4464,7 +4616,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="16" t="s">
         <v>414</v>
       </c>
@@ -4478,7 +4630,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="16" t="s">
         <v>415</v>
       </c>
@@ -4492,7 +4644,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="16" t="s">
         <v>416</v>
       </c>
@@ -4506,7 +4658,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="16" t="s">
         <v>417</v>
       </c>
@@ -4520,7 +4672,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="16" t="s">
         <v>418</v>
       </c>
@@ -4534,7 +4686,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
         <v>419</v>
       </c>
@@ -4548,7 +4700,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="16" t="s">
         <v>442</v>
       </c>
@@ -4562,7 +4714,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
         <v>443</v>
       </c>
@@ -4576,7 +4728,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>483</v>
       </c>
@@ -4590,7 +4742,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>484</v>
       </c>
@@ -4604,7 +4756,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>485</v>
       </c>
@@ -4618,7 +4770,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>486</v>
       </c>
@@ -4632,7 +4784,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>487</v>
       </c>
@@ -4646,7 +4798,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>488</v>
       </c>
@@ -4660,7 +4812,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>489</v>
       </c>
@@ -4674,7 +4826,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>490</v>
       </c>
@@ -4688,7 +4840,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>491</v>
       </c>
@@ -4702,7 +4854,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>492</v>
       </c>
@@ -4716,7 +4868,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>493</v>
       </c>
@@ -4730,7 +4882,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>494</v>
       </c>
@@ -4744,7 +4896,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>495</v>
       </c>
@@ -4758,7 +4910,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>496</v>
       </c>
@@ -4772,7 +4924,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>497</v>
       </c>
@@ -4786,7 +4938,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>498</v>
       </c>
@@ -4800,7 +4952,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>499</v>
       </c>
@@ -4814,7 +4966,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>500</v>
       </c>
@@ -4828,7 +4980,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>501</v>
       </c>
@@ -4842,7 +4994,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>502</v>
       </c>
@@ -4856,7 +5008,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>503</v>
       </c>
@@ -4870,7 +5022,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A175" s="22" t="s">
         <v>575</v>
       </c>
@@ -4884,7 +5036,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A176" s="22" t="s">
         <v>576</v>
       </c>
@@ -4898,7 +5050,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A177" s="22" t="s">
         <v>577</v>
       </c>
@@ -4912,7 +5064,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="74" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A178" s="22" t="s">
         <v>578</v>
       </c>
@@ -4926,7 +5078,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="74" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A179" s="22" t="s">
         <v>579</v>
       </c>
@@ -4940,7 +5092,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A180" s="22" t="s">
         <v>580</v>
       </c>
@@ -4954,7 +5106,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="22" t="s">
         <v>581</v>
       </c>
@@ -4968,7 +5120,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="22" t="s">
         <v>582</v>
       </c>
@@ -4982,7 +5134,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="22" t="s">
         <v>583</v>
       </c>
@@ -4996,7 +5148,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="22" t="s">
         <v>584</v>
       </c>
@@ -5010,7 +5162,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="22" t="s">
         <v>585</v>
       </c>
@@ -5024,7 +5176,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A186" s="22" t="s">
         <v>586</v>
       </c>
@@ -5038,7 +5190,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A187" s="22" t="s">
         <v>587</v>
       </c>
@@ -5052,7 +5204,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:4" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A188" s="22" t="s">
         <v>588</v>
       </c>
@@ -5066,7 +5218,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A189" s="22" t="s">
         <v>589</v>
       </c>
@@ -5080,7 +5232,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="22" t="s">
         <v>590</v>
       </c>
@@ -5094,7 +5246,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A191" s="22" t="s">
         <v>591</v>
       </c>
@@ -5108,7 +5260,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="22" t="s">
         <v>592</v>
       </c>
@@ -5122,7 +5274,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A193" s="22" t="s">
         <v>593</v>
       </c>
@@ -5136,7 +5288,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A194" s="22" t="s">
         <v>594</v>
       </c>
@@ -5150,7 +5302,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="22" t="s">
         <v>595</v>
       </c>
@@ -5164,7 +5316,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A196" s="22" t="s">
         <v>596</v>
       </c>
@@ -5178,7 +5330,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="22" t="s">
         <v>597</v>
       </c>
@@ -5192,7 +5344,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="22" t="s">
         <v>598</v>
       </c>
@@ -5206,7 +5358,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="22" t="s">
         <v>599</v>
       </c>
@@ -5220,7 +5372,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A200" s="22" t="s">
         <v>600</v>
       </c>
@@ -5234,7 +5386,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="22" t="s">
         <v>601</v>
       </c>
@@ -5248,7 +5400,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A202" s="22" t="s">
         <v>602</v>
       </c>
@@ -5262,7 +5414,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="22" t="s">
         <v>603</v>
       </c>
@@ -5276,7 +5428,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A204" s="22" t="s">
         <v>604</v>
       </c>
@@ -5290,7 +5442,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="22" t="s">
         <v>605</v>
       </c>
@@ -5304,7 +5456,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="22" t="s">
         <v>606</v>
       </c>
@@ -5318,7 +5470,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A207" s="22" t="s">
         <v>607</v>
       </c>
@@ -5332,7 +5484,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="22" t="s">
         <v>608</v>
       </c>
@@ -5346,7 +5498,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:18" ht="75" x14ac:dyDescent="0.3">
       <c r="A209" s="22" t="s">
         <v>609</v>
       </c>
@@ -5360,7 +5512,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="37" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:18" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A210" s="22" t="s">
         <v>610</v>
       </c>
@@ -5374,7 +5526,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="22" t="s">
         <v>611</v>
       </c>
@@ -5388,7 +5540,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>612</v>
       </c>
@@ -5401,8 +5553,11 @@
       <c r="D212" s="1" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E212" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>616</v>
       </c>
@@ -5416,7 +5571,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>619</v>
       </c>
@@ -5429,8 +5584,11 @@
       <c r="D214" s="1" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E214" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>622</v>
       </c>
@@ -5443,8 +5601,11 @@
       <c r="D215" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E215" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>625</v>
       </c>
@@ -5457,8 +5618,11 @@
       <c r="D216" s="1" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E216" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>628</v>
       </c>
@@ -5471,8 +5635,11 @@
       <c r="D217" s="1" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E217" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>631</v>
       </c>
@@ -5485,8 +5652,11 @@
       <c r="D218" s="1" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E218" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>634</v>
       </c>
@@ -5499,8 +5669,11 @@
       <c r="D219" s="1" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E219" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>636</v>
       </c>
@@ -5513,8 +5686,11 @@
       <c r="D220" s="1" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="R220" s="1" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>639</v>
       </c>
@@ -5527,8 +5703,11 @@
       <c r="D221" s="1" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="R221" s="1" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>642</v>
       </c>
@@ -5541,8 +5720,11 @@
       <c r="D222" s="1" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="R222" s="1" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>645</v>
       </c>
@@ -5554,6 +5736,9 @@
       </c>
       <c r="D223" s="1" t="s">
         <v>647</v>
+      </c>
+      <c r="R223" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected GamePlay spelling mistakes
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phanm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D743EC20-6199-420C-9F90-65CDC3FF2254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8898CB7-5CEE-4B95-BEF9-6214ACA21407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,12 +186,6 @@
     <t>move()</t>
   </si>
   <si>
-    <t>The system shall enusre the checkers are only allowed to move on the dark sqaures of the board</t>
-  </si>
-  <si>
-    <t>The system shall allow checkers controled by one player to 'jump' checkers controled by the other player by "moving a piece that is diagonally adjacent an opponent's piece, to an empty square immediately beyond it in the same direction"</t>
-  </si>
-  <si>
     <t>getPossibleForwardJump(), getPossibleBackwardJump()</t>
   </si>
   <si>
@@ -207,18 +201,9 @@
     <t>kingMe()</t>
   </si>
   <si>
-    <t>The system shall allow all king checkers to move in both foward and backwards directions (twoards AND away from the player controling them)</t>
-  </si>
-  <si>
-    <t>The system shall send new game states to the Game Manager once a valid move is proccesed</t>
-  </si>
-  <si>
     <t>getBoard()</t>
   </si>
   <si>
-    <t xml:space="preserve">The system shall allow the player required to make a jump with a checker to chose which series of jumps to be performed when multiple are availible   </t>
-  </si>
-  <si>
     <t>The system shall be assigned an ID by Game Manager on instance</t>
   </si>
   <si>
@@ -2053,6 +2038,21 @@
   </si>
   <si>
     <t>GP_19</t>
+  </si>
+  <si>
+    <t>The system shall send new game states to the Game Manager once a valid move is processed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall require the player to make a jump with a checker to choose which series of jumps to be performed when multiple are available  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The system shall ensure the checkers are only allowed to move on the dark squares of the board</t>
+  </si>
+  <si>
+    <t>The system shall allow checkers controlled by one player to 'jump' checkers controlled by the other player by "moving a piece that is diagonally adjacent an opponent's piece, to an empty square immediately beyond it in the same direction"</t>
+  </si>
+  <si>
+    <t>The system shall allow all king checkers to move in both forward and backwards directions (towards AND away from the player controlling them)</t>
   </si>
 </sst>
 </file>
@@ -2594,7 +2594,7 @@
   <dimension ref="A1:S223"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>24</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>24</v>
@@ -2756,7 +2756,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>24</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>24</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>24</v>
@@ -2798,7 +2798,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>24</v>
@@ -2812,13 +2812,13 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>35</v>
+        <v>655</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>32</v>
@@ -2826,55 +2826,55 @@
     </row>
     <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>36</v>
+        <v>656</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>42</v>
+        <v>657</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>34</v>
@@ -2882,2842 +2882,2842 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>43</v>
+        <v>653</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>45</v>
+        <v>654</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="8" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="8" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B128" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="D128" s="8" t="s">
         <v>353</v>
-      </c>
-      <c r="C128" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="8" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="8" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="8" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="8" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="8" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="8" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="8" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="8" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="8" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B140" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D140" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="D140" s="8" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="23" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A142" s="15" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B142" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D142" s="15" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A143" s="15" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B143" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D143" s="15" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A144" s="15" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D144" s="15" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="15" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C145" s="15" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D145" s="15" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A146" s="15" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B146" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C146" s="15" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D146" s="15" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A147" s="15" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C147" s="15" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D147" s="15" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A148" s="15" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B148" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D148" s="15" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A149" s="15" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D149" s="15" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A150" s="15" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D150" s="15" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A151" s="15" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D151" s="15" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A152" s="15" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D152" s="15" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A153" s="15" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D153" s="15" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D154" s="16" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D155" s="16" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D156" s="16" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D157" s="16" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C158" s="16" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D158" s="16" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D159" s="16" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D160" s="16" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D161" s="16" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D162" s="16" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C163" s="16" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D163" s="16" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D164" s="16" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C165" s="16" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D165" s="16" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C166" s="16" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D166" s="16" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C167" s="16" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D167" s="16" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C168" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D168" s="16" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C169" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D169" s="16" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C170" s="16" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D170" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C171" s="16" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D171" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C172" s="16" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D172" s="16" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C173" s="16" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D173" s="16" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C174" s="16" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D174" s="16" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A175" s="21" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="B175" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C175" s="20" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D175" s="17" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A176" s="21" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="B176" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C176" s="17" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D176" s="17" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A177" s="21" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="B177" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C177" s="17" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D177" s="17" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="72" x14ac:dyDescent="0.35">
       <c r="A178" s="21" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B178" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C178" s="18" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D178" s="18" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="72" x14ac:dyDescent="0.35">
       <c r="A179" s="21" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="B179" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C179" s="18" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D179" s="18" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="54" x14ac:dyDescent="0.35">
       <c r="A180" s="21" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="B180" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C180" s="17" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D180" s="17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A181" s="21" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="B181" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C181" s="17" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D181" s="17" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A182" s="21" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="B182" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C182" s="17" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D182" s="17" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A183" s="21" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="B183" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C183" s="17" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D183" s="17" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A184" s="21" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B184" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C184" s="17" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D184" s="17" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A185" s="21" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="B185" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C185" s="17" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D185" s="17" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A186" s="21" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="B186" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C186" s="17" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D186" s="17" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A187" s="21" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="B187" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C187" s="17" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D187" s="17" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="54" x14ac:dyDescent="0.35">
       <c r="A188" s="21" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="B188" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C188" s="17" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D188" s="17" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A189" s="21" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="B189" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C189" s="17" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D189" s="17" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A190" s="21" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="B190" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C190" s="17" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D190" s="17" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A191" s="21" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="B191" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C191" s="17" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="D191" s="17" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A192" s="21" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="B192" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C192" s="17" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="D192" s="17" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A193" s="21" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="B193" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C193" s="17" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D193" s="17" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A194" s="21" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="B194" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C194" s="17" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="D194" s="17" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A195" s="21" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="B195" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C195" s="17" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="D195" s="17" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A196" s="21" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="B196" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C196" s="17" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D196" s="17" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A197" s="21" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="B197" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C197" s="17" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="D197" s="17" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A198" s="21" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="B198" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C198" s="17" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="D198" s="17" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A199" s="21" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="B199" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C199" s="17" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D199" s="17" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A200" s="21" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="B200" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C200" s="17" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D200" s="17" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A201" s="21" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="B201" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C201" s="17" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D201" s="17" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A202" s="21" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="B202" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C202" s="17" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D202" s="17" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A203" s="21" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="B203" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C203" s="17" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D203" s="17" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A204" s="21" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="B204" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C204" s="17" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="D204" s="17" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A205" s="21" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="B205" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C205" s="19" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D205" s="17" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A206" s="21" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="B206" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C206" s="17" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D206" s="17" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A207" s="21" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="B207" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C207" s="19" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D207" s="17" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A208" s="21" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="B208" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C208" s="19" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D208" s="17" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="209" spans="1:5" ht="54" x14ac:dyDescent="0.35">
       <c r="A209" s="21" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B209" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C209" s="17" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D209" s="17" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="210" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A210" s="21" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B210" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C210" s="17" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D210" s="17" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="211" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A211" s="21" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="B211" s="21" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C211" s="17" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D211" s="17" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C212" s="22" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="D213" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
     </row>
     <row r="220" spans="1:5" ht="211.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="E220" s="1" t="e" vm="1">
         <v>#VALUE!</v>
@@ -5725,16 +5725,16 @@
     </row>
     <row r="221" spans="1:5" ht="205.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="E221" s="1" t="e" vm="2">
         <v>#VALUE!</v>
@@ -5742,16 +5742,16 @@
     </row>
     <row r="222" spans="1:5" ht="169.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="E222" s="1" t="e" vm="3">
         <v>#VALUE!</v>
@@ -5759,16 +5759,16 @@
     </row>
     <row r="223" spans="1:5" ht="147" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="E223" s="1" t="e" vm="4">
         <v>#VALUE!</v>

</xml_diff>

<commit_message>
some untestable features in Page Manager
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phanm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyncthingServiceAcct\school work\2025\Spring 2025\CSE 3310 FUNDAMENTALS OF SOFTWARE ENGR\cse3310-sp25-004\FinalRequirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8898CB7-5CEE-4B95-BEF9-6214ACA21407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716188A6-741C-4B13-9825-02F3953FB873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="659">
   <si>
     <t>Tested By</t>
   </si>
@@ -2053,6 +2053,9 @@
   </si>
   <si>
     <t>The system shall allow all king checkers to move in both forward and backwards directions (towards AND away from the player controlling them)</t>
+  </si>
+  <si>
+    <t>untestable</t>
   </si>
 </sst>
 </file>
@@ -2593,8 +2596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2605,7 +2608,9 @@
     <col min="4" max="4" width="65.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" style="2" customWidth="1"/>
-    <col min="7" max="16" width="8.6640625" style="1"/>
+    <col min="7" max="9" width="8.6640625" style="1"/>
+    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="8.6640625" style="1"/>
     <col min="17" max="17" width="8.6640625" style="3"/>
     <col min="18" max="18" width="8.6640625" style="1"/>
     <col min="19" max="19" width="36.44140625" style="1" customWidth="1"/>
@@ -5083,7 +5088,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" ht="36" x14ac:dyDescent="0.35">
       <c r="A177" s="21" t="s">
         <v>554</v>
       </c>
@@ -5097,7 +5102,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" ht="72" x14ac:dyDescent="0.35">
       <c r="A178" s="21" t="s">
         <v>555</v>
       </c>
@@ -5111,7 +5116,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="72" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" ht="72" x14ac:dyDescent="0.35">
       <c r="A179" s="21" t="s">
         <v>556</v>
       </c>
@@ -5125,7 +5130,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" ht="54" x14ac:dyDescent="0.35">
       <c r="A180" s="21" t="s">
         <v>557</v>
       </c>
@@ -5139,7 +5144,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A181" s="21" t="s">
         <v>558</v>
       </c>
@@ -5152,8 +5157,11 @@
       <c r="D181" s="17" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="J181" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A182" s="21" t="s">
         <v>559</v>
       </c>
@@ -5166,8 +5174,11 @@
       <c r="D182" s="17" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="J182" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A183" s="21" t="s">
         <v>560</v>
       </c>
@@ -5180,8 +5191,11 @@
       <c r="D183" s="17" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="J183" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A184" s="21" t="s">
         <v>561</v>
       </c>
@@ -5194,8 +5208,11 @@
       <c r="D184" s="17" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="J184" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A185" s="21" t="s">
         <v>562</v>
       </c>
@@ -5208,8 +5225,11 @@
       <c r="D185" s="17" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="J185" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="36" x14ac:dyDescent="0.35">
       <c r="A186" s="21" t="s">
         <v>563</v>
       </c>
@@ -5222,8 +5242,11 @@
       <c r="D186" s="17" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="J186" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" ht="36" x14ac:dyDescent="0.35">
       <c r="A187" s="21" t="s">
         <v>564</v>
       </c>
@@ -5236,8 +5259,11 @@
       <c r="D187" s="17" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+      <c r="J187" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" ht="54" x14ac:dyDescent="0.35">
       <c r="A188" s="21" t="s">
         <v>565</v>
       </c>
@@ -5250,8 +5276,11 @@
       <c r="D188" s="17" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="J188" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" ht="36" x14ac:dyDescent="0.35">
       <c r="A189" s="21" t="s">
         <v>566</v>
       </c>
@@ -5264,8 +5293,11 @@
       <c r="D189" s="17" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="J189" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A190" s="21" t="s">
         <v>567</v>
       </c>
@@ -5278,8 +5310,11 @@
       <c r="D190" s="17" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="J190" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A191" s="21" t="s">
         <v>568</v>
       </c>
@@ -5293,7 +5328,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A192" s="21" t="s">
         <v>569</v>
       </c>

</xml_diff>

<commit_message>
untestable requirements in Page Manager
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyncthingServiceAcct\school work\2025\Spring 2025\CSE 3310 FUNDAMENTALS OF SOFTWARE ENGR\cse3310-sp25-004\FinalRequirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716188A6-741C-4B13-9825-02F3953FB873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0A2672-079C-478E-B189-AD9F9341EEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2596,8 +2596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="C170" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L192" sqref="L192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2801,7 +2801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>644</v>
       </c>

</xml_diff>

<commit_message>
Indicated requirements tested by Test 1 -- Group 20
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aisha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A854E7-E5A9-4CA6-ABAC-3B36ADD78CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E89A6B-F3C3-4FC3-8FE9-D09A797ECECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="670">
   <si>
     <t>Tested By</t>
   </si>
@@ -2024,6 +2024,30 @@
   </si>
   <si>
     <t>Group 21</t>
+  </si>
+  <si>
+    <t>Test 1, Step 6</t>
+  </si>
+  <si>
+    <t>Test 1, Step 7</t>
+  </si>
+  <si>
+    <t>Test 1, Step 3</t>
+  </si>
+  <si>
+    <t>Test 1, Step 5</t>
+  </si>
+  <si>
+    <t>Test 1, Step 4</t>
+  </si>
+  <si>
+    <t>Test 1, Step 1</t>
+  </si>
+  <si>
+    <t>Test 1, Step 2</t>
+  </si>
+  <si>
+    <t>Test 1, Step 8</t>
   </si>
 </sst>
 </file>
@@ -2472,15 +2496,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T216" sqref="T216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.6328125" style="1"/>
     <col min="2" max="2" width="36.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="123.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="65.36328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="47.81640625" style="1" customWidth="1"/>
@@ -2490,7 +2514,7 @@
     <col min="12" max="13" width="8.6328125" style="1"/>
     <col min="14" max="14" width="10.90625" style="1" customWidth="1"/>
     <col min="15" max="16" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.7265625" style="3" customWidth="1"/>
     <col min="19" max="19" width="8.6328125" style="1"/>
     <col min="20" max="20" width="36.453125" style="1" customWidth="1"/>
@@ -2701,14 +2725,15 @@
       <c r="B14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="8" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
@@ -2749,14 +2774,15 @@
       <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q17" s="8"/>
+      <c r="Q17" s="8" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
@@ -2956,6 +2982,9 @@
       <c r="G28" s="11" t="s">
         <v>76</v>
       </c>
+      <c r="Q28" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -2971,6 +3000,9 @@
         <v>79</v>
       </c>
       <c r="G29" s="11"/>
+      <c r="Q29" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -2987,6 +3019,9 @@
       </c>
       <c r="G30" s="11"/>
       <c r="H30" s="13"/>
+      <c r="Q30" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
@@ -3004,6 +3039,9 @@
       <c r="G31" s="11" t="s">
         <v>76</v>
       </c>
+      <c r="Q31" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
@@ -3283,6 +3321,9 @@
       <c r="E46" s="5" t="s">
         <v>132</v>
       </c>
+      <c r="Q46" s="1" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
@@ -3546,6 +3587,9 @@
       <c r="E62" s="5" t="s">
         <v>182</v>
       </c>
+      <c r="Q62" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="63" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
@@ -3600,6 +3644,9 @@
       <c r="E65" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="Q65" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
@@ -3648,6 +3695,9 @@
       <c r="E68" s="5" t="s">
         <v>161</v>
       </c>
+      <c r="Q68" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
@@ -3662,6 +3712,9 @@
       <c r="E69" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="Q69" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
@@ -3704,6 +3757,9 @@
       <c r="E72" s="5" t="s">
         <v>174</v>
       </c>
+      <c r="Q72" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
@@ -3800,6 +3856,9 @@
       <c r="E78" s="5" t="s">
         <v>223</v>
       </c>
+      <c r="Q78" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
@@ -3848,6 +3907,9 @@
       <c r="E81" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="Q81" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
@@ -3862,6 +3924,9 @@
       <c r="E82" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="Q82" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
@@ -3876,6 +3941,9 @@
       <c r="E83" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="Q83" s="1" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
@@ -3994,6 +4062,9 @@
       <c r="E91" s="15" t="s">
         <v>277</v>
       </c>
+      <c r="Q91" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
@@ -4008,6 +4079,9 @@
       <c r="E92" s="15" t="s">
         <v>277</v>
       </c>
+      <c r="Q92" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
@@ -4022,6 +4096,9 @@
       <c r="E93" s="15" t="s">
         <v>283</v>
       </c>
+      <c r="Q93" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
@@ -4036,6 +4113,9 @@
       <c r="E94" s="15" t="s">
         <v>283</v>
       </c>
+      <c r="Q94" s="1" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
@@ -4050,6 +4130,9 @@
       <c r="E95" s="15" t="s">
         <v>288</v>
       </c>
+      <c r="Q95" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
@@ -4064,6 +4147,9 @@
       <c r="E96" s="15" t="s">
         <v>291</v>
       </c>
+      <c r="Q96" s="1" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
@@ -4140,6 +4226,9 @@
       <c r="E101" s="15" t="s">
         <v>291</v>
       </c>
+      <c r="Q101" s="1" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
@@ -4154,6 +4243,9 @@
       <c r="E102" s="15" t="s">
         <v>291</v>
       </c>
+      <c r="Q102" s="1" t="s">
+        <v>668</v>
+      </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
@@ -4168,6 +4260,9 @@
       <c r="E103" s="15" t="s">
         <v>310</v>
       </c>
+      <c r="Q103" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
@@ -4182,6 +4277,9 @@
       <c r="E104" s="15" t="s">
         <v>313</v>
       </c>
+      <c r="Q104" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
@@ -4196,6 +4294,9 @@
       <c r="E105" s="15" t="s">
         <v>316</v>
       </c>
+      <c r="Q105" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
@@ -4210,6 +4311,9 @@
       <c r="E106" s="15" t="s">
         <v>316</v>
       </c>
+      <c r="Q106" s="1" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
@@ -4782,14 +4886,15 @@
       <c r="B142" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="C142" s="17"/>
       <c r="D142" s="17" t="s">
         <v>413</v>
       </c>
       <c r="E142" s="17" t="s">
         <v>414</v>
       </c>
-      <c r="Q142" s="17"/>
+      <c r="Q142" s="1" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A143" s="17" t="s">
@@ -4798,7 +4903,6 @@
       <c r="B143" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="C143" s="17"/>
       <c r="D143" s="17" t="s">
         <v>416</v>
       </c>
@@ -4814,14 +4918,15 @@
       <c r="B144" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="C144" s="17"/>
       <c r="D144" s="17" t="s">
         <v>419</v>
       </c>
       <c r="E144" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="Q144" s="17"/>
+      <c r="Q144" s="17" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="17" t="s">
@@ -4830,14 +4935,15 @@
       <c r="B145" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="C145" s="17"/>
       <c r="D145" s="17" t="s">
         <v>422</v>
       </c>
       <c r="E145" s="17" t="s">
         <v>423</v>
       </c>
-      <c r="Q145" s="17"/>
+      <c r="Q145" s="17" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A146" s="17" t="s">
@@ -5704,14 +5810,15 @@
       <c r="B195" s="18" t="s">
         <v>507</v>
       </c>
-      <c r="C195" s="18"/>
       <c r="D195" s="20" t="s">
         <v>568</v>
       </c>
       <c r="E195" s="20" t="s">
         <v>569</v>
       </c>
-      <c r="Q195" s="18"/>
+      <c r="Q195" s="18" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="196" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A196" s="18" t="s">
@@ -5848,14 +5955,15 @@
       <c r="B203" s="18" t="s">
         <v>507</v>
       </c>
-      <c r="C203" s="18"/>
       <c r="D203" s="20" t="s">
         <v>589</v>
       </c>
       <c r="E203" s="20" t="s">
         <v>590</v>
       </c>
-      <c r="Q203" s="18"/>
+      <c r="Q203" s="18" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="204" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A204" s="18" t="s">
@@ -6058,6 +6166,9 @@
       <c r="F214" s="1" t="s">
         <v>626</v>
       </c>
+      <c r="Q214" s="1" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
@@ -6092,6 +6203,9 @@
       <c r="F216" s="1" t="s">
         <v>634</v>
       </c>
+      <c r="Q216" s="1" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
@@ -6109,6 +6223,9 @@
       <c r="F217" s="1" t="s">
         <v>638</v>
       </c>
+      <c r="Q217" s="1" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
@@ -6125,6 +6242,9 @@
       </c>
       <c r="F218" s="1" t="s">
         <v>642</v>
+      </c>
+      <c r="Q218" s="1" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="219" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update group 19 finalrequiremets
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -2205,55 +2205,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2261,35 +2261,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2549,7 +2549,7 @@
       <selection pane="topLeft" activeCell="W220" activeCellId="0" sqref="W220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.63671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.45"/>

</xml_diff>

<commit_message>
testing to see how game breaking the StackOverflowError really is
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyncthingServiceAcct\school work\2025\Spring 2025\CSE 3310 FUNDAMENTALS OF SOFTWARE ENGR\cse3310-sp25-004\FinalRequirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E637128-77D8-4633-A9A4-BE894A1BEDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A13E766-2D3E-43FF-A925-997D9A2AA8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update excel file - tested login/signup and bot 1
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyncthingServiceAcct\school work\2025\Spring 2025\CSE 3310 FUNDAMENTALS OF SOFTWARE ENGR\cse3310-sp25-004\FinalRequirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardankarki/Desktop/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A13E766-2D3E-43FF-A925-997D9A2AA8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34788134-EBA4-CE4D-9431-B18B33C71783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11235" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="680">
   <si>
     <t>Tested By</t>
   </si>
@@ -2055,6 +2055,30 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>Step 1, pass</t>
+  </si>
+  <si>
+    <t>Step 4, pass</t>
+  </si>
+  <si>
+    <t>Step 2, pass</t>
+  </si>
+  <si>
+    <t>Step 5, fail</t>
+  </si>
+  <si>
+    <t>Step 8, pass</t>
+  </si>
+  <si>
+    <t>Step 3, pass</t>
+  </si>
+  <si>
+    <t>Step 5, pass</t>
+  </si>
+  <si>
+    <t>Step 4, fail</t>
   </si>
 </sst>
 </file>
@@ -2497,37 +2521,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="63" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="K175" sqref="K175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="36.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="123.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="123.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="65.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="47.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="2" customWidth="1"/>
     <col min="8" max="10" width="8.6640625" style="1"/>
-    <col min="11" max="11" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="8.6640625" style="1"/>
-    <col min="14" max="14" width="10.88671875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.44140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.21875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3" customWidth="1"/>
     <col min="19" max="19" width="8.6640625" style="1"/>
-    <col min="20" max="20" width="36.44140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="36.5" style="1" customWidth="1"/>
     <col min="21" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2565,7 +2589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2588,7 +2612,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2611,7 +2635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2619,27 +2643,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2665,7 +2689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -2691,7 +2715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -2717,7 +2741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2743,7 +2767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2763,7 +2787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
@@ -2782,7 +2806,7 @@
       </c>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2801,7 +2825,7 @@
       </c>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -2821,7 +2845,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
@@ -2840,7 +2864,7 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -2859,7 +2883,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2878,7 +2902,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>59</v>
       </c>
@@ -2904,7 +2928,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
@@ -2923,7 +2947,7 @@
       </c>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>64</v>
       </c>
@@ -2949,7 +2973,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -2976,7 +3000,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -3003,7 +3027,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -3021,7 +3045,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -3048,7 +3072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -3071,7 +3095,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -3092,7 +3116,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -3114,7 +3138,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
@@ -3137,7 +3161,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
@@ -3157,7 +3181,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
@@ -3171,7 +3195,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -3185,7 +3209,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
@@ -3211,7 +3235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>107</v>
       </c>
@@ -3237,7 +3261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -3263,7 +3287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3289,7 +3313,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -3312,7 +3336,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>118</v>
       </c>
@@ -3335,7 +3359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -3358,7 +3382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -3372,7 +3396,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -3395,7 +3419,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -3418,7 +3442,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -3432,7 +3456,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -3449,7 +3473,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
@@ -3463,7 +3487,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -3477,7 +3501,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -3491,7 +3515,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -3514,7 +3538,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
@@ -3528,7 +3552,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>156</v>
       </c>
@@ -3542,7 +3566,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>158</v>
       </c>
@@ -3556,7 +3580,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -3570,7 +3594,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
@@ -3584,7 +3608,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>164</v>
       </c>
@@ -3607,7 +3631,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>166</v>
       </c>
@@ -3636,7 +3660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
@@ -3662,7 +3686,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>175</v>
       </c>
@@ -3688,7 +3712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>179</v>
       </c>
@@ -3705,7 +3729,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>183</v>
       </c>
@@ -3731,7 +3755,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>187</v>
       </c>
@@ -3751,7 +3775,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>191</v>
       </c>
@@ -3777,7 +3801,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
@@ -3803,7 +3827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>199</v>
       </c>
@@ -3823,7 +3847,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>203</v>
       </c>
@@ -3840,7 +3864,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>206</v>
       </c>
@@ -3866,7 +3890,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>209</v>
       </c>
@@ -3886,7 +3910,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>212</v>
       </c>
@@ -3906,7 +3930,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>215</v>
       </c>
@@ -3923,7 +3947,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>218</v>
       </c>
@@ -3940,7 +3964,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>221</v>
       </c>
@@ -3960,7 +3984,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>224</v>
       </c>
@@ -3986,7 +4010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>228</v>
       </c>
@@ -4003,7 +4027,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>232</v>
       </c>
@@ -4029,7 +4053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>236</v>
       </c>
@@ -4046,7 +4070,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>239</v>
       </c>
@@ -4063,7 +4087,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>242</v>
       </c>
@@ -4083,7 +4107,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>245</v>
       </c>
@@ -4100,7 +4124,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>249</v>
       </c>
@@ -4126,7 +4150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>252</v>
       </c>
@@ -4146,7 +4170,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>255</v>
       </c>
@@ -4166,7 +4190,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>258</v>
       </c>
@@ -4186,7 +4210,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>261</v>
       </c>
@@ -4203,7 +4227,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>264</v>
       </c>
@@ -4220,7 +4244,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>267</v>
       </c>
@@ -4237,7 +4261,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>270</v>
       </c>
@@ -4254,7 +4278,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>273</v>
       </c>
@@ -4280,7 +4304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>276</v>
       </c>
@@ -4297,7 +4321,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>279</v>
       </c>
@@ -4314,7 +4338,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>282</v>
       </c>
@@ -4327,11 +4351,14 @@
       <c r="E91" s="15" t="s">
         <v>285</v>
       </c>
+      <c r="K91" s="1" t="s">
+        <v>672</v>
+      </c>
       <c r="Q91" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>287</v>
       </c>
@@ -4344,11 +4371,14 @@
       <c r="E92" s="15" t="s">
         <v>285</v>
       </c>
+      <c r="K92" s="1" t="s">
+        <v>672</v>
+      </c>
       <c r="Q92" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>289</v>
       </c>
@@ -4361,11 +4391,14 @@
       <c r="E93" s="15" t="s">
         <v>292</v>
       </c>
+      <c r="K93" s="1" t="s">
+        <v>673</v>
+      </c>
       <c r="Q93" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>293</v>
       </c>
@@ -4378,11 +4411,14 @@
       <c r="E94" s="15" t="s">
         <v>292</v>
       </c>
+      <c r="K94" s="1" t="s">
+        <v>673</v>
+      </c>
       <c r="Q94" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
@@ -4395,11 +4431,14 @@
       <c r="E95" s="15" t="s">
         <v>298</v>
       </c>
+      <c r="K95" s="1" t="s">
+        <v>674</v>
+      </c>
       <c r="Q95" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -4412,11 +4451,14 @@
       <c r="E96" s="15" t="s">
         <v>301</v>
       </c>
+      <c r="K96" s="1" t="s">
+        <v>672</v>
+      </c>
       <c r="Q96" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>302</v>
       </c>
@@ -4429,8 +4471,11 @@
       <c r="E97" s="15" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K97" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>305</v>
       </c>
@@ -4443,8 +4488,11 @@
       <c r="E98" s="15" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K98" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>308</v>
       </c>
@@ -4457,8 +4505,11 @@
       <c r="E99" s="15" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K99" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -4474,6 +4525,9 @@
       <c r="E100" s="15" t="s">
         <v>313</v>
       </c>
+      <c r="K100" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="P100" s="8" t="s">
         <v>30</v>
       </c>
@@ -4481,7 +4535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>314</v>
       </c>
@@ -4494,11 +4548,14 @@
       <c r="E101" s="15" t="s">
         <v>301</v>
       </c>
+      <c r="K101" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="Q101" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>316</v>
       </c>
@@ -4511,11 +4568,14 @@
       <c r="E102" s="15" t="s">
         <v>301</v>
       </c>
+      <c r="K102" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="Q102" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>318</v>
       </c>
@@ -4528,11 +4588,14 @@
       <c r="E103" s="15" t="s">
         <v>320</v>
       </c>
+      <c r="K103" s="1" t="s">
+        <v>538</v>
+      </c>
       <c r="Q103" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>321</v>
       </c>
@@ -4545,11 +4608,14 @@
       <c r="E104" s="15" t="s">
         <v>323</v>
       </c>
+      <c r="K104" s="1" t="s">
+        <v>674</v>
+      </c>
       <c r="Q104" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>324</v>
       </c>
@@ -4562,11 +4628,14 @@
       <c r="E105" s="15" t="s">
         <v>326</v>
       </c>
+      <c r="K105" s="1" t="s">
+        <v>674</v>
+      </c>
       <c r="Q105" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>327</v>
       </c>
@@ -4579,11 +4648,14 @@
       <c r="E106" s="15" t="s">
         <v>326</v>
       </c>
+      <c r="K106" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="Q106" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>329</v>
       </c>
@@ -4597,9 +4669,12 @@
       <c r="E107" s="5" t="s">
         <v>332</v>
       </c>
+      <c r="K107" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="Q107" s="5"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>333</v>
       </c>
@@ -4613,9 +4688,12 @@
       <c r="E108" s="5" t="s">
         <v>332</v>
       </c>
+      <c r="K108" s="1" t="s">
+        <v>674</v>
+      </c>
       <c r="Q108" s="5"/>
     </row>
-    <row r="109" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>335</v>
       </c>
@@ -4629,9 +4707,12 @@
       <c r="E109" s="5" t="s">
         <v>337</v>
       </c>
+      <c r="K109" s="1" t="s">
+        <v>677</v>
+      </c>
       <c r="Q109" s="5"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>338</v>
       </c>
@@ -4647,7 +4728,7 @@
       </c>
       <c r="Q110" s="5"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>340</v>
       </c>
@@ -4663,7 +4744,7 @@
       </c>
       <c r="Q111" s="5"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>342</v>
       </c>
@@ -4679,7 +4760,7 @@
       </c>
       <c r="Q112" s="5"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>344</v>
       </c>
@@ -4695,7 +4776,7 @@
       </c>
       <c r="Q113" s="5"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>347</v>
       </c>
@@ -4711,7 +4792,7 @@
       </c>
       <c r="Q114" s="5"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>349</v>
       </c>
@@ -4727,7 +4808,7 @@
       </c>
       <c r="Q115" s="5"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>351</v>
       </c>
@@ -4743,7 +4824,7 @@
       </c>
       <c r="Q116" s="5"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>354</v>
       </c>
@@ -4759,7 +4840,7 @@
       </c>
       <c r="Q117" s="5"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>356</v>
       </c>
@@ -4775,7 +4856,7 @@
       </c>
       <c r="Q118" s="5"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>358</v>
       </c>
@@ -4791,7 +4872,7 @@
       </c>
       <c r="Q119" s="5"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>360</v>
       </c>
@@ -4807,7 +4888,7 @@
       </c>
       <c r="Q120" s="5"/>
     </row>
-    <row r="121" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>362</v>
       </c>
@@ -4823,7 +4904,7 @@
       </c>
       <c r="Q121" s="5"/>
     </row>
-    <row r="122" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>365</v>
       </c>
@@ -4839,7 +4920,7 @@
       </c>
       <c r="Q122" s="5"/>
     </row>
-    <row r="123" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>367</v>
       </c>
@@ -4855,7 +4936,7 @@
       </c>
       <c r="Q123" s="5"/>
     </row>
-    <row r="124" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>369</v>
       </c>
@@ -4871,7 +4952,7 @@
       </c>
       <c r="Q124" s="5"/>
     </row>
-    <row r="125" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>371</v>
       </c>
@@ -4887,7 +4968,7 @@
       </c>
       <c r="Q125" s="5"/>
     </row>
-    <row r="126" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>373</v>
       </c>
@@ -4903,7 +4984,7 @@
       </c>
       <c r="Q126" s="5"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
         <v>375</v>
       </c>
@@ -4919,7 +5000,7 @@
       </c>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
         <v>379</v>
       </c>
@@ -4942,7 +5023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
         <v>382</v>
       </c>
@@ -4958,7 +5039,7 @@
       </c>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
         <v>385</v>
       </c>
@@ -4974,7 +5055,7 @@
       </c>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>387</v>
       </c>
@@ -4990,7 +5071,7 @@
       </c>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
         <v>390</v>
       </c>
@@ -5006,7 +5087,7 @@
       </c>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
         <v>393</v>
       </c>
@@ -5022,7 +5103,7 @@
       </c>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>396</v>
       </c>
@@ -5038,7 +5119,7 @@
       </c>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
         <v>399</v>
       </c>
@@ -5054,7 +5135,7 @@
       </c>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
         <v>402</v>
       </c>
@@ -5070,7 +5151,7 @@
       </c>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
         <v>405</v>
       </c>
@@ -5086,7 +5167,7 @@
       </c>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
         <v>408</v>
       </c>
@@ -5102,7 +5183,7 @@
       </c>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
         <v>411</v>
       </c>
@@ -5118,7 +5199,7 @@
       </c>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
         <v>415</v>
       </c>
@@ -5134,7 +5215,7 @@
       </c>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" s="16" t="s">
         <v>418</v>
       </c>
@@ -5150,7 +5231,7 @@
       </c>
       <c r="Q141" s="16"/>
     </row>
-    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
         <v>421</v>
       </c>
@@ -5167,7 +5248,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
         <v>426</v>
       </c>
@@ -5182,7 +5263,7 @@
       </c>
       <c r="Q143" s="17"/>
     </row>
-    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
         <v>429</v>
       </c>
@@ -5199,7 +5280,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
         <v>432</v>
       </c>
@@ -5216,7 +5297,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
         <v>435</v>
       </c>
@@ -5232,7 +5313,7 @@
       </c>
       <c r="Q146" s="17"/>
     </row>
-    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
         <v>438</v>
       </c>
@@ -5248,7 +5329,7 @@
       </c>
       <c r="Q147" s="17"/>
     </row>
-    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
         <v>441</v>
       </c>
@@ -5264,7 +5345,7 @@
       </c>
       <c r="Q148" s="17"/>
     </row>
-    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
         <v>444</v>
       </c>
@@ -5280,7 +5361,7 @@
       </c>
       <c r="Q149" s="17"/>
     </row>
-    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
         <v>447</v>
       </c>
@@ -5296,7 +5377,7 @@
       </c>
       <c r="Q150" s="17"/>
     </row>
-    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
         <v>450</v>
       </c>
@@ -5312,7 +5393,7 @@
       </c>
       <c r="Q151" s="17"/>
     </row>
-    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
         <v>453</v>
       </c>
@@ -5328,7 +5409,7 @@
       </c>
       <c r="Q152" s="17"/>
     </row>
-    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
         <v>456</v>
       </c>
@@ -5344,7 +5425,7 @@
       </c>
       <c r="Q153" s="17"/>
     </row>
-    <row r="154" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>458</v>
       </c>
@@ -5357,8 +5438,11 @@
       <c r="E154" s="18" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="155" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K154" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>462</v>
       </c>
@@ -5374,6 +5458,9 @@
       <c r="E155" s="18" t="s">
         <v>464</v>
       </c>
+      <c r="K155" s="1" t="s">
+        <v>538</v>
+      </c>
       <c r="P155" s="8" t="s">
         <v>30</v>
       </c>
@@ -5381,7 +5468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>465</v>
       </c>
@@ -5394,8 +5481,11 @@
       <c r="E156" s="18" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="157" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K156" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>468</v>
       </c>
@@ -5408,8 +5498,11 @@
       <c r="E157" s="18" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="158" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K157" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>471</v>
       </c>
@@ -5422,8 +5515,11 @@
       <c r="E158" s="18" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="159" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K158" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>474</v>
       </c>
@@ -5436,8 +5532,11 @@
       <c r="E159" s="18" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="160" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K159" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>476</v>
       </c>
@@ -5450,8 +5549,11 @@
       <c r="E160" s="18" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="161" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K160" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>479</v>
       </c>
@@ -5464,8 +5566,11 @@
       <c r="E161" s="18" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="162" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K161" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>482</v>
       </c>
@@ -5478,8 +5583,11 @@
       <c r="E162" s="18" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="163" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K162" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>484</v>
       </c>
@@ -5492,8 +5600,11 @@
       <c r="E163" s="18" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="164" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K163" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>486</v>
       </c>
@@ -5506,8 +5617,11 @@
       <c r="E164" s="18" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="165" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K164" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>489</v>
       </c>
@@ -5520,8 +5634,11 @@
       <c r="E165" s="18" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="166" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K165" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>492</v>
       </c>
@@ -5534,8 +5651,11 @@
       <c r="E166" s="18" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="167" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K166" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>495</v>
       </c>
@@ -5548,8 +5668,11 @@
       <c r="E167" s="18" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="168" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K167" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>498</v>
       </c>
@@ -5562,8 +5685,11 @@
       <c r="E168" s="18" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="169" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K168" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>501</v>
       </c>
@@ -5576,8 +5702,11 @@
       <c r="E169" s="18" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="170" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K169" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>504</v>
       </c>
@@ -5590,8 +5719,11 @@
       <c r="E170" s="18" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="171" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K170" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>507</v>
       </c>
@@ -5604,8 +5736,11 @@
       <c r="E171" s="18" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="172" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K171" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>509</v>
       </c>
@@ -5618,8 +5753,11 @@
       <c r="E172" s="18" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="173" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K172" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>511</v>
       </c>
@@ -5632,8 +5770,11 @@
       <c r="E173" s="18" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="174" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="K173" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>514</v>
       </c>
@@ -5646,8 +5787,11 @@
       <c r="E174" s="18" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="175" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+      <c r="K174" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A175" s="18" t="s">
         <v>517</v>
       </c>
@@ -5670,7 +5814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A176" s="18" t="s">
         <v>521</v>
       </c>
@@ -5693,7 +5837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A177" s="18" t="s">
         <v>524</v>
       </c>
@@ -5716,7 +5860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="72" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A178" s="18" t="s">
         <v>527</v>
       </c>
@@ -5739,7 +5883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="72" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A179" s="18" t="s">
         <v>530</v>
       </c>
@@ -5762,7 +5906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="54" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A180" s="18" t="s">
         <v>532</v>
       </c>
@@ -5785,7 +5929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A181" s="18" t="s">
         <v>535</v>
       </c>
@@ -5811,7 +5955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A182" s="18" t="s">
         <v>539</v>
       </c>
@@ -5837,7 +5981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A183" s="18" t="s">
         <v>542</v>
       </c>
@@ -5863,7 +6007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A184" s="18" t="s">
         <v>545</v>
       </c>
@@ -5889,7 +6033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A185" s="18" t="s">
         <v>548</v>
       </c>
@@ -5915,7 +6059,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A186" s="18" t="s">
         <v>551</v>
       </c>
@@ -5941,7 +6085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A187" s="18" t="s">
         <v>554</v>
       </c>
@@ -5967,7 +6111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="54" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A188" s="18" t="s">
         <v>557</v>
       </c>
@@ -5993,7 +6137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A189" s="18" t="s">
         <v>560</v>
       </c>
@@ -6019,7 +6163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A190" s="18" t="s">
         <v>563</v>
       </c>
@@ -6045,7 +6189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A191" s="18" t="s">
         <v>566</v>
       </c>
@@ -6068,7 +6212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A192" s="18" t="s">
         <v>569</v>
       </c>
@@ -6091,7 +6235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A193" s="18" t="s">
         <v>572</v>
       </c>
@@ -6114,7 +6258,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A194" s="18" t="s">
         <v>575</v>
       </c>
@@ -6137,7 +6281,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A195" s="18" t="s">
         <v>578</v>
       </c>
@@ -6154,7 +6298,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A196" s="18" t="s">
         <v>581</v>
       </c>
@@ -6177,7 +6321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A197" s="18" t="s">
         <v>583</v>
       </c>
@@ -6194,7 +6338,7 @@
       <c r="P197" s="18"/>
       <c r="Q197" s="18"/>
     </row>
-    <row r="198" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A198" s="18" t="s">
         <v>586</v>
       </c>
@@ -6211,7 +6355,7 @@
       <c r="P198" s="18"/>
       <c r="Q198" s="18"/>
     </row>
-    <row r="199" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A199" s="18" t="s">
         <v>589</v>
       </c>
@@ -6234,7 +6378,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A200" s="18" t="s">
         <v>591</v>
       </c>
@@ -6251,7 +6395,7 @@
       <c r="P200" s="18"/>
       <c r="Q200" s="18"/>
     </row>
-    <row r="201" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A201" s="18" t="s">
         <v>594</v>
       </c>
@@ -6274,7 +6418,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A202" s="18" t="s">
         <v>597</v>
       </c>
@@ -6297,7 +6441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A203" s="18" t="s">
         <v>599</v>
       </c>
@@ -6314,7 +6458,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A204" s="18" t="s">
         <v>602</v>
       </c>
@@ -6330,7 +6474,7 @@
       </c>
       <c r="Q204" s="18"/>
     </row>
-    <row r="205" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A205" s="18" t="s">
         <v>605</v>
       </c>
@@ -6346,7 +6490,7 @@
       </c>
       <c r="Q205" s="18"/>
     </row>
-    <row r="206" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
         <v>608</v>
       </c>
@@ -6362,7 +6506,7 @@
       </c>
       <c r="Q206" s="18"/>
     </row>
-    <row r="207" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A207" s="18" t="s">
         <v>611</v>
       </c>
@@ -6385,7 +6529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A208" s="18" t="s">
         <v>614</v>
       </c>
@@ -6408,7 +6552,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="54" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A209" s="18" t="s">
         <v>617</v>
       </c>
@@ -6431,7 +6575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A210" s="18" t="s">
         <v>620</v>
       </c>
@@ -6454,7 +6598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A211" s="18" t="s">
         <v>623</v>
       </c>
@@ -6477,7 +6621,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>626</v>
       </c>
@@ -6494,7 +6638,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>631</v>
       </c>
@@ -6517,7 +6661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>634</v>
       </c>
@@ -6537,7 +6681,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>638</v>
       </c>
@@ -6554,7 +6698,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>642</v>
       </c>
@@ -6574,7 +6718,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>646</v>
       </c>
@@ -6594,7 +6738,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>651</v>
       </c>
@@ -6614,7 +6758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>655</v>
       </c>
@@ -6631,7 +6775,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>658</v>
       </c>
@@ -6649,7 +6793,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>661</v>
       </c>
@@ -6667,7 +6811,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>664</v>
       </c>
@@ -6685,7 +6829,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>667</v>
       </c>
@@ -6719,7 +6863,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Determined untestable reqs and tested getNumberOfAvailableGames
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pier_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BAC183-B340-4A2C-A2F2-5CA785AB6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{24BAC183-B340-4A2C-A2F2-5CA785AB6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA4959AB-C040-4B71-ABAC-FF3F59C461EE}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="34605" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="682">
   <si>
     <t>Tested By</t>
   </si>
@@ -2082,6 +2082,9 @@
   </si>
   <si>
     <t>ut</t>
+  </si>
+  <si>
+    <t>Test 2, Step 4</t>
   </si>
 </sst>
 </file>
@@ -2524,38 +2527,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B188" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M213" sqref="M213"/>
+    <sheetView tabSelected="1" topLeftCell="F222" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="123.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.7109375" style="1"/>
-    <col min="11" max="11" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1"/>
-    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" style="1"/>
-    <col min="20" max="20" width="36.42578125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="36.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="123.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.7265625" style="1"/>
+    <col min="11" max="11" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="1"/>
+    <col min="13" max="13" width="12.81640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13.08984375" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1796875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="8.7265625" style="1"/>
+    <col min="20" max="20" width="36.453125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2616,7 +2619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2647,27 +2650,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2689,6 +2692,9 @@
       <c r="M10" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N10" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P10" s="8" t="s">
         <v>30</v>
       </c>
@@ -2696,7 +2702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -2718,6 +2724,9 @@
       <c r="M11" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P11" s="8" t="s">
         <v>30</v>
       </c>
@@ -2725,7 +2734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -2747,6 +2756,9 @@
       <c r="M12" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P12" s="8" t="s">
         <v>30</v>
       </c>
@@ -2754,7 +2766,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2776,6 +2788,9 @@
       <c r="M13" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N13" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P13" s="8" t="s">
         <v>30</v>
       </c>
@@ -2783,7 +2798,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2803,7 +2818,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
@@ -2822,7 +2837,7 @@
       </c>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2841,7 +2856,7 @@
       </c>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -2861,7 +2876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
@@ -2880,7 +2895,7 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -2899,7 +2914,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2918,7 +2933,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>59</v>
       </c>
@@ -2940,6 +2955,9 @@
       <c r="M21" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N21" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P21" s="8" t="s">
         <v>30</v>
       </c>
@@ -2947,7 +2965,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
@@ -2966,7 +2984,7 @@
       </c>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>64</v>
       </c>
@@ -2988,6 +3006,9 @@
       <c r="M23" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N23" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P23" s="8" t="s">
         <v>30</v>
       </c>
@@ -2995,7 +3016,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -3018,6 +3039,9 @@
       <c r="M24" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N24" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P24" s="8" t="s">
         <v>30</v>
       </c>
@@ -3025,7 +3049,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -3048,6 +3072,9 @@
       <c r="M25" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N25" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P25" s="8" t="s">
         <v>30</v>
       </c>
@@ -3055,7 +3082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -3075,8 +3102,11 @@
       <c r="M26" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -3099,6 +3129,9 @@
       <c r="M27" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N27" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P27" s="8" t="s">
         <v>30</v>
       </c>
@@ -3106,7 +3139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -3129,7 +3162,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -3150,7 +3183,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -3171,11 +3204,14 @@
       <c r="M30" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N30" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="Q30" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
@@ -3198,7 +3234,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
@@ -3218,7 +3254,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
@@ -3234,8 +3270,11 @@
       <c r="K33" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N33" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -3251,8 +3290,11 @@
       <c r="K34" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N34" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
@@ -3284,7 +3326,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>107</v>
       </c>
@@ -3316,7 +3358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -3348,7 +3390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3380,7 +3422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -3402,6 +3444,9 @@
       <c r="M39" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N39" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P39" s="8" t="s">
         <v>30</v>
       </c>
@@ -3409,7 +3454,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>118</v>
       </c>
@@ -3431,6 +3476,9 @@
       <c r="M40" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N40" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P40" s="8" t="s">
         <v>30</v>
       </c>
@@ -3438,7 +3486,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -3460,6 +3508,9 @@
       <c r="M41" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N41" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P41" s="8" t="s">
         <v>30</v>
       </c>
@@ -3467,7 +3518,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -3484,7 +3535,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -3506,6 +3557,9 @@
       <c r="M43" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N43" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P43" s="8" t="s">
         <v>30</v>
       </c>
@@ -3513,7 +3567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -3535,6 +3589,9 @@
       <c r="M44" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N44" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P44" s="8" t="s">
         <v>30</v>
       </c>
@@ -3542,7 +3599,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -3559,7 +3616,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -3579,7 +3636,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
@@ -3596,7 +3653,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -3613,7 +3670,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -3630,7 +3687,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -3652,6 +3709,9 @@
       <c r="M50" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N50" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P50" s="8" t="s">
         <v>30</v>
       </c>
@@ -3659,7 +3719,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
@@ -3676,7 +3736,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>156</v>
       </c>
@@ -3693,7 +3753,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>158</v>
       </c>
@@ -3710,7 +3770,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -3727,7 +3787,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
@@ -3744,7 +3804,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>164</v>
       </c>
@@ -3766,6 +3826,9 @@
       <c r="M56" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N56" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P56" s="8" t="s">
         <v>30</v>
       </c>
@@ -3773,7 +3836,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>166</v>
       </c>
@@ -3798,6 +3861,9 @@
       <c r="M57" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N57" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P57" s="8" t="s">
         <v>30</v>
       </c>
@@ -3805,7 +3871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
@@ -3827,6 +3893,9 @@
       <c r="M58" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N58" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P58" s="8" t="s">
         <v>30</v>
       </c>
@@ -3834,7 +3903,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>175</v>
       </c>
@@ -3856,6 +3925,9 @@
       <c r="M59" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N59" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P59" s="8" t="s">
         <v>30</v>
       </c>
@@ -3863,7 +3935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>179</v>
       </c>
@@ -3882,8 +3954,11 @@
       <c r="M60" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="N60" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>183</v>
       </c>
@@ -3905,6 +3980,9 @@
       <c r="M61" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N61" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P61" s="8" t="s">
         <v>30</v>
       </c>
@@ -3912,7 +3990,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>187</v>
       </c>
@@ -3932,7 +4010,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>191</v>
       </c>
@@ -3954,6 +4032,9 @@
       <c r="M63" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N63" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P63" s="8" t="s">
         <v>30</v>
       </c>
@@ -3961,7 +4042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
@@ -3983,6 +4064,9 @@
       <c r="M64" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N64" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P64" s="8" t="s">
         <v>30</v>
       </c>
@@ -3990,7 +4074,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>199</v>
       </c>
@@ -4010,7 +4094,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>203</v>
       </c>
@@ -4027,7 +4111,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>206</v>
       </c>
@@ -4049,6 +4133,9 @@
       <c r="M67" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N67" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P67" s="8" t="s">
         <v>30</v>
       </c>
@@ -4056,7 +4143,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>209</v>
       </c>
@@ -4076,7 +4163,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>212</v>
       </c>
@@ -4096,7 +4183,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>215</v>
       </c>
@@ -4113,7 +4200,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>218</v>
       </c>
@@ -4132,8 +4219,11 @@
       <c r="M71" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N71" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>221</v>
       </c>
@@ -4153,7 +4243,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>224</v>
       </c>
@@ -4175,6 +4265,9 @@
       <c r="M73" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N73" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P73" s="8" t="s">
         <v>30</v>
       </c>
@@ -4182,7 +4275,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>228</v>
       </c>
@@ -4199,7 +4292,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>232</v>
       </c>
@@ -4221,6 +4314,9 @@
       <c r="M75" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N75" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P75" s="8" t="s">
         <v>30</v>
       </c>
@@ -4228,7 +4324,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>236</v>
       </c>
@@ -4247,8 +4343,11 @@
       <c r="M76" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N76" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>239</v>
       </c>
@@ -4265,7 +4364,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>242</v>
       </c>
@@ -4285,7 +4384,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>245</v>
       </c>
@@ -4304,8 +4403,11 @@
       <c r="M79" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N79" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>249</v>
       </c>
@@ -4327,6 +4429,9 @@
       <c r="M80" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N80" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P80" s="8" t="s">
         <v>30</v>
       </c>
@@ -4334,7 +4439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>252</v>
       </c>
@@ -4354,7 +4459,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>255</v>
       </c>
@@ -4374,7 +4479,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>258</v>
       </c>
@@ -4394,7 +4499,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>261</v>
       </c>
@@ -4413,8 +4518,11 @@
       <c r="M84" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N84" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>264</v>
       </c>
@@ -4433,8 +4541,11 @@
       <c r="M85" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N85" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>267</v>
       </c>
@@ -4453,8 +4564,11 @@
       <c r="M86" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N86" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>270</v>
       </c>
@@ -4473,8 +4587,11 @@
       <c r="M87" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="88" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="N87" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>273</v>
       </c>
@@ -4496,6 +4613,9 @@
       <c r="M88" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N88" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P88" s="8" t="s">
         <v>30</v>
       </c>
@@ -4503,7 +4623,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>276</v>
       </c>
@@ -4522,8 +4642,11 @@
       <c r="M89" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N89" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>279</v>
       </c>
@@ -4542,8 +4665,11 @@
       <c r="M90" s="1" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N90" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>282</v>
       </c>
@@ -4563,7 +4689,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>287</v>
       </c>
@@ -4583,7 +4709,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>289</v>
       </c>
@@ -4603,7 +4729,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>293</v>
       </c>
@@ -4623,7 +4749,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
@@ -4643,7 +4769,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -4663,7 +4789,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>302</v>
       </c>
@@ -4680,7 +4806,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>305</v>
       </c>
@@ -4697,7 +4823,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>308</v>
       </c>
@@ -4714,7 +4840,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -4736,6 +4862,9 @@
       <c r="M100" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N100" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P100" s="8" t="s">
         <v>30</v>
       </c>
@@ -4743,7 +4872,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>314</v>
       </c>
@@ -4763,7 +4892,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>316</v>
       </c>
@@ -4783,7 +4912,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>318</v>
       </c>
@@ -4803,7 +4932,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>321</v>
       </c>
@@ -4823,7 +4952,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>324</v>
       </c>
@@ -4843,7 +4972,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>327</v>
       </c>
@@ -4863,7 +4992,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>329</v>
       </c>
@@ -4882,7 +5011,7 @@
       </c>
       <c r="Q107" s="5"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>333</v>
       </c>
@@ -4901,7 +5030,7 @@
       </c>
       <c r="Q108" s="5"/>
     </row>
-    <row r="109" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>335</v>
       </c>
@@ -4920,7 +5049,7 @@
       </c>
       <c r="Q109" s="5"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>338</v>
       </c>
@@ -4936,7 +5065,7 @@
       </c>
       <c r="Q110" s="5"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>340</v>
       </c>
@@ -4952,7 +5081,7 @@
       </c>
       <c r="Q111" s="5"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>342</v>
       </c>
@@ -4968,7 +5097,7 @@
       </c>
       <c r="Q112" s="5"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>344</v>
       </c>
@@ -4984,7 +5113,7 @@
       </c>
       <c r="Q113" s="5"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>347</v>
       </c>
@@ -5000,7 +5129,7 @@
       </c>
       <c r="Q114" s="5"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>349</v>
       </c>
@@ -5016,7 +5145,7 @@
       </c>
       <c r="Q115" s="5"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>351</v>
       </c>
@@ -5032,7 +5161,7 @@
       </c>
       <c r="Q116" s="5"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>354</v>
       </c>
@@ -5048,7 +5177,7 @@
       </c>
       <c r="Q117" s="5"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>356</v>
       </c>
@@ -5064,7 +5193,7 @@
       </c>
       <c r="Q118" s="5"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>358</v>
       </c>
@@ -5080,7 +5209,7 @@
       </c>
       <c r="Q119" s="5"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>360</v>
       </c>
@@ -5096,7 +5225,7 @@
       </c>
       <c r="Q120" s="5"/>
     </row>
-    <row r="121" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>362</v>
       </c>
@@ -5112,7 +5241,7 @@
       </c>
       <c r="Q121" s="5"/>
     </row>
-    <row r="122" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>365</v>
       </c>
@@ -5128,7 +5257,7 @@
       </c>
       <c r="Q122" s="5"/>
     </row>
-    <row r="123" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>367</v>
       </c>
@@ -5144,7 +5273,7 @@
       </c>
       <c r="Q123" s="5"/>
     </row>
-    <row r="124" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>369</v>
       </c>
@@ -5160,7 +5289,7 @@
       </c>
       <c r="Q124" s="5"/>
     </row>
-    <row r="125" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>371</v>
       </c>
@@ -5176,7 +5305,7 @@
       </c>
       <c r="Q125" s="5"/>
     </row>
-    <row r="126" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>373</v>
       </c>
@@ -5192,7 +5321,7 @@
       </c>
       <c r="Q126" s="5"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A127" s="10" t="s">
         <v>375</v>
       </c>
@@ -5208,7 +5337,7 @@
       </c>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A128" s="10" t="s">
         <v>379</v>
       </c>
@@ -5227,6 +5356,9 @@
       <c r="M128" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N128" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P128" s="8" t="s">
         <v>30</v>
       </c>
@@ -5234,7 +5366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="s">
         <v>382</v>
       </c>
@@ -5250,7 +5382,7 @@
       </c>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A130" s="10" t="s">
         <v>385</v>
       </c>
@@ -5266,7 +5398,7 @@
       </c>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A131" s="10" t="s">
         <v>387</v>
       </c>
@@ -5282,7 +5414,7 @@
       </c>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A132" s="10" t="s">
         <v>390</v>
       </c>
@@ -5298,7 +5430,7 @@
       </c>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A133" s="10" t="s">
         <v>393</v>
       </c>
@@ -5314,7 +5446,7 @@
       </c>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A134" s="10" t="s">
         <v>396</v>
       </c>
@@ -5330,7 +5462,7 @@
       </c>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A135" s="10" t="s">
         <v>399</v>
       </c>
@@ -5346,7 +5478,7 @@
       </c>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A136" s="10" t="s">
         <v>402</v>
       </c>
@@ -5362,7 +5494,7 @@
       </c>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A137" s="10" t="s">
         <v>405</v>
       </c>
@@ -5378,7 +5510,7 @@
       </c>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A138" s="10" t="s">
         <v>408</v>
       </c>
@@ -5394,7 +5526,7 @@
       </c>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="s">
         <v>411</v>
       </c>
@@ -5410,7 +5542,7 @@
       </c>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A140" s="10" t="s">
         <v>415</v>
       </c>
@@ -5426,7 +5558,7 @@
       </c>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" ht="16" x14ac:dyDescent="0.4">
       <c r="A141" s="16" t="s">
         <v>418</v>
       </c>
@@ -5442,7 +5574,7 @@
       </c>
       <c r="Q141" s="16"/>
     </row>
-    <row r="142" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A142" s="17" t="s">
         <v>421</v>
       </c>
@@ -5462,7 +5594,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A143" s="17" t="s">
         <v>426</v>
       </c>
@@ -5480,7 +5612,7 @@
       </c>
       <c r="Q143" s="17"/>
     </row>
-    <row r="144" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A144" s="17" t="s">
         <v>429</v>
       </c>
@@ -5500,7 +5632,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="17" t="s">
         <v>432</v>
       </c>
@@ -5520,7 +5652,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A146" s="17" t="s">
         <v>435</v>
       </c>
@@ -5539,7 +5671,7 @@
       </c>
       <c r="Q146" s="17"/>
     </row>
-    <row r="147" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A147" s="17" t="s">
         <v>438</v>
       </c>
@@ -5558,7 +5690,7 @@
       </c>
       <c r="Q147" s="17"/>
     </row>
-    <row r="148" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A148" s="17" t="s">
         <v>441</v>
       </c>
@@ -5577,7 +5709,7 @@
       </c>
       <c r="Q148" s="17"/>
     </row>
-    <row r="149" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A149" s="17" t="s">
         <v>444</v>
       </c>
@@ -5596,7 +5728,7 @@
       </c>
       <c r="Q149" s="17"/>
     </row>
-    <row r="150" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A150" s="17" t="s">
         <v>447</v>
       </c>
@@ -5615,7 +5747,7 @@
       </c>
       <c r="Q150" s="17"/>
     </row>
-    <row r="151" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A151" s="17" t="s">
         <v>450</v>
       </c>
@@ -5634,7 +5766,7 @@
       </c>
       <c r="Q151" s="17"/>
     </row>
-    <row r="152" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A152" s="17" t="s">
         <v>453</v>
       </c>
@@ -5653,7 +5785,7 @@
       </c>
       <c r="Q152" s="17"/>
     </row>
-    <row r="153" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A153" s="17" t="s">
         <v>456</v>
       </c>
@@ -5672,7 +5804,7 @@
       </c>
       <c r="Q153" s="17"/>
     </row>
-    <row r="154" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A154" s="1" t="s">
         <v>458</v>
       </c>
@@ -5689,7 +5821,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A155" s="1" t="s">
         <v>462</v>
       </c>
@@ -5711,6 +5843,9 @@
       <c r="M155" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N155" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P155" s="8" t="s">
         <v>30</v>
       </c>
@@ -5718,7 +5853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A156" s="1" t="s">
         <v>465</v>
       </c>
@@ -5735,7 +5870,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A157" s="1" t="s">
         <v>468</v>
       </c>
@@ -5752,7 +5887,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A158" s="1" t="s">
         <v>471</v>
       </c>
@@ -5769,7 +5904,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A159" s="1" t="s">
         <v>474</v>
       </c>
@@ -5786,7 +5921,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A160" s="1" t="s">
         <v>476</v>
       </c>
@@ -5803,7 +5938,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
         <v>479</v>
       </c>
@@ -5820,7 +5955,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A162" s="1" t="s">
         <v>482</v>
       </c>
@@ -5837,7 +5972,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A163" s="1" t="s">
         <v>484</v>
       </c>
@@ -5854,7 +5989,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A164" s="1" t="s">
         <v>486</v>
       </c>
@@ -5871,7 +6006,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A165" s="1" t="s">
         <v>489</v>
       </c>
@@ -5888,7 +6023,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A166" s="1" t="s">
         <v>492</v>
       </c>
@@ -5905,7 +6040,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A167" s="1" t="s">
         <v>495</v>
       </c>
@@ -5922,7 +6057,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
         <v>498</v>
       </c>
@@ -5939,7 +6074,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A169" s="1" t="s">
         <v>501</v>
       </c>
@@ -5956,7 +6091,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
         <v>504</v>
       </c>
@@ -5973,7 +6108,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A171" s="1" t="s">
         <v>507</v>
       </c>
@@ -5990,7 +6125,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A172" s="1" t="s">
         <v>509</v>
       </c>
@@ -6007,7 +6142,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A173" s="1" t="s">
         <v>511</v>
       </c>
@@ -6024,7 +6159,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A174" s="1" t="s">
         <v>514</v>
       </c>
@@ -6041,7 +6176,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A175" s="18" t="s">
         <v>517</v>
       </c>
@@ -6060,6 +6195,9 @@
       <c r="M175" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N175" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P175" s="8" t="s">
         <v>30</v>
       </c>
@@ -6067,7 +6205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A176" s="18" t="s">
         <v>521</v>
       </c>
@@ -6086,6 +6224,9 @@
       <c r="M176" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N176" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P176" s="8" t="s">
         <v>30</v>
       </c>
@@ -6093,7 +6234,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A177" s="18" t="s">
         <v>524</v>
       </c>
@@ -6112,6 +6253,9 @@
       <c r="M177" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N177" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P177" s="8" t="s">
         <v>30</v>
       </c>
@@ -6119,7 +6263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="75" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" ht="74" x14ac:dyDescent="0.45">
       <c r="A178" s="18" t="s">
         <v>527</v>
       </c>
@@ -6138,6 +6282,9 @@
       <c r="M178" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N178" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P178" s="8" t="s">
         <v>30</v>
       </c>
@@ -6145,7 +6292,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="75" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" ht="74" x14ac:dyDescent="0.45">
       <c r="A179" s="18" t="s">
         <v>530</v>
       </c>
@@ -6164,6 +6311,9 @@
       <c r="M179" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N179" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P179" s="8" t="s">
         <v>30</v>
       </c>
@@ -6171,7 +6321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A180" s="18" t="s">
         <v>532</v>
       </c>
@@ -6190,6 +6340,9 @@
       <c r="M180" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N180" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P180" s="8" t="s">
         <v>30</v>
       </c>
@@ -6197,7 +6350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A181" s="18" t="s">
         <v>535</v>
       </c>
@@ -6219,6 +6372,9 @@
       <c r="M181" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N181" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P181" s="8" t="s">
         <v>30</v>
       </c>
@@ -6226,7 +6382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A182" s="18" t="s">
         <v>539</v>
       </c>
@@ -6248,6 +6404,9 @@
       <c r="M182" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N182" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P182" s="8" t="s">
         <v>30</v>
       </c>
@@ -6255,7 +6414,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A183" s="18" t="s">
         <v>542</v>
       </c>
@@ -6277,6 +6436,9 @@
       <c r="M183" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N183" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P183" s="8" t="s">
         <v>30</v>
       </c>
@@ -6284,7 +6446,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A184" s="18" t="s">
         <v>545</v>
       </c>
@@ -6306,6 +6468,9 @@
       <c r="M184" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N184" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P184" s="8" t="s">
         <v>30</v>
       </c>
@@ -6313,7 +6478,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A185" s="18" t="s">
         <v>548</v>
       </c>
@@ -6335,6 +6500,9 @@
       <c r="M185" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N185" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P185" s="8" t="s">
         <v>30</v>
       </c>
@@ -6342,7 +6510,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A186" s="18" t="s">
         <v>551</v>
       </c>
@@ -6364,6 +6532,9 @@
       <c r="M186" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N186" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P186" s="8" t="s">
         <v>30</v>
       </c>
@@ -6371,7 +6542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A187" s="18" t="s">
         <v>554</v>
       </c>
@@ -6393,6 +6564,9 @@
       <c r="M187" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N187" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P187" s="8" t="s">
         <v>30</v>
       </c>
@@ -6400,7 +6574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A188" s="18" t="s">
         <v>557</v>
       </c>
@@ -6422,6 +6596,9 @@
       <c r="M188" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N188" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P188" s="8" t="s">
         <v>30</v>
       </c>
@@ -6429,7 +6606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A189" s="18" t="s">
         <v>560</v>
       </c>
@@ -6451,6 +6628,9 @@
       <c r="M189" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N189" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P189" s="8" t="s">
         <v>30</v>
       </c>
@@ -6458,7 +6638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A190" s="18" t="s">
         <v>563</v>
       </c>
@@ -6480,6 +6660,9 @@
       <c r="M190" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N190" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P190" s="8" t="s">
         <v>30</v>
       </c>
@@ -6487,7 +6670,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A191" s="18" t="s">
         <v>566</v>
       </c>
@@ -6506,6 +6689,9 @@
       <c r="M191" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N191" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P191" s="8" t="s">
         <v>30</v>
       </c>
@@ -6513,7 +6699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A192" s="18" t="s">
         <v>569</v>
       </c>
@@ -6532,6 +6718,9 @@
       <c r="M192" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N192" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P192" s="8" t="s">
         <v>30</v>
       </c>
@@ -6539,7 +6728,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A193" s="18" t="s">
         <v>572</v>
       </c>
@@ -6558,6 +6747,9 @@
       <c r="M193" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N193" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P193" s="8" t="s">
         <v>30</v>
       </c>
@@ -6565,7 +6757,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A194" s="18" t="s">
         <v>575</v>
       </c>
@@ -6584,6 +6776,9 @@
       <c r="M194" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N194" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P194" s="8" t="s">
         <v>30</v>
       </c>
@@ -6591,7 +6786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A195" s="18" t="s">
         <v>578</v>
       </c>
@@ -6608,7 +6803,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A196" s="18" t="s">
         <v>581</v>
       </c>
@@ -6627,6 +6822,9 @@
       <c r="M196" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N196" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P196" s="8" t="s">
         <v>30</v>
       </c>
@@ -6634,7 +6832,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A197" s="18" t="s">
         <v>583</v>
       </c>
@@ -6651,7 +6849,7 @@
       <c r="P197" s="18"/>
       <c r="Q197" s="18"/>
     </row>
-    <row r="198" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A198" s="18" t="s">
         <v>586</v>
       </c>
@@ -6668,7 +6866,7 @@
       <c r="P198" s="18"/>
       <c r="Q198" s="18"/>
     </row>
-    <row r="199" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A199" s="18" t="s">
         <v>589</v>
       </c>
@@ -6687,6 +6885,9 @@
       <c r="M199" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N199" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P199" s="8" t="s">
         <v>30</v>
       </c>
@@ -6694,7 +6895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A200" s="18" t="s">
         <v>591</v>
       </c>
@@ -6711,7 +6912,7 @@
       <c r="P200" s="18"/>
       <c r="Q200" s="18"/>
     </row>
-    <row r="201" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A201" s="18" t="s">
         <v>594</v>
       </c>
@@ -6730,6 +6931,9 @@
       <c r="M201" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N201" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P201" s="8" t="s">
         <v>30</v>
       </c>
@@ -6737,7 +6941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A202" s="18" t="s">
         <v>597</v>
       </c>
@@ -6756,6 +6960,9 @@
       <c r="M202" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N202" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P202" s="8" t="s">
         <v>30</v>
       </c>
@@ -6763,7 +6970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A203" s="18" t="s">
         <v>599</v>
       </c>
@@ -6780,7 +6987,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A204" s="18" t="s">
         <v>602</v>
       </c>
@@ -6796,7 +7003,7 @@
       </c>
       <c r="Q204" s="18"/>
     </row>
-    <row r="205" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A205" s="18" t="s">
         <v>605</v>
       </c>
@@ -6812,7 +7019,7 @@
       </c>
       <c r="Q205" s="18"/>
     </row>
-    <row r="206" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A206" s="18" t="s">
         <v>608</v>
       </c>
@@ -6828,7 +7035,7 @@
       </c>
       <c r="Q206" s="18"/>
     </row>
-    <row r="207" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A207" s="18" t="s">
         <v>611</v>
       </c>
@@ -6847,6 +7054,9 @@
       <c r="M207" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N207" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P207" s="8" t="s">
         <v>30</v>
       </c>
@@ -6854,7 +7064,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A208" s="18" t="s">
         <v>614</v>
       </c>
@@ -6873,6 +7083,9 @@
       <c r="M208" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N208" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P208" s="8" t="s">
         <v>30</v>
       </c>
@@ -6880,7 +7093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="75" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A209" s="18" t="s">
         <v>617</v>
       </c>
@@ -6899,6 +7112,9 @@
       <c r="M209" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N209" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P209" s="8" t="s">
         <v>30</v>
       </c>
@@ -6906,7 +7122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A210" s="18" t="s">
         <v>620</v>
       </c>
@@ -6925,6 +7141,9 @@
       <c r="M210" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N210" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P210" s="8" t="s">
         <v>30</v>
       </c>
@@ -6932,7 +7151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A211" s="18" t="s">
         <v>623</v>
       </c>
@@ -6951,6 +7170,9 @@
       <c r="M211" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N211" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P211" s="8" t="s">
         <v>30</v>
       </c>
@@ -6958,7 +7180,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>626</v>
       </c>
@@ -6975,7 +7197,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>631</v>
       </c>
@@ -6994,6 +7216,9 @@
       <c r="M213" s="1" t="s">
         <v>538</v>
       </c>
+      <c r="N213" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="P213" s="8" t="s">
         <v>30</v>
       </c>
@@ -7001,7 +7226,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>634</v>
       </c>
@@ -7021,7 +7246,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>638</v>
       </c>
@@ -7038,7 +7263,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>642</v>
       </c>
@@ -7058,7 +7283,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>646</v>
       </c>
@@ -7078,7 +7303,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>651</v>
       </c>
@@ -7098,7 +7323,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>655</v>
       </c>
@@ -7115,7 +7340,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>658</v>
       </c>
@@ -7133,7 +7358,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>661</v>
       </c>
@@ -7151,7 +7376,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>664</v>
       </c>
@@ -7169,7 +7394,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>667</v>
       </c>
@@ -7203,7 +7428,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished testable reqs for GM
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{24BAC183-B340-4A2C-A2F2-5CA785AB6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA4959AB-C040-4B71-ABAC-FF3F59C461EE}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{24BAC183-B340-4A2C-A2F2-5CA785AB6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6175BE79-1F09-4F9F-9FBC-86540886BE22}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="683">
   <si>
     <t>Tested By</t>
   </si>
@@ -2085,6 +2085,9 @@
   </si>
   <si>
     <t>Test 2, Step 4</t>
+  </si>
+  <si>
+    <t>Test 10, Step 3</t>
   </si>
 </sst>
 </file>
@@ -2527,8 +2530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F222" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2544,7 +2547,7 @@
     <col min="11" max="11" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.7265625" style="1"/>
     <col min="13" max="13" width="12.81640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.08984375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
     <col min="15" max="16" width="9.453125" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.1796875" style="1" customWidth="1"/>
     <col min="18" max="18" width="10.81640625" style="3" customWidth="1"/>
@@ -3533,6 +3536,9 @@
       </c>
       <c r="K42" s="1" t="s">
         <v>671</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update test for Bot 2
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/FinalRequirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardankarki/Desktop/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{24BAC183-B340-4A2C-A2F2-5CA785AB6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6175BE79-1F09-4F9F-9FBC-86540886BE22}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C466EA3-9A60-E744-A48A-C83CAAAE85E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="683">
   <si>
     <t>Tested By</t>
   </si>
@@ -2530,38 +2530,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="E104" zoomScale="93" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K130" sqref="K130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="36.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="123.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.7265625" style="1"/>
-    <col min="11" max="11" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="1"/>
-    <col min="13" max="13" width="12.81640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.81640625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1796875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.81640625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="8.7265625" style="1"/>
-    <col min="20" max="20" width="36.453125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="36.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="123.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.6640625" style="1"/>
+    <col min="11" max="11" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="1"/>
+    <col min="13" max="13" width="12.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" style="1"/>
+    <col min="20" max="20" width="36.5" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2653,27 +2653,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>59</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>64</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>107</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>118</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>156</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>158</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>164</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>166</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>175</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>179</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>183</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>187</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>191</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>199</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>203</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>206</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>209</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>212</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>215</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>218</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>221</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>224</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>228</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>232</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>236</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>239</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>242</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>245</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>249</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>252</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>255</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>258</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>261</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>264</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>267</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>270</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>273</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>276</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>279</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>282</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>287</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>289</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>293</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>302</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>305</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>308</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>314</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>316</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>318</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>321</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>324</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>327</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>329</v>
       </c>
@@ -5017,7 +5017,7 @@
       </c>
       <c r="Q107" s="5"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>333</v>
       </c>
@@ -5036,7 +5036,7 @@
       </c>
       <c r="Q108" s="5"/>
     </row>
-    <row r="109" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>335</v>
       </c>
@@ -5055,7 +5055,7 @@
       </c>
       <c r="Q109" s="5"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>338</v>
       </c>
@@ -5071,7 +5071,7 @@
       </c>
       <c r="Q110" s="5"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>340</v>
       </c>
@@ -5087,7 +5087,7 @@
       </c>
       <c r="Q111" s="5"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>342</v>
       </c>
@@ -5103,7 +5103,7 @@
       </c>
       <c r="Q112" s="5"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>344</v>
       </c>
@@ -5119,7 +5119,7 @@
       </c>
       <c r="Q113" s="5"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>347</v>
       </c>
@@ -5135,7 +5135,7 @@
       </c>
       <c r="Q114" s="5"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>349</v>
       </c>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="Q115" s="5"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>351</v>
       </c>
@@ -5167,7 +5167,7 @@
       </c>
       <c r="Q116" s="5"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>354</v>
       </c>
@@ -5183,7 +5183,7 @@
       </c>
       <c r="Q117" s="5"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>356</v>
       </c>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="Q118" s="5"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>358</v>
       </c>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="Q119" s="5"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>360</v>
       </c>
@@ -5231,7 +5231,7 @@
       </c>
       <c r="Q120" s="5"/>
     </row>
-    <row r="121" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>362</v>
       </c>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="Q121" s="5"/>
     </row>
-    <row r="122" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>365</v>
       </c>
@@ -5263,7 +5263,7 @@
       </c>
       <c r="Q122" s="5"/>
     </row>
-    <row r="123" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>367</v>
       </c>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="Q123" s="5"/>
     </row>
-    <row r="124" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>369</v>
       </c>
@@ -5295,7 +5295,7 @@
       </c>
       <c r="Q124" s="5"/>
     </row>
-    <row r="125" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>371</v>
       </c>
@@ -5311,7 +5311,7 @@
       </c>
       <c r="Q125" s="5"/>
     </row>
-    <row r="126" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>373</v>
       </c>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="Q126" s="5"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
         <v>375</v>
       </c>
@@ -5341,9 +5341,12 @@
       <c r="E127" s="10" t="s">
         <v>378</v>
       </c>
+      <c r="K127" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
         <v>379</v>
       </c>
@@ -5359,6 +5362,9 @@
       <c r="E128" s="10" t="s">
         <v>381</v>
       </c>
+      <c r="K128" s="1" t="s">
+        <v>673</v>
+      </c>
       <c r="M128" s="1" t="s">
         <v>538</v>
       </c>
@@ -5372,7 +5378,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
         <v>382</v>
       </c>
@@ -5386,9 +5392,12 @@
       <c r="E129" s="10" t="s">
         <v>384</v>
       </c>
+      <c r="K129" s="1" t="s">
+        <v>538</v>
+      </c>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
         <v>385</v>
       </c>
@@ -5402,9 +5411,12 @@
       <c r="E130" s="10" t="s">
         <v>378</v>
       </c>
+      <c r="K130" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>387</v>
       </c>
@@ -5418,9 +5430,12 @@
       <c r="E131" s="10" t="s">
         <v>389</v>
       </c>
+      <c r="K131" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
         <v>390</v>
       </c>
@@ -5434,9 +5449,12 @@
       <c r="E132" s="10" t="s">
         <v>392</v>
       </c>
+      <c r="K132" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
         <v>393</v>
       </c>
@@ -5450,9 +5468,12 @@
       <c r="E133" s="10" t="s">
         <v>395</v>
       </c>
+      <c r="K133" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
         <v>396</v>
       </c>
@@ -5466,9 +5487,12 @@
       <c r="E134" s="10" t="s">
         <v>398</v>
       </c>
+      <c r="K134" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
         <v>399</v>
       </c>
@@ -5482,9 +5506,12 @@
       <c r="E135" s="10" t="s">
         <v>401</v>
       </c>
+      <c r="K135" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
         <v>402</v>
       </c>
@@ -5498,9 +5525,12 @@
       <c r="E136" s="10" t="s">
         <v>404</v>
       </c>
+      <c r="K136" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
         <v>405</v>
       </c>
@@ -5514,9 +5544,12 @@
       <c r="E137" s="10" t="s">
         <v>407</v>
       </c>
+      <c r="K137" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
         <v>408</v>
       </c>
@@ -5530,9 +5563,12 @@
       <c r="E138" s="10" t="s">
         <v>410</v>
       </c>
+      <c r="K138" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
         <v>411</v>
       </c>
@@ -5546,9 +5582,12 @@
       <c r="E139" s="10" t="s">
         <v>414</v>
       </c>
+      <c r="K139" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
         <v>415</v>
       </c>
@@ -5562,9 +5601,12 @@
       <c r="E140" s="10" t="s">
         <v>417</v>
       </c>
+      <c r="K140" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" ht="16" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" s="16" t="s">
         <v>418</v>
       </c>
@@ -5578,9 +5620,12 @@
       <c r="E141" s="1" t="s">
         <v>420</v>
       </c>
+      <c r="K141" s="1" t="s">
+        <v>679</v>
+      </c>
       <c r="Q141" s="16"/>
     </row>
-    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
         <v>421</v>
       </c>
@@ -5600,7 +5645,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
         <v>426</v>
       </c>
@@ -5618,7 +5663,7 @@
       </c>
       <c r="Q143" s="17"/>
     </row>
-    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
         <v>429</v>
       </c>
@@ -5638,7 +5683,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
         <v>432</v>
       </c>
@@ -5658,7 +5703,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
         <v>435</v>
       </c>
@@ -5677,7 +5722,7 @@
       </c>
       <c r="Q146" s="17"/>
     </row>
-    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
         <v>438</v>
       </c>
@@ -5696,7 +5741,7 @@
       </c>
       <c r="Q147" s="17"/>
     </row>
-    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
         <v>441</v>
       </c>
@@ -5715,7 +5760,7 @@
       </c>
       <c r="Q148" s="17"/>
     </row>
-    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
         <v>444</v>
       </c>
@@ -5734,7 +5779,7 @@
       </c>
       <c r="Q149" s="17"/>
     </row>
-    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
         <v>447</v>
       </c>
@@ -5753,7 +5798,7 @@
       </c>
       <c r="Q150" s="17"/>
     </row>
-    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
         <v>450</v>
       </c>
@@ -5772,7 +5817,7 @@
       </c>
       <c r="Q151" s="17"/>
     </row>
-    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
         <v>453</v>
       </c>
@@ -5791,7 +5836,7 @@
       </c>
       <c r="Q152" s="17"/>
     </row>
-    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
         <v>456</v>
       </c>
@@ -5810,7 +5855,7 @@
       </c>
       <c r="Q153" s="17"/>
     </row>
-    <row r="154" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>458</v>
       </c>
@@ -5827,7 +5872,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>462</v>
       </c>
@@ -5859,7 +5904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>465</v>
       </c>
@@ -5876,7 +5921,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>468</v>
       </c>
@@ -5893,7 +5938,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>471</v>
       </c>
@@ -5910,7 +5955,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>474</v>
       </c>
@@ -5927,7 +5972,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>476</v>
       </c>
@@ -5944,7 +5989,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>479</v>
       </c>
@@ -5961,7 +6006,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>482</v>
       </c>
@@ -5978,7 +6023,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>484</v>
       </c>
@@ -5995,7 +6040,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>486</v>
       </c>
@@ -6012,7 +6057,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>489</v>
       </c>
@@ -6029,7 +6074,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>492</v>
       </c>
@@ -6046,7 +6091,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>495</v>
       </c>
@@ -6063,7 +6108,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>498</v>
       </c>
@@ -6080,7 +6125,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>501</v>
       </c>
@@ -6097,7 +6142,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>504</v>
       </c>
@@ -6114,7 +6159,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>507</v>
       </c>
@@ -6131,7 +6176,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>509</v>
       </c>
@@ -6148,7 +6193,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>511</v>
       </c>
@@ -6165,7 +6210,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>514</v>
       </c>
@@ -6182,7 +6227,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A175" s="18" t="s">
         <v>517</v>
       </c>
@@ -6211,7 +6256,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A176" s="18" t="s">
         <v>521</v>
       </c>
@@ -6240,7 +6285,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A177" s="18" t="s">
         <v>524</v>
       </c>
@@ -6269,7 +6314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="74" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A178" s="18" t="s">
         <v>527</v>
       </c>
@@ -6298,7 +6343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="74" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:17" ht="80" x14ac:dyDescent="0.25">
       <c r="A179" s="18" t="s">
         <v>530</v>
       </c>
@@ -6327,7 +6372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A180" s="18" t="s">
         <v>532</v>
       </c>
@@ -6356,7 +6401,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A181" s="18" t="s">
         <v>535</v>
       </c>
@@ -6388,7 +6433,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A182" s="18" t="s">
         <v>539</v>
       </c>
@@ -6420,7 +6465,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A183" s="18" t="s">
         <v>542</v>
       </c>
@@ -6452,7 +6497,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A184" s="18" t="s">
         <v>545</v>
       </c>
@@ -6484,7 +6529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A185" s="18" t="s">
         <v>548</v>
       </c>
@@ -6516,7 +6561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A186" s="18" t="s">
         <v>551</v>
       </c>
@@ -6548,7 +6593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A187" s="18" t="s">
         <v>554</v>
       </c>
@@ -6580,7 +6625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A188" s="18" t="s">
         <v>557</v>
       </c>
@@ -6612,7 +6657,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A189" s="18" t="s">
         <v>560</v>
       </c>
@@ -6644,7 +6689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A190" s="18" t="s">
         <v>563</v>
       </c>
@@ -6676,7 +6721,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A191" s="18" t="s">
         <v>566</v>
       </c>
@@ -6705,7 +6750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A192" s="18" t="s">
         <v>569</v>
       </c>
@@ -6734,7 +6779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A193" s="18" t="s">
         <v>572</v>
       </c>
@@ -6763,7 +6808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A194" s="18" t="s">
         <v>575</v>
       </c>
@@ -6792,7 +6837,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A195" s="18" t="s">
         <v>578</v>
       </c>
@@ -6809,7 +6854,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A196" s="18" t="s">
         <v>581</v>
       </c>
@@ -6838,7 +6883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A197" s="18" t="s">
         <v>583</v>
       </c>
@@ -6855,7 +6900,7 @@
       <c r="P197" s="18"/>
       <c r="Q197" s="18"/>
     </row>
-    <row r="198" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A198" s="18" t="s">
         <v>586</v>
       </c>
@@ -6872,7 +6917,7 @@
       <c r="P198" s="18"/>
       <c r="Q198" s="18"/>
     </row>
-    <row r="199" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A199" s="18" t="s">
         <v>589</v>
       </c>
@@ -6901,7 +6946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A200" s="18" t="s">
         <v>591</v>
       </c>
@@ -6918,7 +6963,7 @@
       <c r="P200" s="18"/>
       <c r="Q200" s="18"/>
     </row>
-    <row r="201" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A201" s="18" t="s">
         <v>594</v>
       </c>
@@ -6947,7 +6992,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A202" s="18" t="s">
         <v>597</v>
       </c>
@@ -6976,7 +7021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A203" s="18" t="s">
         <v>599</v>
       </c>
@@ -6993,7 +7038,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A204" s="18" t="s">
         <v>602</v>
       </c>
@@ -7009,7 +7054,7 @@
       </c>
       <c r="Q204" s="18"/>
     </row>
-    <row r="205" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A205" s="18" t="s">
         <v>605</v>
       </c>
@@ -7025,7 +7070,7 @@
       </c>
       <c r="Q205" s="18"/>
     </row>
-    <row r="206" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A206" s="18" t="s">
         <v>608</v>
       </c>
@@ -7041,7 +7086,7 @@
       </c>
       <c r="Q206" s="18"/>
     </row>
-    <row r="207" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:17" ht="40" x14ac:dyDescent="0.25">
       <c r="A207" s="18" t="s">
         <v>611</v>
       </c>
@@ -7070,7 +7115,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A208" s="18" t="s">
         <v>614</v>
       </c>
@@ -7099,7 +7144,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A209" s="18" t="s">
         <v>617</v>
       </c>
@@ -7128,7 +7173,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="37" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A210" s="18" t="s">
         <v>620</v>
       </c>
@@ -7157,7 +7202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A211" s="18" t="s">
         <v>623</v>
       </c>
@@ -7186,7 +7231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>626</v>
       </c>
@@ -7203,7 +7248,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>631</v>
       </c>
@@ -7232,7 +7277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>634</v>
       </c>
@@ -7252,7 +7297,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>638</v>
       </c>
@@ -7269,7 +7314,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>642</v>
       </c>
@@ -7289,7 +7334,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>646</v>
       </c>
@@ -7309,7 +7354,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>651</v>
       </c>
@@ -7329,7 +7374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>655</v>
       </c>
@@ -7346,7 +7391,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>658</v>
       </c>
@@ -7364,7 +7409,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>661</v>
       </c>
@@ -7382,7 +7427,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>664</v>
       </c>
@@ -7400,7 +7445,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>667</v>
       </c>
@@ -7434,7 +7479,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Validated tests/ reqs  for other groups
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardankarki/Desktop/cse3310-sp25-004/FinalRequirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C466EA3-9A60-E744-A48A-C83CAAAE85E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{6C466EA3-9A60-E744-A48A-C83CAAAE85E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6D9E89A-9451-4A3E-A0F4-4C47BD26C340}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="681">
   <si>
     <t>Tested By</t>
   </si>
@@ -2082,12 +2082,6 @@
   </si>
   <si>
     <t>ut</t>
-  </si>
-  <si>
-    <t>Test 2, Step 4</t>
-  </si>
-  <si>
-    <t>Test 10, Step 3</t>
   </si>
 </sst>
 </file>
@@ -2530,38 +2524,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E104" zoomScale="93" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K130" sqref="K130"/>
+    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="93" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="36.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="123.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="1"/>
-    <col min="11" max="11" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1"/>
-    <col min="13" max="13" width="12.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" style="1"/>
-    <col min="20" max="20" width="36.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="123.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.7109375" style="1"/>
+    <col min="11" max="11" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" style="1"/>
+    <col min="20" max="20" width="36.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2599,7 +2593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2622,7 +2616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2645,7 +2639,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2653,27 +2647,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2705,7 +2699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -2737,7 +2731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -2769,7 +2763,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>36</v>
       </c>
@@ -2801,7 +2795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -2817,11 +2811,14 @@
       <c r="K14" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q14" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>42</v>
       </c>
@@ -2838,9 +2835,12 @@
       <c r="K15" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N15" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>59</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>64</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -3161,11 +3161,14 @@
       <c r="K28" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N28" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q28" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -3182,11 +3185,14 @@
       <c r="K29" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N29" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q29" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>88</v>
       </c>
@@ -3214,7 +3220,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
@@ -3233,11 +3239,14 @@
       <c r="K31" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N31" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q31" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
@@ -3256,8 +3265,11 @@
       <c r="K32" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="N32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>97</v>
       </c>
@@ -3274,10 +3286,10 @@
         <v>671</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
@@ -3294,10 +3306,10 @@
         <v>671</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>104</v>
       </c>
@@ -3329,7 +3341,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>107</v>
       </c>
@@ -3361,7 +3373,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>110</v>
       </c>
@@ -3393,7 +3405,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3425,7 +3437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -3457,7 +3469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>118</v>
       </c>
@@ -3489,7 +3501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -3521,7 +3533,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -3538,10 +3550,10 @@
         <v>671</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -3573,7 +3585,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -3605,7 +3617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -3622,7 +3634,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>137</v>
       </c>
@@ -3642,7 +3654,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>141</v>
       </c>
@@ -3659,7 +3671,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>144</v>
       </c>
@@ -3676,7 +3688,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -3693,7 +3705,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>150</v>
       </c>
@@ -3725,7 +3737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>153</v>
       </c>
@@ -3742,7 +3754,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>156</v>
       </c>
@@ -3759,7 +3771,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>158</v>
       </c>
@@ -3776,7 +3788,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>160</v>
       </c>
@@ -3793,7 +3805,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>162</v>
       </c>
@@ -3810,7 +3822,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>164</v>
       </c>
@@ -3842,7 +3854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>166</v>
       </c>
@@ -3877,7 +3889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>171</v>
       </c>
@@ -3909,7 +3921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>175</v>
       </c>
@@ -3941,7 +3953,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>179</v>
       </c>
@@ -3964,7 +3976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>183</v>
       </c>
@@ -3996,7 +4008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>187</v>
       </c>
@@ -4012,11 +4024,14 @@
       <c r="K62" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N62" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q62" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>191</v>
       </c>
@@ -4048,7 +4063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>195</v>
       </c>
@@ -4080,7 +4095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>199</v>
       </c>
@@ -4096,11 +4111,14 @@
       <c r="K65" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N65" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q65" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>203</v>
       </c>
@@ -4116,8 +4134,11 @@
       <c r="K66" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="N66" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>206</v>
       </c>
@@ -4149,7 +4170,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>209</v>
       </c>
@@ -4165,11 +4186,14 @@
       <c r="K68" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N68" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q68" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>212</v>
       </c>
@@ -4185,11 +4209,14 @@
       <c r="K69" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N69" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q69" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>215</v>
       </c>
@@ -4205,8 +4232,11 @@
       <c r="K70" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="N70" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>218</v>
       </c>
@@ -4229,7 +4259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>221</v>
       </c>
@@ -4245,11 +4275,14 @@
       <c r="K72" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N72" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q72" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>224</v>
       </c>
@@ -4281,7 +4314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>228</v>
       </c>
@@ -4297,8 +4330,11 @@
       <c r="K74" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="N74" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>232</v>
       </c>
@@ -4330,7 +4366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>236</v>
       </c>
@@ -4353,7 +4389,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>239</v>
       </c>
@@ -4369,8 +4405,11 @@
       <c r="K77" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="N77" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>242</v>
       </c>
@@ -4386,11 +4425,14 @@
       <c r="K78" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N78" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q78" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>245</v>
       </c>
@@ -4413,7 +4455,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>249</v>
       </c>
@@ -4445,7 +4487,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>252</v>
       </c>
@@ -4461,11 +4503,14 @@
       <c r="K81" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N81" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q81" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>255</v>
       </c>
@@ -4481,11 +4526,14 @@
       <c r="K82" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N82" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q82" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>258</v>
       </c>
@@ -4501,11 +4549,14 @@
       <c r="K83" s="1" t="s">
         <v>671</v>
       </c>
+      <c r="N83" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q83" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>261</v>
       </c>
@@ -4528,7 +4579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>264</v>
       </c>
@@ -4551,7 +4602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>267</v>
       </c>
@@ -4574,7 +4625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>270</v>
       </c>
@@ -4597,7 +4648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>273</v>
       </c>
@@ -4629,7 +4680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>276</v>
       </c>
@@ -4652,7 +4703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>279</v>
       </c>
@@ -4675,7 +4726,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>282</v>
       </c>
@@ -4691,11 +4742,14 @@
       <c r="K91" s="1" t="s">
         <v>672</v>
       </c>
+      <c r="N91" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q91" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>287</v>
       </c>
@@ -4711,11 +4765,14 @@
       <c r="K92" s="1" t="s">
         <v>672</v>
       </c>
+      <c r="N92" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q92" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>289</v>
       </c>
@@ -4731,11 +4788,14 @@
       <c r="K93" s="1" t="s">
         <v>673</v>
       </c>
+      <c r="N93" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q93" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>293</v>
       </c>
@@ -4751,11 +4811,14 @@
       <c r="K94" s="1" t="s">
         <v>673</v>
       </c>
+      <c r="N94" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q94" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
@@ -4771,11 +4834,14 @@
       <c r="K95" s="1" t="s">
         <v>674</v>
       </c>
+      <c r="N95" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q95" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -4791,11 +4857,14 @@
       <c r="K96" s="1" t="s">
         <v>672</v>
       </c>
+      <c r="N96" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q96" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>302</v>
       </c>
@@ -4812,7 +4881,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>305</v>
       </c>
@@ -4829,7 +4898,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>308</v>
       </c>
@@ -4845,8 +4914,11 @@
       <c r="K99" s="1" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="100" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="N99" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -4878,7 +4950,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>314</v>
       </c>
@@ -4898,7 +4970,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>316</v>
       </c>
@@ -4918,7 +4990,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>318</v>
       </c>
@@ -4938,7 +5010,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>321</v>
       </c>
@@ -4958,7 +5030,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>324</v>
       </c>
@@ -4978,7 +5050,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>327</v>
       </c>
@@ -4998,7 +5070,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>329</v>
       </c>
@@ -5017,7 +5089,7 @@
       </c>
       <c r="Q107" s="5"/>
     </row>
-    <row r="108" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>333</v>
       </c>
@@ -5036,7 +5108,7 @@
       </c>
       <c r="Q108" s="5"/>
     </row>
-    <row r="109" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>335</v>
       </c>
@@ -5055,7 +5127,7 @@
       </c>
       <c r="Q109" s="5"/>
     </row>
-    <row r="110" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>338</v>
       </c>
@@ -5071,7 +5143,7 @@
       </c>
       <c r="Q110" s="5"/>
     </row>
-    <row r="111" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>340</v>
       </c>
@@ -5087,7 +5159,7 @@
       </c>
       <c r="Q111" s="5"/>
     </row>
-    <row r="112" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>342</v>
       </c>
@@ -5103,7 +5175,7 @@
       </c>
       <c r="Q112" s="5"/>
     </row>
-    <row r="113" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>344</v>
       </c>
@@ -5119,7 +5191,7 @@
       </c>
       <c r="Q113" s="5"/>
     </row>
-    <row r="114" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>347</v>
       </c>
@@ -5135,7 +5207,7 @@
       </c>
       <c r="Q114" s="5"/>
     </row>
-    <row r="115" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>349</v>
       </c>
@@ -5151,7 +5223,7 @@
       </c>
       <c r="Q115" s="5"/>
     </row>
-    <row r="116" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>351</v>
       </c>
@@ -5167,7 +5239,7 @@
       </c>
       <c r="Q116" s="5"/>
     </row>
-    <row r="117" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>354</v>
       </c>
@@ -5183,7 +5255,7 @@
       </c>
       <c r="Q117" s="5"/>
     </row>
-    <row r="118" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>356</v>
       </c>
@@ -5199,7 +5271,7 @@
       </c>
       <c r="Q118" s="5"/>
     </row>
-    <row r="119" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>358</v>
       </c>
@@ -5215,7 +5287,7 @@
       </c>
       <c r="Q119" s="5"/>
     </row>
-    <row r="120" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>360</v>
       </c>
@@ -5231,7 +5303,7 @@
       </c>
       <c r="Q120" s="5"/>
     </row>
-    <row r="121" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>362</v>
       </c>
@@ -5247,7 +5319,7 @@
       </c>
       <c r="Q121" s="5"/>
     </row>
-    <row r="122" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>365</v>
       </c>
@@ -5263,7 +5335,7 @@
       </c>
       <c r="Q122" s="5"/>
     </row>
-    <row r="123" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>367</v>
       </c>
@@ -5279,7 +5351,7 @@
       </c>
       <c r="Q123" s="5"/>
     </row>
-    <row r="124" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>369</v>
       </c>
@@ -5295,7 +5367,7 @@
       </c>
       <c r="Q124" s="5"/>
     </row>
-    <row r="125" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>371</v>
       </c>
@@ -5311,7 +5383,7 @@
       </c>
       <c r="Q125" s="5"/>
     </row>
-    <row r="126" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>373</v>
       </c>
@@ -5327,7 +5399,7 @@
       </c>
       <c r="Q126" s="5"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>375</v>
       </c>
@@ -5346,7 +5418,7 @@
       </c>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>379</v>
       </c>
@@ -5378,7 +5450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>382</v>
       </c>
@@ -5397,7 +5469,7 @@
       </c>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="s">
         <v>385</v>
       </c>
@@ -5416,7 +5488,7 @@
       </c>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>387</v>
       </c>
@@ -5435,7 +5507,7 @@
       </c>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>390</v>
       </c>
@@ -5454,7 +5526,7 @@
       </c>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>393</v>
       </c>
@@ -5473,7 +5545,7 @@
       </c>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>396</v>
       </c>
@@ -5492,7 +5564,7 @@
       </c>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>399</v>
       </c>
@@ -5511,7 +5583,7 @@
       </c>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>402</v>
       </c>
@@ -5530,7 +5602,7 @@
       </c>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>405</v>
       </c>
@@ -5549,7 +5621,7 @@
       </c>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>408</v>
       </c>
@@ -5568,7 +5640,7 @@
       </c>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>411</v>
       </c>
@@ -5587,7 +5659,7 @@
       </c>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" s="10" t="s">
         <v>415</v>
       </c>
@@ -5606,7 +5678,7 @@
       </c>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="16" t="s">
         <v>418</v>
       </c>
@@ -5625,7 +5697,7 @@
       </c>
       <c r="Q141" s="16"/>
     </row>
-    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="17" t="s">
         <v>421</v>
       </c>
@@ -5645,7 +5717,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="17" t="s">
         <v>426</v>
       </c>
@@ -5663,7 +5735,7 @@
       </c>
       <c r="Q143" s="17"/>
     </row>
-    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="17" t="s">
         <v>429</v>
       </c>
@@ -5683,7 +5755,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="17" t="s">
         <v>432</v>
       </c>
@@ -5703,7 +5775,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="17" t="s">
         <v>435</v>
       </c>
@@ -5722,7 +5794,7 @@
       </c>
       <c r="Q146" s="17"/>
     </row>
-    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="17" t="s">
         <v>438</v>
       </c>
@@ -5741,7 +5813,7 @@
       </c>
       <c r="Q147" s="17"/>
     </row>
-    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="17" t="s">
         <v>441</v>
       </c>
@@ -5760,7 +5832,7 @@
       </c>
       <c r="Q148" s="17"/>
     </row>
-    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="17" t="s">
         <v>444</v>
       </c>
@@ -5779,7 +5851,7 @@
       </c>
       <c r="Q149" s="17"/>
     </row>
-    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="17" t="s">
         <v>447</v>
       </c>
@@ -5798,7 +5870,7 @@
       </c>
       <c r="Q150" s="17"/>
     </row>
-    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="17" t="s">
         <v>450</v>
       </c>
@@ -5817,7 +5889,7 @@
       </c>
       <c r="Q151" s="17"/>
     </row>
-    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="17" t="s">
         <v>453</v>
       </c>
@@ -5836,7 +5908,7 @@
       </c>
       <c r="Q152" s="17"/>
     </row>
-    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="17" t="s">
         <v>456</v>
       </c>
@@ -5855,7 +5927,7 @@
       </c>
       <c r="Q153" s="17"/>
     </row>
-    <row r="154" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>458</v>
       </c>
@@ -5872,7 +5944,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>462</v>
       </c>
@@ -5904,7 +5976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>465</v>
       </c>
@@ -5921,7 +5993,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>468</v>
       </c>
@@ -5938,7 +6010,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>471</v>
       </c>
@@ -5955,7 +6027,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>474</v>
       </c>
@@ -5972,7 +6044,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>476</v>
       </c>
@@ -5989,7 +6061,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>479</v>
       </c>
@@ -6006,7 +6078,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>482</v>
       </c>
@@ -6023,7 +6095,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>484</v>
       </c>
@@ -6040,7 +6112,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>486</v>
       </c>
@@ -6057,7 +6129,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>489</v>
       </c>
@@ -6074,7 +6146,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>492</v>
       </c>
@@ -6091,7 +6163,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>495</v>
       </c>
@@ -6108,7 +6180,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>498</v>
       </c>
@@ -6125,7 +6197,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>501</v>
       </c>
@@ -6142,7 +6214,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>504</v>
       </c>
@@ -6159,7 +6231,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>507</v>
       </c>
@@ -6176,7 +6248,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>509</v>
       </c>
@@ -6193,7 +6265,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>511</v>
       </c>
@@ -6210,7 +6282,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>514</v>
       </c>
@@ -6227,7 +6299,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A175" s="18" t="s">
         <v>517</v>
       </c>
@@ -6256,7 +6328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A176" s="18" t="s">
         <v>521</v>
       </c>
@@ -6285,7 +6357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A177" s="18" t="s">
         <v>524</v>
       </c>
@@ -6314,7 +6386,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="80" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" ht="75" x14ac:dyDescent="0.3">
       <c r="A178" s="18" t="s">
         <v>527</v>
       </c>
@@ -6343,7 +6415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="80" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" ht="75" x14ac:dyDescent="0.3">
       <c r="A179" s="18" t="s">
         <v>530</v>
       </c>
@@ -6372,7 +6444,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A180" s="18" t="s">
         <v>532</v>
       </c>
@@ -6401,7 +6473,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="18" t="s">
         <v>535</v>
       </c>
@@ -6433,7 +6505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="18" t="s">
         <v>539</v>
       </c>
@@ -6465,7 +6537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="18" t="s">
         <v>542</v>
       </c>
@@ -6497,7 +6569,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="18" t="s">
         <v>545</v>
       </c>
@@ -6529,7 +6601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="18" t="s">
         <v>548</v>
       </c>
@@ -6561,7 +6633,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A186" s="18" t="s">
         <v>551</v>
       </c>
@@ -6593,7 +6665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A187" s="18" t="s">
         <v>554</v>
       </c>
@@ -6625,7 +6697,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A188" s="18" t="s">
         <v>557</v>
       </c>
@@ -6657,7 +6729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A189" s="18" t="s">
         <v>560</v>
       </c>
@@ -6689,7 +6761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="18" t="s">
         <v>563</v>
       </c>
@@ -6721,7 +6793,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A191" s="18" t="s">
         <v>566</v>
       </c>
@@ -6750,7 +6822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="18" t="s">
         <v>569</v>
       </c>
@@ -6779,7 +6851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A193" s="18" t="s">
         <v>572</v>
       </c>
@@ -6808,7 +6880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A194" s="18" t="s">
         <v>575</v>
       </c>
@@ -6837,7 +6909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="18" t="s">
         <v>578</v>
       </c>
@@ -6854,7 +6926,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A196" s="18" t="s">
         <v>581</v>
       </c>
@@ -6883,7 +6955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="18" t="s">
         <v>583</v>
       </c>
@@ -6900,7 +6972,7 @@
       <c r="P197" s="18"/>
       <c r="Q197" s="18"/>
     </row>
-    <row r="198" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="18" t="s">
         <v>586</v>
       </c>
@@ -6917,7 +6989,7 @@
       <c r="P198" s="18"/>
       <c r="Q198" s="18"/>
     </row>
-    <row r="199" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="18" t="s">
         <v>589</v>
       </c>
@@ -6946,7 +7018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A200" s="18" t="s">
         <v>591</v>
       </c>
@@ -6963,7 +7035,7 @@
       <c r="P200" s="18"/>
       <c r="Q200" s="18"/>
     </row>
-    <row r="201" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="18" t="s">
         <v>594</v>
       </c>
@@ -6992,7 +7064,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A202" s="18" t="s">
         <v>597</v>
       </c>
@@ -7021,7 +7093,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="18" t="s">
         <v>599</v>
       </c>
@@ -7038,7 +7110,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A204" s="18" t="s">
         <v>602</v>
       </c>
@@ -7054,7 +7126,7 @@
       </c>
       <c r="Q204" s="18"/>
     </row>
-    <row r="205" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="18" t="s">
         <v>605</v>
       </c>
@@ -7070,7 +7142,7 @@
       </c>
       <c r="Q205" s="18"/>
     </row>
-    <row r="206" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="18" t="s">
         <v>608</v>
       </c>
@@ -7086,7 +7158,7 @@
       </c>
       <c r="Q206" s="18"/>
     </row>
-    <row r="207" spans="1:17" ht="40" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A207" s="18" t="s">
         <v>611</v>
       </c>
@@ -7115,7 +7187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="18" t="s">
         <v>614</v>
       </c>
@@ -7144,7 +7216,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" ht="75" x14ac:dyDescent="0.3">
       <c r="A209" s="18" t="s">
         <v>617</v>
       </c>
@@ -7173,7 +7245,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A210" s="18" t="s">
         <v>620</v>
       </c>
@@ -7202,7 +7274,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="18" t="s">
         <v>623</v>
       </c>
@@ -7231,7 +7303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>626</v>
       </c>
@@ -7248,7 +7320,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>631</v>
       </c>
@@ -7277,7 +7349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>634</v>
       </c>
@@ -7297,7 +7369,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>638</v>
       </c>
@@ -7314,7 +7386,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>642</v>
       </c>
@@ -7334,7 +7406,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>646</v>
       </c>
@@ -7354,7 +7426,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>651</v>
       </c>
@@ -7374,7 +7446,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>655</v>
       </c>
@@ -7391,7 +7463,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>658</v>
       </c>
@@ -7409,7 +7481,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>661</v>
       </c>
@@ -7427,7 +7499,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>664</v>
       </c>
@@ -7445,7 +7517,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>667</v>
       </c>
@@ -7479,7 +7551,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Test # and Step for GM reqs
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SyncthingServiceAcct\school work\2025\Spring 2025\CSE 3310 FUNDAMENTALS OF SOFTWARE ENGR\cse3310-sp25-004\FinalRequirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbf526d0a72a0725/Desktop/'24-'25 Year/CSE 3310/Project/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4E43DB-E412-410B-B4E6-CC68BA241112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6F4E43DB-E412-410B-B4E6-CC68BA241112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FAB1986-B0DB-45B9-AA8A-1A744E4CA99B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="695">
   <si>
     <t>Tested By</t>
   </si>
@@ -2116,6 +2116,12 @@
   </si>
   <si>
     <t>Step 15, fail</t>
+  </si>
+  <si>
+    <t>Test 2, Step 4</t>
+  </si>
+  <si>
+    <t>Test 3, Step 4</t>
   </si>
 </sst>
 </file>
@@ -2558,33 +2564,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="E24" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="36.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="123.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="65.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.6640625" style="1"/>
-    <col min="11" max="11" width="11.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1"/>
-    <col min="13" max="13" width="12.77734375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.77734375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="9.44140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" style="3" customWidth="1"/>
-    <col min="19" max="19" width="8.6640625" style="1"/>
-    <col min="20" max="20" width="36.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.5703125" style="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="123.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="65.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.5703125" style="1"/>
+    <col min="11" max="11" width="11.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" style="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" style="1"/>
+    <col min="20" max="20" width="36.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2630,7 +2636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2653,7 +2659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -2676,7 +2682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2684,27 +2690,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2736,7 +2742,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
@@ -2768,7 +2774,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
@@ -2800,7 +2806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
@@ -2832,7 +2838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>39</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
@@ -2883,7 +2889,7 @@
       </c>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
@@ -2905,7 +2911,7 @@
       </c>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>50</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>54</v>
       </c>
@@ -2944,7 +2950,7 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>57</v>
       </c>
@@ -2963,7 +2969,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
@@ -2982,7 +2988,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>63</v>
       </c>
@@ -3014,7 +3020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>66</v>
       </c>
@@ -3033,7 +3039,7 @@
       </c>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>68</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>71</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
@@ -3155,7 +3161,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>84</v>
       </c>
@@ -3217,7 +3223,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>88</v>
       </c>
@@ -3244,7 +3250,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>91</v>
       </c>
@@ -3275,7 +3281,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -3304,7 +3310,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
@@ -3330,7 +3336,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>100</v>
       </c>
@@ -3347,13 +3353,13 @@
         <v>42</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>104</v>
       </c>
@@ -3370,13 +3376,13 @@
         <v>42</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>43</v>
+        <v>693</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>107</v>
       </c>
@@ -3408,7 +3414,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>111</v>
       </c>
@@ -3440,7 +3446,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>114</v>
       </c>
@@ -3472,7 +3478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>117</v>
       </c>
@@ -3504,7 +3510,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>119</v>
       </c>
@@ -3536,7 +3542,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>122</v>
       </c>
@@ -3568,7 +3574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>125</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>128</v>
       </c>
@@ -3617,13 +3623,13 @@
         <v>42</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>43</v>
+        <v>694</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>131</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>134</v>
       </c>
@@ -3687,7 +3693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>137</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>141</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>145</v>
       </c>
@@ -3744,7 +3750,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>148</v>
       </c>
@@ -3764,7 +3770,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>151</v>
       </c>
@@ -3784,7 +3790,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>154</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>157</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>160</v>
       </c>
@@ -3853,7 +3859,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>162</v>
       </c>
@@ -3870,7 +3876,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>164</v>
       </c>
@@ -3890,7 +3896,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>166</v>
       </c>
@@ -3910,7 +3916,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>168</v>
       </c>
@@ -3942,7 +3948,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>170</v>
       </c>
@@ -3977,7 +3983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>175</v>
       </c>
@@ -4009,7 +4015,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>179</v>
       </c>
@@ -4041,7 +4047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>183</v>
       </c>
@@ -4064,7 +4070,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>187</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>191</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>195</v>
       </c>
@@ -4154,7 +4160,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>199</v>
       </c>
@@ -4186,7 +4192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>203</v>
       </c>
@@ -4212,7 +4218,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>207</v>
       </c>
@@ -4235,7 +4241,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>210</v>
       </c>
@@ -4267,7 +4273,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>213</v>
       </c>
@@ -4293,7 +4299,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>216</v>
       </c>
@@ -4319,7 +4325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>219</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>222</v>
       </c>
@@ -4368,7 +4374,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>225</v>
       </c>
@@ -4394,7 +4400,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>228</v>
       </c>
@@ -4426,7 +4432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>232</v>
       </c>
@@ -4446,7 +4452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>236</v>
       </c>
@@ -4478,7 +4484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>240</v>
       </c>
@@ -4501,7 +4507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>243</v>
       </c>
@@ -4521,7 +4527,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>246</v>
       </c>
@@ -4544,7 +4550,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>249</v>
       </c>
@@ -4567,7 +4573,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>253</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>256</v>
       </c>
@@ -4622,7 +4628,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>259</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>262</v>
       </c>
@@ -4668,7 +4674,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>265</v>
       </c>
@@ -4691,7 +4697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>268</v>
       </c>
@@ -4714,7 +4720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>271</v>
       </c>
@@ -4737,7 +4743,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>274</v>
       </c>
@@ -4760,7 +4766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>277</v>
       </c>
@@ -4792,7 +4798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>280</v>
       </c>
@@ -4815,7 +4821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>283</v>
       </c>
@@ -4838,7 +4844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>286</v>
       </c>
@@ -4861,7 +4867,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>292</v>
       </c>
@@ -4884,7 +4890,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>294</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>299</v>
       </c>
@@ -4930,7 +4936,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>302</v>
       </c>
@@ -4953,7 +4959,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>306</v>
       </c>
@@ -4976,7 +4982,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>309</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>312</v>
       </c>
@@ -5010,7 +5016,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>316</v>
       </c>
@@ -5030,7 +5036,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>320</v>
       </c>
@@ -5062,7 +5068,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>324</v>
       </c>
@@ -5082,7 +5088,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>326</v>
       </c>
@@ -5102,7 +5108,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>328</v>
       </c>
@@ -5122,7 +5128,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>331</v>
       </c>
@@ -5142,7 +5148,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>334</v>
       </c>
@@ -5162,7 +5168,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>337</v>
       </c>
@@ -5182,7 +5188,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>340</v>
       </c>
@@ -5201,7 +5207,7 @@
       </c>
       <c r="Q107" s="5"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>344</v>
       </c>
@@ -5220,7 +5226,7 @@
       </c>
       <c r="Q108" s="5"/>
     </row>
-    <row r="109" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>346</v>
       </c>
@@ -5239,7 +5245,7 @@
       </c>
       <c r="Q109" s="5"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>349</v>
       </c>
@@ -5255,7 +5261,7 @@
       </c>
       <c r="Q110" s="5"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>351</v>
       </c>
@@ -5271,7 +5277,7 @@
       </c>
       <c r="Q111" s="5"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>353</v>
       </c>
@@ -5287,7 +5293,7 @@
       </c>
       <c r="Q112" s="5"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>355</v>
       </c>
@@ -5303,7 +5309,7 @@
       </c>
       <c r="Q113" s="5"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>358</v>
       </c>
@@ -5319,7 +5325,7 @@
       </c>
       <c r="Q114" s="5"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>360</v>
       </c>
@@ -5335,7 +5341,7 @@
       </c>
       <c r="Q115" s="5"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>362</v>
       </c>
@@ -5351,7 +5357,7 @@
       </c>
       <c r="Q116" s="5"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>365</v>
       </c>
@@ -5367,7 +5373,7 @@
       </c>
       <c r="Q117" s="5"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>367</v>
       </c>
@@ -5383,7 +5389,7 @@
       </c>
       <c r="Q118" s="5"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>369</v>
       </c>
@@ -5399,7 +5405,7 @@
       </c>
       <c r="Q119" s="5"/>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>371</v>
       </c>
@@ -5415,7 +5421,7 @@
       </c>
       <c r="Q120" s="5"/>
     </row>
-    <row r="121" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>373</v>
       </c>
@@ -5431,7 +5437,7 @@
       </c>
       <c r="Q121" s="5"/>
     </row>
-    <row r="122" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>376</v>
       </c>
@@ -5447,7 +5453,7 @@
       </c>
       <c r="Q122" s="5"/>
     </row>
-    <row r="123" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>378</v>
       </c>
@@ -5463,7 +5469,7 @@
       </c>
       <c r="Q123" s="5"/>
     </row>
-    <row r="124" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>380</v>
       </c>
@@ -5479,7 +5485,7 @@
       </c>
       <c r="Q124" s="5"/>
     </row>
-    <row r="125" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>382</v>
       </c>
@@ -5495,7 +5501,7 @@
       </c>
       <c r="Q125" s="5"/>
     </row>
-    <row r="126" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>384</v>
       </c>
@@ -5511,7 +5517,7 @@
       </c>
       <c r="Q126" s="5"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>386</v>
       </c>
@@ -5530,7 +5536,7 @@
       </c>
       <c r="Q127" s="10"/>
     </row>
-    <row r="128" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>391</v>
       </c>
@@ -5562,7 +5568,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="129" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>394</v>
       </c>
@@ -5581,7 +5587,7 @@
       </c>
       <c r="Q129" s="10"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="s">
         <v>397</v>
       </c>
@@ -5600,7 +5606,7 @@
       </c>
       <c r="Q130" s="10"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>399</v>
       </c>
@@ -5619,7 +5625,7 @@
       </c>
       <c r="Q131" s="10"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>402</v>
       </c>
@@ -5638,7 +5644,7 @@
       </c>
       <c r="Q132" s="10"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>405</v>
       </c>
@@ -5657,7 +5663,7 @@
       </c>
       <c r="Q133" s="10"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>408</v>
       </c>
@@ -5676,7 +5682,7 @@
       </c>
       <c r="Q134" s="10"/>
     </row>
-    <row r="135" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>411</v>
       </c>
@@ -5695,7 +5701,7 @@
       </c>
       <c r="Q135" s="10"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>414</v>
       </c>
@@ -5714,7 +5720,7 @@
       </c>
       <c r="Q136" s="10"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>417</v>
       </c>
@@ -5733,7 +5739,7 @@
       </c>
       <c r="Q137" s="10"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>420</v>
       </c>
@@ -5752,7 +5758,7 @@
       </c>
       <c r="Q138" s="10"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>423</v>
       </c>
@@ -5771,7 +5777,7 @@
       </c>
       <c r="Q139" s="10"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" s="10" t="s">
         <v>427</v>
       </c>
@@ -5790,7 +5796,7 @@
       </c>
       <c r="Q140" s="10"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="16" t="s">
         <v>430</v>
       </c>
@@ -5809,7 +5815,7 @@
       </c>
       <c r="Q141" s="16"/>
     </row>
-    <row r="142" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="17" t="s">
         <v>433</v>
       </c>
@@ -5829,7 +5835,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A143" s="17" t="s">
         <v>438</v>
       </c>
@@ -5847,7 +5853,7 @@
       </c>
       <c r="Q143" s="17"/>
     </row>
-    <row r="144" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A144" s="17" t="s">
         <v>441</v>
       </c>
@@ -5867,7 +5873,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="17" t="s">
         <v>444</v>
       </c>
@@ -5887,7 +5893,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="17" t="s">
         <v>447</v>
       </c>
@@ -5906,7 +5912,7 @@
       </c>
       <c r="Q146" s="17"/>
     </row>
-    <row r="147" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A147" s="17" t="s">
         <v>450</v>
       </c>
@@ -5925,7 +5931,7 @@
       </c>
       <c r="Q147" s="17"/>
     </row>
-    <row r="148" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A148" s="17" t="s">
         <v>453</v>
       </c>
@@ -5944,7 +5950,7 @@
       </c>
       <c r="Q148" s="17"/>
     </row>
-    <row r="149" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A149" s="17" t="s">
         <v>456</v>
       </c>
@@ -5963,7 +5969,7 @@
       </c>
       <c r="Q149" s="17"/>
     </row>
-    <row r="150" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="17" t="s">
         <v>459</v>
       </c>
@@ -5982,7 +5988,7 @@
       </c>
       <c r="Q150" s="17"/>
     </row>
-    <row r="151" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A151" s="17" t="s">
         <v>462</v>
       </c>
@@ -6001,7 +6007,7 @@
       </c>
       <c r="Q151" s="17"/>
     </row>
-    <row r="152" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="17" t="s">
         <v>465</v>
       </c>
@@ -6020,7 +6026,7 @@
       </c>
       <c r="Q152" s="17"/>
     </row>
-    <row r="153" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A153" s="17" t="s">
         <v>468</v>
       </c>
@@ -6039,7 +6045,7 @@
       </c>
       <c r="Q153" s="17"/>
     </row>
-    <row r="154" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>470</v>
       </c>
@@ -6056,7 +6062,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>474</v>
       </c>
@@ -6088,7 +6094,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>477</v>
       </c>
@@ -6105,7 +6111,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>480</v>
       </c>
@@ -6122,7 +6128,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>483</v>
       </c>
@@ -6139,7 +6145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>486</v>
       </c>
@@ -6156,7 +6162,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>488</v>
       </c>
@@ -6173,7 +6179,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>491</v>
       </c>
@@ -6190,7 +6196,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>494</v>
       </c>
@@ -6207,7 +6213,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>496</v>
       </c>
@@ -6224,7 +6230,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>498</v>
       </c>
@@ -6241,7 +6247,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>501</v>
       </c>
@@ -6258,7 +6264,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>504</v>
       </c>
@@ -6275,7 +6281,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>507</v>
       </c>
@@ -6292,7 +6298,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>510</v>
       </c>
@@ -6309,7 +6315,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>513</v>
       </c>
@@ -6326,7 +6332,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>516</v>
       </c>
@@ -6343,7 +6349,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>519</v>
       </c>
@@ -6360,7 +6366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>521</v>
       </c>
@@ -6377,7 +6383,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>523</v>
       </c>
@@ -6394,7 +6400,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>526</v>
       </c>
@@ -6411,7 +6417,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A175" s="18" t="s">
         <v>529</v>
       </c>
@@ -6440,7 +6446,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A176" s="18" t="s">
         <v>533</v>
       </c>
@@ -6469,7 +6475,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A177" s="18" t="s">
         <v>536</v>
       </c>
@@ -6498,7 +6504,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="178" spans="1:17" ht="72" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" ht="75" x14ac:dyDescent="0.3">
       <c r="A178" s="18" t="s">
         <v>539</v>
       </c>
@@ -6527,7 +6533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="72" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="75" x14ac:dyDescent="0.3">
       <c r="A179" s="18" t="s">
         <v>542</v>
       </c>
@@ -6556,7 +6562,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="54" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A180" s="18" t="s">
         <v>544</v>
       </c>
@@ -6585,7 +6591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="181" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="18" t="s">
         <v>547</v>
       </c>
@@ -6617,7 +6623,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="18" t="s">
         <v>550</v>
       </c>
@@ -6649,7 +6655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="18" t="s">
         <v>553</v>
       </c>
@@ -6681,7 +6687,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A184" s="18" t="s">
         <v>556</v>
       </c>
@@ -6713,7 +6719,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A185" s="18" t="s">
         <v>559</v>
       </c>
@@ -6745,7 +6751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A186" s="18" t="s">
         <v>562</v>
       </c>
@@ -6777,7 +6783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A187" s="18" t="s">
         <v>565</v>
       </c>
@@ -6809,7 +6815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="54" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A188" s="18" t="s">
         <v>568</v>
       </c>
@@ -6841,7 +6847,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A189" s="18" t="s">
         <v>571</v>
       </c>
@@ -6873,7 +6879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="18" t="s">
         <v>574</v>
       </c>
@@ -6905,7 +6911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A191" s="18" t="s">
         <v>577</v>
       </c>
@@ -6934,7 +6940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="18" t="s">
         <v>580</v>
       </c>
@@ -6963,7 +6969,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="193" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A193" s="18" t="s">
         <v>583</v>
       </c>
@@ -6992,7 +6998,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="194" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A194" s="18" t="s">
         <v>586</v>
       </c>
@@ -7021,7 +7027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="18" t="s">
         <v>589</v>
       </c>
@@ -7038,7 +7044,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A196" s="18" t="s">
         <v>592</v>
       </c>
@@ -7067,7 +7073,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="197" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A197" s="18" t="s">
         <v>594</v>
       </c>
@@ -7084,7 +7090,7 @@
       <c r="P197" s="18"/>
       <c r="Q197" s="18"/>
     </row>
-    <row r="198" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A198" s="18" t="s">
         <v>597</v>
       </c>
@@ -7101,7 +7107,7 @@
       <c r="P198" s="18"/>
       <c r="Q198" s="18"/>
     </row>
-    <row r="199" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A199" s="18" t="s">
         <v>600</v>
       </c>
@@ -7130,7 +7136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A200" s="18" t="s">
         <v>602</v>
       </c>
@@ -7147,7 +7153,7 @@
       <c r="P200" s="18"/>
       <c r="Q200" s="18"/>
     </row>
-    <row r="201" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A201" s="18" t="s">
         <v>605</v>
       </c>
@@ -7176,7 +7182,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A202" s="18" t="s">
         <v>608</v>
       </c>
@@ -7205,7 +7211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A203" s="18" t="s">
         <v>610</v>
       </c>
@@ -7222,7 +7228,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A204" s="18" t="s">
         <v>613</v>
       </c>
@@ -7238,7 +7244,7 @@
       </c>
       <c r="Q204" s="18"/>
     </row>
-    <row r="205" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A205" s="18" t="s">
         <v>616</v>
       </c>
@@ -7254,7 +7260,7 @@
       </c>
       <c r="Q205" s="18"/>
     </row>
-    <row r="206" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A206" s="18" t="s">
         <v>619</v>
       </c>
@@ -7270,7 +7276,7 @@
       </c>
       <c r="Q206" s="18"/>
     </row>
-    <row r="207" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A207" s="18" t="s">
         <v>622</v>
       </c>
@@ -7299,7 +7305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A208" s="18" t="s">
         <v>625</v>
       </c>
@@ -7328,7 +7334,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="54" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" ht="75" x14ac:dyDescent="0.3">
       <c r="A209" s="18" t="s">
         <v>628</v>
       </c>
@@ -7357,7 +7363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="36" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A210" s="18" t="s">
         <v>631</v>
       </c>
@@ -7386,7 +7392,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A211" s="18" t="s">
         <v>634</v>
       </c>
@@ -7415,7 +7421,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>637</v>
       </c>
@@ -7432,7 +7438,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>642</v>
       </c>
@@ -7461,7 +7467,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>645</v>
       </c>
@@ -7481,7 +7487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>649</v>
       </c>
@@ -7498,7 +7504,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>653</v>
       </c>
@@ -7518,7 +7524,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>657</v>
       </c>
@@ -7538,7 +7544,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>662</v>
       </c>
@@ -7558,7 +7564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>666</v>
       </c>
@@ -7575,7 +7581,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>669</v>
       </c>
@@ -7593,7 +7599,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>672</v>
       </c>
@@ -7611,7 +7617,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>675</v>
       </c>
@@ -7629,7 +7635,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>678</v>
       </c>
@@ -7663,7 +7669,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
reviewd and tested Game Play and Game Termination requirements
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bipinadhikari/Downloads/project/cse3310-sp25-004/FinalRequirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pirte/Desktop/funda/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082BF674-5082-784B-BC27-CCDF783BB769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C1CD74-D52D-2E4C-90FF-51899F99E403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="775">
   <si>
     <t>Tested By</t>
   </si>
@@ -2365,6 +2365,9 @@
   </si>
   <si>
     <t>pass test 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pass </t>
   </si>
 </sst>
 </file>
@@ -2485,7 +2488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2531,7 +2534,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3328,8 +3330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="68" workbookViewId="0">
-      <selection activeCell="I150" sqref="I150"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.3984375" defaultRowHeight="15"/>
@@ -3893,7 +3895,9 @@
       <c r="G14" s="3"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>774</v>
+      </c>
       <c r="K14" s="2" t="s">
         <v>122</v>
       </c>
@@ -3937,7 +3941,9 @@
       <c r="G15" s="3"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="K15" s="2" t="s">
         <v>125</v>
       </c>
@@ -3981,7 +3987,9 @@
       <c r="G16" s="3"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="J16" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="K16" s="2" t="s">
         <v>128</v>
       </c>
@@ -4025,7 +4033,9 @@
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="K17" s="2" t="s">
         <v>132</v>
       </c>
@@ -4067,7 +4077,9 @@
       <c r="G18" s="3"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="K18" s="2" t="s">
         <v>135</v>
       </c>
@@ -4109,7 +4121,9 @@
       <c r="G19" s="3"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="K19" s="2" t="s">
         <v>140</v>
       </c>
@@ -4147,7 +4161,9 @@
       <c r="G20" s="3"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="K20" s="2" t="s">
         <v>143</v>
       </c>
@@ -5337,7 +5353,9 @@
       <c r="G45" s="3"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="J45" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K45" s="2" t="s">
         <v>228</v>
       </c>
@@ -5375,7 +5393,9 @@
       <c r="G46" s="3"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="J46" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K46" s="2" t="s">
         <v>231</v>
       </c>
@@ -5415,7 +5435,9 @@
       <c r="G47" s="3"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="J47" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K47" s="2" t="s">
         <v>234</v>
       </c>
@@ -5457,7 +5479,9 @@
       <c r="G48" s="3"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="J48" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K48" s="2" t="s">
         <v>238</v>
       </c>
@@ -5497,7 +5521,9 @@
       <c r="G49" s="3"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
+      <c r="J49" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K49" s="2" t="s">
         <v>241</v>
       </c>
@@ -5587,7 +5613,9 @@
       <c r="G51" s="3"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="J51" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K51" s="2" t="s">
         <v>31</v>
       </c>
@@ -5627,7 +5655,9 @@
       <c r="G52" s="3"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="J52" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K52" s="2" t="s">
         <v>31</v>
       </c>
@@ -5667,7 +5697,9 @@
       <c r="G53" s="3"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
+      <c r="J53" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K53" s="2" t="s">
         <v>253</v>
       </c>
@@ -5704,7 +5736,9 @@
       <c r="G54" s="3"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
+      <c r="J54" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K54" s="2" t="s">
         <v>256</v>
       </c>
@@ -5744,7 +5778,9 @@
       <c r="G55" s="3"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="J55" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K55" s="2" t="s">
         <v>259</v>
       </c>
@@ -5786,7 +5822,9 @@
       <c r="G56" s="3"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
+      <c r="J56" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K56" s="2" t="s">
         <v>262</v>
       </c>
@@ -9370,7 +9408,7 @@
       <c r="G142" s="3"/>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
-      <c r="J142" s="23" t="s">
+      <c r="J142" s="22" t="s">
         <v>186</v>
       </c>
       <c r="K142" s="2" t="s">

</xml_diff>

<commit_message>
bot I and Bot II requirements tested
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pirte/Desktop/funda/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C1CD74-D52D-2E4C-90FF-51899F99E403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80949B83-1D1D-6D40-90DB-A473952130E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="27040" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="776">
   <si>
     <t>Tested By</t>
   </si>
@@ -2368,6 +2368,9 @@
   </si>
   <si>
     <t xml:space="preserve">pass </t>
+  </si>
+  <si>
+    <t>step4, fail</t>
   </si>
 </sst>
 </file>
@@ -3330,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="89" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.3984375" defaultRowHeight="15"/>
@@ -8952,7 +8955,9 @@
       <c r="G130" s="3"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
-      <c r="J130" s="2"/>
+      <c r="J130" s="2" t="s">
+        <v>775</v>
+      </c>
       <c r="K130" s="6" t="s">
         <v>65</v>
       </c>
@@ -8990,7 +8995,9 @@
       <c r="G131" s="3"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
-      <c r="J131" s="2"/>
+      <c r="J131" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K131" s="2" t="s">
         <v>53</v>
       </c>
@@ -9028,7 +9035,9 @@
       <c r="G132" s="3"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
-      <c r="J132" s="2"/>
+      <c r="J132" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K132" s="2" t="s">
         <v>478</v>
       </c>
@@ -9066,7 +9075,9 @@
       <c r="G133" s="3"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
-      <c r="J133" s="2"/>
+      <c r="J133" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K133" s="2" t="s">
         <v>481</v>
       </c>
@@ -9104,7 +9115,9 @@
       <c r="G134" s="3"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
-      <c r="J134" s="2"/>
+      <c r="J134" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K134" s="2" t="s">
         <v>485</v>
       </c>
@@ -9142,7 +9155,9 @@
       <c r="G135" s="3"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
+      <c r="J135" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K135" s="2" t="s">
         <v>489</v>
       </c>
@@ -9180,7 +9195,9 @@
       <c r="G136" s="3"/>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
-      <c r="J136" s="2"/>
+      <c r="J136" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K136" s="2" t="s">
         <v>493</v>
       </c>
@@ -9218,7 +9235,9 @@
       <c r="G137" s="3"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
-      <c r="J137" s="2"/>
+      <c r="J137" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K137" s="2" t="s">
         <v>497</v>
       </c>
@@ -9256,7 +9275,9 @@
       <c r="G138" s="3"/>
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
-      <c r="J138" s="2"/>
+      <c r="J138" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K138" s="2" t="s">
         <v>501</v>
       </c>
@@ -9294,7 +9315,9 @@
       <c r="G139" s="3"/>
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
-      <c r="J139" s="2"/>
+      <c r="J139" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K139" s="2" t="s">
         <v>505</v>
       </c>
@@ -9332,7 +9355,9 @@
       <c r="G140" s="3"/>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
-      <c r="J140" s="2"/>
+      <c r="J140" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K140" s="2" t="s">
         <v>509</v>
       </c>
@@ -9370,7 +9395,9 @@
       <c r="G141" s="3"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
-      <c r="J141" s="2"/>
+      <c r="J141" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K141" s="2" t="s">
         <v>513</v>
       </c>
@@ -10106,7 +10133,9 @@
       <c r="G159" s="3"/>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
-      <c r="J159" s="2"/>
+      <c r="J159" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K159" s="2" t="s">
         <v>65</v>
       </c>
@@ -10148,7 +10177,9 @@
       <c r="G160" s="3"/>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
-      <c r="J160" s="2"/>
+      <c r="J160" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K160" s="2" t="s">
         <v>65</v>
       </c>
@@ -10274,7 +10305,9 @@
       <c r="G163" s="3"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
-      <c r="J163" s="2"/>
+      <c r="J163" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K163" s="2" t="s">
         <v>65</v>
       </c>
@@ -10358,7 +10391,9 @@
       <c r="G165" s="3"/>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
-      <c r="J165" s="2"/>
+      <c r="J165" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K165" s="2" t="s">
         <v>65</v>
       </c>
@@ -10400,7 +10435,9 @@
       <c r="G166" s="3"/>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
-      <c r="J166" s="2"/>
+      <c r="J166" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K166" s="2" t="s">
         <v>65</v>
       </c>
@@ -10442,7 +10479,9 @@
       <c r="G167" s="3"/>
       <c r="H167" s="2"/>
       <c r="I167" s="2"/>
-      <c r="J167" s="2"/>
+      <c r="J167" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K167" s="2" t="s">
         <v>65</v>
       </c>
@@ -10484,7 +10523,9 @@
       <c r="G168" s="3"/>
       <c r="H168" s="2"/>
       <c r="I168" s="2"/>
-      <c r="J168" s="2"/>
+      <c r="J168" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K168" s="2" t="s">
         <v>65</v>
       </c>
@@ -10526,7 +10567,9 @@
       <c r="G169" s="3"/>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
-      <c r="J169" s="2"/>
+      <c r="J169" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K169" s="2" t="s">
         <v>65</v>
       </c>
@@ -10568,7 +10611,9 @@
       <c r="G170" s="3"/>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
-      <c r="J170" s="2"/>
+      <c r="J170" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K170" s="2" t="s">
         <v>65</v>
       </c>
@@ -10694,7 +10739,9 @@
       <c r="G173" s="3"/>
       <c r="H173" s="2"/>
       <c r="I173" s="2"/>
-      <c r="J173" s="2"/>
+      <c r="J173" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K173" s="2" t="s">
         <v>65</v>
       </c>
@@ -10736,7 +10783,9 @@
       <c r="G174" s="3"/>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
-      <c r="J174" s="2"/>
+      <c r="J174" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="K174" s="2" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
T7 summary req update
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\code\CSE3310\cse3310-sp25-004\FinalRequirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6494FE25-25FE-458A-AD8A-310BB3E2575D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFC52AA-B0D0-47DF-9CAF-D72934D23850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="851">
   <si>
     <t>Tested By</t>
   </si>
@@ -2581,6 +2581,18 @@
   </si>
   <si>
     <t>T4 S3</t>
+  </si>
+  <si>
+    <t>T4 S30</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>T4 S32</t>
+  </si>
+  <si>
+    <t>T4 S31</t>
   </si>
 </sst>
 </file>
@@ -3098,7 +3110,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E130" zoomScale="96" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E132" zoomScale="96" workbookViewId="0">
       <selection activeCell="M154" sqref="M154"/>
     </sheetView>
   </sheetViews>
@@ -9694,7 +9706,7 @@
         <v>392</v>
       </c>
       <c r="M145" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="N145" s="2"/>
       <c r="O145" s="2"/>
@@ -9740,7 +9752,7 @@
       </c>
       <c r="L146" s="2"/>
       <c r="M146" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
@@ -9784,7 +9796,7 @@
       </c>
       <c r="L147" s="2"/>
       <c r="M147" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
@@ -9872,7 +9884,7 @@
       </c>
       <c r="L149" s="2"/>
       <c r="M149" s="2" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -9916,7 +9928,7 @@
       </c>
       <c r="L150" s="2"/>
       <c r="M150" s="2" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="N150" s="2"/>
       <c r="O150" s="2"/>
@@ -9960,7 +9972,7 @@
       </c>
       <c r="L151" s="2"/>
       <c r="M151" s="2" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -10006,7 +10018,7 @@
         <v>392</v>
       </c>
       <c r="M152" s="2" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="N152" s="2"/>
       <c r="O152" s="2"/>
@@ -10052,7 +10064,7 @@
         <v>392</v>
       </c>
       <c r="M153" s="2" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="N153" s="2"/>
       <c r="O153" s="2"/>

</xml_diff>

<commit_message>
finaaaaal team 3 add
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a314dec4b6146c21/Desktop/school/spring2025/cse3310/cse3310-sp25-004/FinalRequirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F602BED-CC2B-4A11-B04C-4760583D48A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6AA057C0-ABDD-42E0-B100-BB6BD23361F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="1041">
   <si>
     <t>Tested By</t>
   </si>
@@ -3139,6 +3139,30 @@
   </si>
   <si>
     <t>2 : S1-6</t>
+  </si>
+  <si>
+    <t>Test 6: Step 1</t>
+  </si>
+  <si>
+    <t>Test 6: Step 2</t>
+  </si>
+  <si>
+    <t>Test 6: Step 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 6: Step 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 6: Step 2 </t>
+  </si>
+  <si>
+    <t>Test 6: Step 3</t>
+  </si>
+  <si>
+    <t>Test 6: Step 3 fail</t>
+  </si>
+  <si>
+    <t>Test 6: Step 16 fail</t>
   </si>
 </sst>
 </file>
@@ -3668,8 +3692,8 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D176" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L200" sqref="L200"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I224" sqref="I224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11711,7 +11735,7 @@
         <v>656</v>
       </c>
       <c r="I159" s="7" t="s">
-        <v>946</v>
+        <v>1033</v>
       </c>
       <c r="J159" s="2" t="s">
         <v>85</v>
@@ -11763,7 +11787,7 @@
         <v>643</v>
       </c>
       <c r="I160" s="7" t="s">
-        <v>946</v>
+        <v>1034</v>
       </c>
       <c r="J160" s="2" t="s">
         <v>85</v>
@@ -11815,7 +11839,7 @@
         <v>29</v>
       </c>
       <c r="I161" s="7" t="s">
-        <v>946</v>
+        <v>1034</v>
       </c>
       <c r="J161" s="2"/>
       <c r="K161" s="2" t="s">
@@ -11865,7 +11889,7 @@
         <v>667</v>
       </c>
       <c r="I162" s="7" t="s">
-        <v>946</v>
+        <v>30</v>
       </c>
       <c r="J162" s="2"/>
       <c r="K162" s="2" t="s">
@@ -11915,7 +11939,7 @@
         <v>670</v>
       </c>
       <c r="I163" s="7" t="s">
-        <v>946</v>
+        <v>1035</v>
       </c>
       <c r="J163" s="2" t="s">
         <v>85</v>
@@ -11967,7 +11991,7 @@
         <v>29</v>
       </c>
       <c r="I164" s="7" t="s">
-        <v>946</v>
+        <v>1036</v>
       </c>
       <c r="J164" s="2"/>
       <c r="K164" s="2" t="s">
@@ -12069,7 +12093,7 @@
         <v>682</v>
       </c>
       <c r="I166" s="7" t="s">
-        <v>946</v>
+        <v>1037</v>
       </c>
       <c r="J166" s="2" t="s">
         <v>85</v>
@@ -12121,7 +12145,7 @@
         <v>687</v>
       </c>
       <c r="I167" s="7" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="J167" s="2" t="s">
         <v>85</v>
@@ -12173,7 +12197,7 @@
         <v>29</v>
       </c>
       <c r="I168" s="7" t="s">
-        <v>946</v>
+        <v>1038</v>
       </c>
       <c r="J168" s="2" t="s">
         <v>85</v>
@@ -12277,7 +12301,7 @@
         <v>29</v>
       </c>
       <c r="I170" s="7" t="s">
-        <v>946</v>
+        <v>1039</v>
       </c>
       <c r="J170" s="2" t="s">
         <v>85</v>
@@ -12429,7 +12453,7 @@
         <v>29</v>
       </c>
       <c r="I173" s="7" t="s">
-        <v>946</v>
+        <v>1034</v>
       </c>
       <c r="J173" s="2" t="s">
         <v>85</v>
@@ -12481,7 +12505,7 @@
         <v>29</v>
       </c>
       <c r="I174" s="7" t="s">
-        <v>946</v>
+        <v>1040</v>
       </c>
       <c r="J174" s="2" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
req update pair up j column
</commit_message>
<xml_diff>
--- a/FinalRequirements/FinalRequirements.xlsx
+++ b/FinalRequirements/FinalRequirements.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2768" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="1049">
   <si>
     <t xml:space="preserve">Tested By</t>
   </si>
@@ -3356,64 +3356,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3421,47 +3413,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3715,8 +3719,8 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J107" activeCellId="0" sqref="J107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3734,7 +3738,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="9.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="9.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="26.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="10.83"/>
@@ -5093,7 +5097,9 @@
       <c r="I28" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="J28" s="4"/>
+      <c r="J28" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="K28" s="4" t="s">
         <v>129</v>
       </c>
@@ -5131,7 +5137,7 @@
         <v>107</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="14" t="s">
         <v>134</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -5147,7 +5153,9 @@
       <c r="I29" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="J29" s="4"/>
+      <c r="J29" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="K29" s="4" t="s">
         <v>138</v>
       </c>
@@ -5195,13 +5203,15 @@
       <c r="G30" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="14" t="s">
         <v>143</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="K30" s="4" t="s">
         <v>29</v>
       </c>
@@ -5255,7 +5265,9 @@
       <c r="I31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="J31" s="4"/>
+      <c r="J31" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="K31" s="4" t="s">
         <v>148</v>
       </c>
@@ -5309,7 +5321,9 @@
       <c r="I32" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="J32" s="4"/>
+      <c r="J32" s="13" t="s">
+        <v>46</v>
+      </c>
       <c r="K32" s="4" t="s">
         <v>155</v>
       </c>
@@ -6925,7 +6939,7 @@
         <v>306</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="15" t="s">
         <v>307</v>
       </c>
       <c r="E62" s="4" t="s">
@@ -9335,7 +9349,7 @@
       <c r="I107" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="J107" s="15" t="s">
+      <c r="J107" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K107" s="4" t="s">
@@ -9352,7 +9366,7 @@
       <c r="P107" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q107" s="16"/>
+      <c r="Q107" s="17"/>
       <c r="R107" s="11" t="s">
         <v>536</v>
       </c>
@@ -9387,7 +9401,7 @@
       <c r="I108" s="10" t="s">
         <v>539</v>
       </c>
-      <c r="J108" s="15" t="s">
+      <c r="J108" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K108" s="4" t="s">
@@ -9402,7 +9416,7 @@
       <c r="P108" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q108" s="16"/>
+      <c r="Q108" s="17"/>
       <c r="R108" s="11" t="s">
         <v>541</v>
       </c>
@@ -9439,7 +9453,7 @@
       <c r="I109" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="J109" s="15" t="s">
+      <c r="J109" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K109" s="4" t="s">
@@ -9456,7 +9470,7 @@
       <c r="P109" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q109" s="16"/>
+      <c r="Q109" s="17"/>
       <c r="R109" s="11" t="s">
         <v>132</v>
       </c>
@@ -9491,7 +9505,7 @@
       <c r="I110" s="10" t="s">
         <v>550</v>
       </c>
-      <c r="J110" s="15" t="s">
+      <c r="J110" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K110" s="4"/>
@@ -9504,7 +9518,7 @@
       <c r="P110" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q110" s="16"/>
+      <c r="Q110" s="17"/>
       <c r="R110" s="11" t="s">
         <v>30</v>
       </c>
@@ -9539,7 +9553,7 @@
       <c r="I111" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J111" s="15" t="s">
+      <c r="J111" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K111" s="4"/>
@@ -9552,7 +9566,7 @@
       <c r="P111" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q111" s="16"/>
+      <c r="Q111" s="17"/>
       <c r="R111" s="11" t="s">
         <v>412</v>
       </c>
@@ -9587,7 +9601,7 @@
       <c r="I112" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="J112" s="15" t="s">
+      <c r="J112" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K112" s="4"/>
@@ -9600,7 +9614,7 @@
       <c r="P112" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q112" s="16"/>
+      <c r="Q112" s="17"/>
       <c r="R112" s="11" t="s">
         <v>30</v>
       </c>
@@ -9635,7 +9649,7 @@
       <c r="I113" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="J113" s="15" t="s">
+      <c r="J113" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K113" s="4"/>
@@ -9648,7 +9662,7 @@
       <c r="P113" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q113" s="16"/>
+      <c r="Q113" s="17"/>
       <c r="R113" s="11" t="s">
         <v>536</v>
       </c>
@@ -9683,7 +9697,7 @@
       <c r="I114" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="J114" s="15" t="s">
+      <c r="J114" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K114" s="4"/>
@@ -9696,7 +9710,7 @@
       <c r="P114" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q114" s="16"/>
+      <c r="Q114" s="17"/>
       <c r="R114" s="11" t="s">
         <v>30</v>
       </c>
@@ -9731,7 +9745,7 @@
       <c r="I115" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="J115" s="15" t="s">
+      <c r="J115" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K115" s="4"/>
@@ -9744,7 +9758,7 @@
       <c r="P115" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q115" s="16"/>
+      <c r="Q115" s="17"/>
       <c r="R115" s="11" t="s">
         <v>168</v>
       </c>
@@ -9779,7 +9793,7 @@
       <c r="I116" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="J116" s="15" t="s">
+      <c r="J116" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K116" s="4"/>
@@ -9794,7 +9808,7 @@
       <c r="P116" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q116" s="16"/>
+      <c r="Q116" s="17"/>
       <c r="R116" s="11" t="s">
         <v>570</v>
       </c>
@@ -9829,7 +9843,7 @@
       <c r="I117" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="J117" s="15" t="s">
+      <c r="J117" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K117" s="4"/>
@@ -9842,7 +9856,7 @@
       <c r="P117" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q117" s="16"/>
+      <c r="Q117" s="17"/>
       <c r="R117" s="11" t="s">
         <v>570</v>
       </c>
@@ -9877,7 +9891,7 @@
       <c r="I118" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="J118" s="15" t="s">
+      <c r="J118" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K118" s="4"/>
@@ -9890,7 +9904,7 @@
       <c r="P118" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q118" s="16"/>
+      <c r="Q118" s="17"/>
       <c r="R118" s="11" t="s">
         <v>570</v>
       </c>
@@ -9925,7 +9939,7 @@
       <c r="I119" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="J119" s="15" t="s">
+      <c r="J119" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K119" s="4"/>
@@ -9938,7 +9952,7 @@
       <c r="P119" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q119" s="16"/>
+      <c r="Q119" s="17"/>
       <c r="R119" s="11" t="s">
         <v>570</v>
       </c>
@@ -9973,7 +9987,7 @@
       <c r="I120" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="J120" s="15" t="s">
+      <c r="J120" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K120" s="4"/>
@@ -9986,7 +10000,7 @@
       <c r="P120" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q120" s="16"/>
+      <c r="Q120" s="17"/>
       <c r="R120" s="11" t="s">
         <v>132</v>
       </c>
@@ -10021,7 +10035,7 @@
       <c r="I121" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="J121" s="15" t="s">
+      <c r="J121" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K121" s="4"/>
@@ -10034,7 +10048,7 @@
       <c r="P121" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="Q121" s="16"/>
+      <c r="Q121" s="17"/>
       <c r="R121" s="11" t="s">
         <v>132</v>
       </c>
@@ -10069,7 +10083,7 @@
       <c r="I122" s="10" t="s">
         <v>588</v>
       </c>
-      <c r="J122" s="15" t="s">
+      <c r="J122" s="16" t="s">
         <v>30</v>
       </c>
       <c r="K122" s="4"/>
@@ -10082,7 +10096,7 @@
       <c r="P122" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q122" s="16"/>
+      <c r="Q122" s="17"/>
       <c r="R122" s="11" t="s">
         <v>541</v>
       </c>
@@ -10117,7 +10131,7 @@
       <c r="I123" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="J123" s="15" t="s">
+      <c r="J123" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K123" s="4"/>
@@ -10130,7 +10144,7 @@
       <c r="P123" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q123" s="16"/>
+      <c r="Q123" s="17"/>
       <c r="R123" s="11" t="s">
         <v>570</v>
       </c>
@@ -10165,7 +10179,7 @@
       <c r="I124" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="J124" s="15" t="s">
+      <c r="J124" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K124" s="4"/>
@@ -10178,7 +10192,7 @@
       <c r="P124" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q124" s="16"/>
+      <c r="Q124" s="17"/>
       <c r="R124" s="11" t="s">
         <v>570</v>
       </c>
@@ -10213,7 +10227,7 @@
       <c r="I125" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="J125" s="15" t="s">
+      <c r="J125" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K125" s="4"/>
@@ -10226,7 +10240,7 @@
       <c r="P125" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q125" s="16"/>
+      <c r="Q125" s="17"/>
       <c r="R125" s="11" t="s">
         <v>570</v>
       </c>
@@ -10261,7 +10275,7 @@
       <c r="I126" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="J126" s="15" t="s">
+      <c r="J126" s="16" t="s">
         <v>46</v>
       </c>
       <c r="K126" s="4"/>
@@ -10274,7 +10288,7 @@
       <c r="P126" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="Q126" s="16"/>
+      <c r="Q126" s="17"/>
       <c r="R126" s="11" t="s">
         <v>570</v>
       </c>
@@ -10288,10 +10302,10 @@
       <c r="Z126" s="4"/>
     </row>
     <row r="127" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="17" t="s">
+      <c r="A127" s="18" t="s">
         <v>599</v>
       </c>
-      <c r="B127" s="17" t="s">
+      <c r="B127" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C127" s="12"/>
@@ -10322,7 +10336,7 @@
       <c r="P127" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="Q127" s="18" t="s">
+      <c r="Q127" s="19" t="s">
         <v>607</v>
       </c>
       <c r="R127" s="11" t="s">
@@ -10338,10 +10352,10 @@
       <c r="Z127" s="4"/>
     </row>
     <row r="128" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="17" t="s">
+      <c r="A128" s="18" t="s">
         <v>609</v>
       </c>
-      <c r="B128" s="17" t="s">
+      <c r="B128" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C128" s="12" t="s">
@@ -10392,10 +10406,10 @@
       <c r="Z128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="17" t="s">
+      <c r="A129" s="18" t="s">
         <v>612</v>
       </c>
-      <c r="B129" s="17" t="s">
+      <c r="B129" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C129" s="12"/>
@@ -10426,7 +10440,7 @@
       <c r="P129" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q129" s="18" t="s">
+      <c r="Q129" s="19" t="s">
         <v>607</v>
       </c>
       <c r="R129" s="11" t="s">
@@ -10442,10 +10456,10 @@
       <c r="Z129" s="4"/>
     </row>
     <row r="130" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="17" t="s">
+      <c r="A130" s="18" t="s">
         <v>618</v>
       </c>
-      <c r="B130" s="17" t="s">
+      <c r="B130" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C130" s="12"/>
@@ -10478,7 +10492,7 @@
       <c r="P130" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q130" s="18" t="s">
+      <c r="Q130" s="19" t="s">
         <v>623</v>
       </c>
       <c r="R130" s="11" t="s">
@@ -10494,10 +10508,10 @@
       <c r="Z130" s="4"/>
     </row>
     <row r="131" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="17" t="s">
+      <c r="A131" s="18" t="s">
         <v>625</v>
       </c>
-      <c r="B131" s="17" t="s">
+      <c r="B131" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C131" s="12"/>
@@ -10530,7 +10544,7 @@
       <c r="P131" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q131" s="18"/>
+      <c r="Q131" s="19"/>
       <c r="R131" s="11" t="s">
         <v>629</v>
       </c>
@@ -10544,10 +10558,10 @@
       <c r="Z131" s="4"/>
     </row>
     <row r="132" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="17" t="s">
+      <c r="A132" s="18" t="s">
         <v>630</v>
       </c>
-      <c r="B132" s="17" t="s">
+      <c r="B132" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C132" s="12"/>
@@ -10580,7 +10594,7 @@
       <c r="P132" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q132" s="18" t="s">
+      <c r="Q132" s="19" t="s">
         <v>101</v>
       </c>
       <c r="R132" s="11" t="s">
@@ -10596,10 +10610,10 @@
       <c r="Z132" s="4"/>
     </row>
     <row r="133" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="17" t="s">
+      <c r="A133" s="18" t="s">
         <v>637</v>
       </c>
-      <c r="B133" s="17" t="s">
+      <c r="B133" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C133" s="12"/>
@@ -10632,7 +10646,7 @@
       <c r="P133" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q133" s="18" t="s">
+      <c r="Q133" s="19" t="s">
         <v>101</v>
       </c>
       <c r="R133" s="11" t="s">
@@ -10648,10 +10662,10 @@
       <c r="Z133" s="4"/>
     </row>
     <row r="134" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="17" t="s">
+      <c r="A134" s="18" t="s">
         <v>641</v>
       </c>
-      <c r="B134" s="17" t="s">
+      <c r="B134" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C134" s="12"/>
@@ -10684,7 +10698,7 @@
       <c r="P134" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q134" s="18" t="s">
+      <c r="Q134" s="19" t="s">
         <v>647</v>
       </c>
       <c r="R134" s="11" t="s">
@@ -10700,10 +10714,10 @@
       <c r="Z134" s="4"/>
     </row>
     <row r="135" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="17" t="s">
+      <c r="A135" s="18" t="s">
         <v>648</v>
       </c>
-      <c r="B135" s="17" t="s">
+      <c r="B135" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C135" s="12"/>
@@ -10736,7 +10750,7 @@
       <c r="P135" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q135" s="18" t="s">
+      <c r="Q135" s="19" t="s">
         <v>101</v>
       </c>
       <c r="R135" s="11" t="s">
@@ -10752,10 +10766,10 @@
       <c r="Z135" s="4"/>
     </row>
     <row r="136" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="17" t="s">
+      <c r="A136" s="18" t="s">
         <v>654</v>
       </c>
-      <c r="B136" s="17" t="s">
+      <c r="B136" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C136" s="12"/>
@@ -10788,7 +10802,7 @@
       <c r="P136" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q136" s="18" t="s">
+      <c r="Q136" s="19" t="s">
         <v>101</v>
       </c>
       <c r="R136" s="11" t="s">
@@ -10804,10 +10818,10 @@
       <c r="Z136" s="4"/>
     </row>
     <row r="137" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="17" t="s">
+      <c r="A137" s="18" t="s">
         <v>659</v>
       </c>
-      <c r="B137" s="17" t="s">
+      <c r="B137" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C137" s="12"/>
@@ -10840,7 +10854,7 @@
       <c r="P137" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q137" s="18" t="s">
+      <c r="Q137" s="19" t="s">
         <v>664</v>
       </c>
       <c r="R137" s="11" t="s">
@@ -10856,10 +10870,10 @@
       <c r="Z137" s="4"/>
     </row>
     <row r="138" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="17" t="s">
+      <c r="A138" s="18" t="s">
         <v>665</v>
       </c>
-      <c r="B138" s="17" t="s">
+      <c r="B138" s="18" t="s">
         <v>600</v>
       </c>
       <c r="C138" s="12"/>
@@ -10892,7 +10906,7 @@
       <c r="P138" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q138" s="18" t="s">
+      <c r="Q138" s="19" t="s">
         <v>623</v>
       </c>
       <c r="R138" s="11" t="s">
@@ -10908,10 +10922,10 @@
       <c r="Z138" s="4"/>
     </row>
     <row r="139" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="17" t="s">
+      <c r="A139" s="18" t="s">
         <v>670</v>
       </c>
-      <c r="B139" s="17" t="s">
+      <c r="B139" s="18" t="s">
         <v>671</v>
       </c>
       <c r="C139" s="12"/>
@@ -10944,7 +10958,7 @@
       <c r="P139" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q139" s="18" t="s">
+      <c r="Q139" s="19" t="s">
         <v>101</v>
       </c>
       <c r="R139" s="11" t="s">
@@ -10960,10 +10974,10 @@
       <c r="Z139" s="4"/>
     </row>
     <row r="140" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="17" t="s">
+      <c r="A140" s="18" t="s">
         <v>676</v>
       </c>
-      <c r="B140" s="17" t="s">
+      <c r="B140" s="18" t="s">
         <v>671</v>
       </c>
       <c r="C140" s="12"/>
@@ -10996,7 +11010,7 @@
       <c r="P140" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q140" s="18" t="s">
+      <c r="Q140" s="19" t="s">
         <v>623</v>
       </c>
       <c r="R140" s="11" t="s">
@@ -11012,13 +11026,13 @@
       <c r="Z140" s="4"/>
     </row>
     <row r="141" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="19" t="s">
+      <c r="A141" s="20" t="s">
         <v>681</v>
       </c>
-      <c r="B141" s="19" t="s">
+      <c r="B141" s="20" t="s">
         <v>600</v>
       </c>
-      <c r="C141" s="20"/>
+      <c r="C141" s="21"/>
       <c r="D141" s="4" t="s">
         <v>682</v>
       </c>
@@ -11048,7 +11062,7 @@
       <c r="P141" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="Q141" s="20" t="s">
+      <c r="Q141" s="21" t="s">
         <v>607</v>
       </c>
       <c r="R141" s="11" t="s">
@@ -11064,17 +11078,17 @@
       <c r="Z141" s="4"/>
     </row>
     <row r="142" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="21" t="s">
+      <c r="A142" s="22" t="s">
         <v>687</v>
       </c>
-      <c r="B142" s="21" t="s">
+      <c r="B142" s="22" t="s">
         <v>688</v>
       </c>
       <c r="C142" s="4"/>
-      <c r="D142" s="22" t="s">
+      <c r="D142" s="23" t="s">
         <v>689</v>
       </c>
-      <c r="E142" s="22" t="s">
+      <c r="E142" s="23" t="s">
         <v>690</v>
       </c>
       <c r="F142" s="4"/>
@@ -11118,17 +11132,17 @@
       <c r="Z142" s="4"/>
     </row>
     <row r="143" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="21" t="s">
+      <c r="A143" s="22" t="s">
         <v>696</v>
       </c>
-      <c r="B143" s="21" t="s">
+      <c r="B143" s="22" t="s">
         <v>688</v>
       </c>
       <c r="C143" s="4"/>
-      <c r="D143" s="22" t="s">
+      <c r="D143" s="23" t="s">
         <v>697</v>
       </c>
-      <c r="E143" s="22" t="s">
+      <c r="E143" s="23" t="s">
         <v>698</v>
       </c>
       <c r="F143" s="4"/>
@@ -11156,7 +11170,7 @@
       <c r="P143" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="Q143" s="22"/>
+      <c r="Q143" s="23"/>
       <c r="R143" s="11" t="s">
         <v>699</v>
       </c>
@@ -11170,17 +11184,17 @@
       <c r="Z143" s="4"/>
     </row>
     <row r="144" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="21" t="s">
+      <c r="A144" s="22" t="s">
         <v>700</v>
       </c>
-      <c r="B144" s="21" t="s">
+      <c r="B144" s="22" t="s">
         <v>688</v>
       </c>
       <c r="C144" s="4"/>
-      <c r="D144" s="22" t="s">
+      <c r="D144" s="23" t="s">
         <v>701</v>
       </c>
-      <c r="E144" s="22" t="s">
+      <c r="E144" s="23" t="s">
         <v>702</v>
       </c>
       <c r="F144" s="4"/>
@@ -11208,7 +11222,7 @@
       <c r="P144" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="Q144" s="22" t="s">
+      <c r="Q144" s="23" t="s">
         <v>694</v>
       </c>
       <c r="R144" s="11" t="s">
@@ -11224,17 +11238,17 @@
       <c r="Z144" s="4"/>
     </row>
     <row r="145" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="21" t="s">
+      <c r="A145" s="22" t="s">
         <v>706</v>
       </c>
-      <c r="B145" s="21" t="s">
+      <c r="B145" s="22" t="s">
         <v>688</v>
       </c>
       <c r="C145" s="4"/>
-      <c r="D145" s="22" t="s">
+      <c r="D145" s="23" t="s">
         <v>707</v>
       </c>
-      <c r="E145" s="22" t="s">
+      <c r="E145" s="23" t="s">
         <v>708</v>
       </c>
       <c r="F145" s="4"/>
@@ -11262,7 +11276,7 @@
       <c r="P145" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="Q145" s="22" t="s">
+      <c r="Q145" s="23" t="s">
         <v>694</v>
       </c>
       <c r="R145" s="11" t="s">
@@ -11278,17 +11292,17 @@
       <c r="Z145" s="4"/>
     </row>
     <row r="146" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="21" t="s">
+      <c r="A146" s="22" t="s">
         <v>713</v>
       </c>
-      <c r="B146" s="21" t="s">
+      <c r="B146" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C146" s="22"/>
-      <c r="D146" s="22" t="s">
+      <c r="C146" s="23"/>
+      <c r="D146" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="E146" s="22" t="s">
+      <c r="E146" s="23" t="s">
         <v>715</v>
       </c>
       <c r="F146" s="4"/>
@@ -11314,7 +11328,7 @@
       <c r="P146" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q146" s="22"/>
+      <c r="Q146" s="23"/>
       <c r="R146" s="11" t="s">
         <v>699</v>
       </c>
@@ -11328,17 +11342,17 @@
       <c r="Z146" s="4"/>
     </row>
     <row r="147" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="21" t="s">
+      <c r="A147" s="22" t="s">
         <v>720</v>
       </c>
-      <c r="B147" s="21" t="s">
+      <c r="B147" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C147" s="22"/>
-      <c r="D147" s="22" t="s">
+      <c r="C147" s="23"/>
+      <c r="D147" s="23" t="s">
         <v>721</v>
       </c>
-      <c r="E147" s="22" t="s">
+      <c r="E147" s="23" t="s">
         <v>722</v>
       </c>
       <c r="F147" s="4"/>
@@ -11364,7 +11378,7 @@
       <c r="P147" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q147" s="22" t="s">
+      <c r="Q147" s="23" t="s">
         <v>54</v>
       </c>
       <c r="R147" s="11" t="s">
@@ -11380,17 +11394,17 @@
       <c r="Z147" s="4"/>
     </row>
     <row r="148" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="21" t="s">
+      <c r="A148" s="22" t="s">
         <v>726</v>
       </c>
-      <c r="B148" s="21" t="s">
+      <c r="B148" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C148" s="22"/>
-      <c r="D148" s="22" t="s">
+      <c r="C148" s="23"/>
+      <c r="D148" s="23" t="s">
         <v>727</v>
       </c>
-      <c r="E148" s="22" t="s">
+      <c r="E148" s="23" t="s">
         <v>728</v>
       </c>
       <c r="F148" s="4"/>
@@ -11416,7 +11430,7 @@
       <c r="P148" s="4" t="s">
         <v>731</v>
       </c>
-      <c r="Q148" s="22"/>
+      <c r="Q148" s="23"/>
       <c r="R148" s="11" t="s">
         <v>699</v>
       </c>
@@ -11430,17 +11444,17 @@
       <c r="Z148" s="4"/>
     </row>
     <row r="149" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="21" t="s">
+      <c r="A149" s="22" t="s">
         <v>732</v>
       </c>
-      <c r="B149" s="21" t="s">
+      <c r="B149" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C149" s="22"/>
-      <c r="D149" s="22" t="s">
+      <c r="C149" s="23"/>
+      <c r="D149" s="23" t="s">
         <v>733</v>
       </c>
-      <c r="E149" s="22" t="s">
+      <c r="E149" s="23" t="s">
         <v>734</v>
       </c>
       <c r="F149" s="4"/>
@@ -11466,7 +11480,7 @@
       <c r="P149" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="Q149" s="22"/>
+      <c r="Q149" s="23"/>
       <c r="R149" s="11" t="s">
         <v>699</v>
       </c>
@@ -11480,17 +11494,17 @@
       <c r="Z149" s="4"/>
     </row>
     <row r="150" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="21" t="s">
+      <c r="A150" s="22" t="s">
         <v>739</v>
       </c>
-      <c r="B150" s="21" t="s">
+      <c r="B150" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C150" s="22"/>
-      <c r="D150" s="22" t="s">
+      <c r="C150" s="23"/>
+      <c r="D150" s="23" t="s">
         <v>740</v>
       </c>
-      <c r="E150" s="22" t="s">
+      <c r="E150" s="23" t="s">
         <v>741</v>
       </c>
       <c r="F150" s="4"/>
@@ -11516,7 +11530,7 @@
       <c r="P150" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Q150" s="22"/>
+      <c r="Q150" s="23"/>
       <c r="R150" s="11" t="s">
         <v>745</v>
       </c>
@@ -11530,17 +11544,17 @@
       <c r="Z150" s="4"/>
     </row>
     <row r="151" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="21" t="s">
+      <c r="A151" s="22" t="s">
         <v>746</v>
       </c>
-      <c r="B151" s="21" t="s">
+      <c r="B151" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C151" s="22"/>
-      <c r="D151" s="22" t="s">
+      <c r="C151" s="23"/>
+      <c r="D151" s="23" t="s">
         <v>747</v>
       </c>
-      <c r="E151" s="22" t="s">
+      <c r="E151" s="23" t="s">
         <v>748</v>
       </c>
       <c r="F151" s="4"/>
@@ -11566,7 +11580,7 @@
       <c r="P151" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q151" s="22"/>
+      <c r="Q151" s="23"/>
       <c r="R151" s="11" t="s">
         <v>699</v>
       </c>
@@ -11580,17 +11594,17 @@
       <c r="Z151" s="4"/>
     </row>
     <row r="152" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="21" t="s">
+      <c r="A152" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="B152" s="21" t="s">
+      <c r="B152" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C152" s="22"/>
-      <c r="D152" s="22" t="s">
+      <c r="C152" s="23"/>
+      <c r="D152" s="23" t="s">
         <v>753</v>
       </c>
-      <c r="E152" s="22" t="s">
+      <c r="E152" s="23" t="s">
         <v>754</v>
       </c>
       <c r="F152" s="4"/>
@@ -11618,7 +11632,7 @@
       <c r="P152" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q152" s="22" t="s">
+      <c r="Q152" s="23" t="s">
         <v>759</v>
       </c>
       <c r="R152" s="11" t="s">
@@ -11634,17 +11648,17 @@
       <c r="Z152" s="4"/>
     </row>
     <row r="153" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="21" t="s">
+      <c r="A153" s="22" t="s">
         <v>760</v>
       </c>
-      <c r="B153" s="21" t="s">
+      <c r="B153" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="C153" s="22"/>
-      <c r="D153" s="22" t="s">
+      <c r="C153" s="23"/>
+      <c r="D153" s="23" t="s">
         <v>761</v>
       </c>
-      <c r="E153" s="22" t="s">
+      <c r="E153" s="23" t="s">
         <v>754</v>
       </c>
       <c r="F153" s="4"/>
@@ -11672,7 +11686,7 @@
       <c r="P153" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Q153" s="22" t="s">
+      <c r="Q153" s="23" t="s">
         <v>46</v>
       </c>
       <c r="R153" s="11" t="s">
@@ -11695,10 +11709,10 @@
         <v>766</v>
       </c>
       <c r="C154" s="4"/>
-      <c r="D154" s="23" t="s">
+      <c r="D154" s="24" t="s">
         <v>767</v>
       </c>
-      <c r="E154" s="23" t="s">
+      <c r="E154" s="24" t="s">
         <v>768</v>
       </c>
       <c r="F154" s="4"/>
@@ -11751,10 +11765,10 @@
       <c r="C155" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D155" s="23" t="s">
+      <c r="D155" s="24" t="s">
         <v>773</v>
       </c>
-      <c r="E155" s="23" t="s">
+      <c r="E155" s="24" t="s">
         <v>774</v>
       </c>
       <c r="F155" s="4"/>
@@ -11805,10 +11819,10 @@
         <v>766</v>
       </c>
       <c r="C156" s="4"/>
-      <c r="D156" s="23" t="s">
+      <c r="D156" s="24" t="s">
         <v>777</v>
       </c>
-      <c r="E156" s="23" t="s">
+      <c r="E156" s="24" t="s">
         <v>778</v>
       </c>
       <c r="F156" s="4"/>
@@ -11859,10 +11873,10 @@
         <v>766</v>
       </c>
       <c r="C157" s="4"/>
-      <c r="D157" s="23" t="s">
+      <c r="D157" s="24" t="s">
         <v>781</v>
       </c>
-      <c r="E157" s="23" t="s">
+      <c r="E157" s="24" t="s">
         <v>782</v>
       </c>
       <c r="F157" s="4"/>
@@ -11913,10 +11927,10 @@
         <v>766</v>
       </c>
       <c r="C158" s="4"/>
-      <c r="D158" s="23" t="s">
+      <c r="D158" s="24" t="s">
         <v>786</v>
       </c>
-      <c r="E158" s="23" t="s">
+      <c r="E158" s="24" t="s">
         <v>787</v>
       </c>
       <c r="F158" s="4"/>
@@ -11967,10 +11981,10 @@
         <v>766</v>
       </c>
       <c r="C159" s="4"/>
-      <c r="D159" s="23" t="s">
+      <c r="D159" s="24" t="s">
         <v>789</v>
       </c>
-      <c r="E159" s="23" t="s">
+      <c r="E159" s="24" t="s">
         <v>774</v>
       </c>
       <c r="F159" s="4"/>
@@ -12021,10 +12035,10 @@
         <v>766</v>
       </c>
       <c r="C160" s="4"/>
-      <c r="D160" s="23" t="s">
+      <c r="D160" s="24" t="s">
         <v>795</v>
       </c>
-      <c r="E160" s="23" t="s">
+      <c r="E160" s="24" t="s">
         <v>796</v>
       </c>
       <c r="F160" s="4"/>
@@ -12075,10 +12089,10 @@
         <v>766</v>
       </c>
       <c r="C161" s="4"/>
-      <c r="D161" s="23" t="s">
+      <c r="D161" s="24" t="s">
         <v>799</v>
       </c>
-      <c r="E161" s="23" t="s">
+      <c r="E161" s="24" t="s">
         <v>800</v>
       </c>
       <c r="F161" s="4"/>
@@ -12127,10 +12141,10 @@
         <v>766</v>
       </c>
       <c r="C162" s="4"/>
-      <c r="D162" s="23" t="s">
+      <c r="D162" s="24" t="s">
         <v>803</v>
       </c>
-      <c r="E162" s="23" t="s">
+      <c r="E162" s="24" t="s">
         <v>787</v>
       </c>
       <c r="F162" s="4"/>
@@ -12179,10 +12193,10 @@
         <v>766</v>
       </c>
       <c r="C163" s="4"/>
-      <c r="D163" s="23" t="s">
+      <c r="D163" s="24" t="s">
         <v>806</v>
       </c>
-      <c r="E163" s="23" t="s">
+      <c r="E163" s="24" t="s">
         <v>774</v>
       </c>
       <c r="F163" s="4"/>
@@ -12233,10 +12247,10 @@
         <v>766</v>
       </c>
       <c r="C164" s="4"/>
-      <c r="D164" s="23" t="s">
+      <c r="D164" s="24" t="s">
         <v>811</v>
       </c>
-      <c r="E164" s="23" t="s">
+      <c r="E164" s="24" t="s">
         <v>812</v>
       </c>
       <c r="F164" s="4"/>
@@ -12285,10 +12299,10 @@
         <v>766</v>
       </c>
       <c r="C165" s="4"/>
-      <c r="D165" s="23" t="s">
+      <c r="D165" s="24" t="s">
         <v>815</v>
       </c>
-      <c r="E165" s="23" t="s">
+      <c r="E165" s="24" t="s">
         <v>816</v>
       </c>
       <c r="F165" s="4"/>
@@ -12339,10 +12353,10 @@
         <v>766</v>
       </c>
       <c r="C166" s="4"/>
-      <c r="D166" s="23" t="s">
+      <c r="D166" s="24" t="s">
         <v>820</v>
       </c>
-      <c r="E166" s="23" t="s">
+      <c r="E166" s="24" t="s">
         <v>821</v>
       </c>
       <c r="F166" s="4"/>
@@ -12393,10 +12407,10 @@
         <v>766</v>
       </c>
       <c r="C167" s="4"/>
-      <c r="D167" s="24" t="s">
+      <c r="D167" s="25" t="s">
         <v>826</v>
       </c>
-      <c r="E167" s="23" t="s">
+      <c r="E167" s="24" t="s">
         <v>827</v>
       </c>
       <c r="F167" s="4"/>
@@ -12447,10 +12461,10 @@
         <v>766</v>
       </c>
       <c r="C168" s="4"/>
-      <c r="D168" s="24" t="s">
+      <c r="D168" s="25" t="s">
         <v>831</v>
       </c>
-      <c r="E168" s="23" t="s">
+      <c r="E168" s="24" t="s">
         <v>832</v>
       </c>
       <c r="F168" s="4"/>
@@ -12501,10 +12515,10 @@
         <v>766</v>
       </c>
       <c r="C169" s="4"/>
-      <c r="D169" s="23" t="s">
+      <c r="D169" s="24" t="s">
         <v>835</v>
       </c>
-      <c r="E169" s="23" t="s">
+      <c r="E169" s="24" t="s">
         <v>836</v>
       </c>
       <c r="F169" s="4"/>
@@ -12555,10 +12569,10 @@
         <v>766</v>
       </c>
       <c r="C170" s="4"/>
-      <c r="D170" s="23" t="s">
+      <c r="D170" s="24" t="s">
         <v>840</v>
       </c>
-      <c r="E170" s="23" t="s">
+      <c r="E170" s="24" t="s">
         <v>841</v>
       </c>
       <c r="F170" s="4"/>
@@ -12609,10 +12623,10 @@
         <v>766</v>
       </c>
       <c r="C171" s="4"/>
-      <c r="D171" s="23" t="s">
+      <c r="D171" s="24" t="s">
         <v>845</v>
       </c>
-      <c r="E171" s="23" t="s">
+      <c r="E171" s="24" t="s">
         <v>841</v>
       </c>
       <c r="F171" s="4"/>
@@ -12661,10 +12675,10 @@
         <v>766</v>
       </c>
       <c r="C172" s="4"/>
-      <c r="D172" s="23" t="s">
+      <c r="D172" s="24" t="s">
         <v>847</v>
       </c>
-      <c r="E172" s="23" t="s">
+      <c r="E172" s="24" t="s">
         <v>841</v>
       </c>
       <c r="F172" s="4"/>
@@ -12713,10 +12727,10 @@
         <v>766</v>
       </c>
       <c r="C173" s="4"/>
-      <c r="D173" s="23" t="s">
+      <c r="D173" s="24" t="s">
         <v>849</v>
       </c>
-      <c r="E173" s="23" t="s">
+      <c r="E173" s="24" t="s">
         <v>850</v>
       </c>
       <c r="F173" s="4"/>
@@ -12767,10 +12781,10 @@
         <v>766</v>
       </c>
       <c r="C174" s="4"/>
-      <c r="D174" s="23" t="s">
+      <c r="D174" s="24" t="s">
         <v>852</v>
       </c>
-      <c r="E174" s="23" t="s">
+      <c r="E174" s="24" t="s">
         <v>853</v>
       </c>
       <c r="F174" s="4"/>
@@ -12814,19 +12828,19 @@
       <c r="Z174" s="4"/>
     </row>
     <row r="175" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="25" t="s">
+      <c r="A175" s="26" t="s">
         <v>855</v>
       </c>
-      <c r="B175" s="25" t="s">
+      <c r="B175" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C175" s="23" t="s">
+      <c r="C175" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D175" s="23" t="s">
+      <c r="D175" s="24" t="s">
         <v>857</v>
       </c>
-      <c r="E175" s="23" t="s">
+      <c r="E175" s="24" t="s">
         <v>858</v>
       </c>
       <c r="F175" s="4"/>
@@ -12872,19 +12886,19 @@
       <c r="Z175" s="4"/>
     </row>
     <row r="176" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="25" t="s">
+      <c r="A176" s="26" t="s">
         <v>859</v>
       </c>
-      <c r="B176" s="25" t="s">
+      <c r="B176" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C176" s="23" t="s">
+      <c r="C176" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D176" s="23" t="s">
+      <c r="D176" s="24" t="s">
         <v>860</v>
       </c>
-      <c r="E176" s="23" t="s">
+      <c r="E176" s="24" t="s">
         <v>861</v>
       </c>
       <c r="F176" s="4"/>
@@ -12930,19 +12944,19 @@
       <c r="Z176" s="4"/>
     </row>
     <row r="177" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="25" t="s">
+      <c r="A177" s="26" t="s">
         <v>862</v>
       </c>
-      <c r="B177" s="25" t="s">
+      <c r="B177" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C177" s="23" t="s">
+      <c r="C177" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D177" s="23" t="s">
+      <c r="D177" s="24" t="s">
         <v>863</v>
       </c>
-      <c r="E177" s="23" t="s">
+      <c r="E177" s="24" t="s">
         <v>864</v>
       </c>
       <c r="F177" s="4"/>
@@ -12988,19 +13002,19 @@
       <c r="Z177" s="4"/>
     </row>
     <row r="178" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="25" t="s">
+      <c r="A178" s="26" t="s">
         <v>865</v>
       </c>
-      <c r="B178" s="25" t="s">
+      <c r="B178" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C178" s="23" t="s">
+      <c r="C178" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D178" s="23" t="s">
+      <c r="D178" s="24" t="s">
         <v>866</v>
       </c>
-      <c r="E178" s="23" t="s">
+      <c r="E178" s="24" t="s">
         <v>867</v>
       </c>
       <c r="F178" s="4"/>
@@ -13046,19 +13060,19 @@
       <c r="Z178" s="4"/>
     </row>
     <row r="179" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="25" t="s">
+      <c r="A179" s="26" t="s">
         <v>868</v>
       </c>
-      <c r="B179" s="25" t="s">
+      <c r="B179" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C179" s="23" t="s">
+      <c r="C179" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D179" s="23" t="s">
+      <c r="D179" s="24" t="s">
         <v>869</v>
       </c>
-      <c r="E179" s="23" t="s">
+      <c r="E179" s="24" t="s">
         <v>867</v>
       </c>
       <c r="F179" s="4"/>
@@ -13104,19 +13118,19 @@
       <c r="Z179" s="4"/>
     </row>
     <row r="180" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="25" t="s">
+      <c r="A180" s="26" t="s">
         <v>870</v>
       </c>
-      <c r="B180" s="25" t="s">
+      <c r="B180" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C180" s="23" t="s">
+      <c r="C180" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D180" s="23" t="s">
+      <c r="D180" s="24" t="s">
         <v>871</v>
       </c>
-      <c r="E180" s="23" t="s">
+      <c r="E180" s="24" t="s">
         <v>872</v>
       </c>
       <c r="F180" s="4"/>
@@ -13162,19 +13176,19 @@
       <c r="Z180" s="4"/>
     </row>
     <row r="181" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="25" t="s">
+      <c r="A181" s="26" t="s">
         <v>873</v>
       </c>
-      <c r="B181" s="25" t="s">
+      <c r="B181" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C181" s="23" t="s">
+      <c r="C181" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D181" s="23" t="s">
+      <c r="D181" s="24" t="s">
         <v>874</v>
       </c>
-      <c r="E181" s="23" t="s">
+      <c r="E181" s="24" t="s">
         <v>875</v>
       </c>
       <c r="F181" s="4"/>
@@ -13220,19 +13234,19 @@
       <c r="Z181" s="4"/>
     </row>
     <row r="182" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="25" t="s">
+      <c r="A182" s="26" t="s">
         <v>876</v>
       </c>
-      <c r="B182" s="25" t="s">
+      <c r="B182" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C182" s="23" t="s">
+      <c r="C182" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D182" s="23" t="s">
+      <c r="D182" s="24" t="s">
         <v>877</v>
       </c>
-      <c r="E182" s="23" t="s">
+      <c r="E182" s="24" t="s">
         <v>878</v>
       </c>
       <c r="F182" s="4"/>
@@ -13278,19 +13292,19 @@
       <c r="Z182" s="4"/>
     </row>
     <row r="183" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="25" t="s">
+      <c r="A183" s="26" t="s">
         <v>879</v>
       </c>
-      <c r="B183" s="25" t="s">
+      <c r="B183" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C183" s="23" t="s">
+      <c r="C183" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D183" s="23" t="s">
+      <c r="D183" s="24" t="s">
         <v>880</v>
       </c>
-      <c r="E183" s="23" t="s">
+      <c r="E183" s="24" t="s">
         <v>881</v>
       </c>
       <c r="F183" s="4"/>
@@ -13336,19 +13350,19 @@
       <c r="Z183" s="4"/>
     </row>
     <row r="184" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="25" t="s">
+      <c r="A184" s="26" t="s">
         <v>882</v>
       </c>
-      <c r="B184" s="25" t="s">
+      <c r="B184" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C184" s="23" t="s">
+      <c r="C184" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D184" s="23" t="s">
+      <c r="D184" s="24" t="s">
         <v>883</v>
       </c>
-      <c r="E184" s="23" t="s">
+      <c r="E184" s="24" t="s">
         <v>884</v>
       </c>
       <c r="F184" s="4"/>
@@ -13394,19 +13408,19 @@
       <c r="Z184" s="4"/>
     </row>
     <row r="185" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="25" t="s">
+      <c r="A185" s="26" t="s">
         <v>885</v>
       </c>
-      <c r="B185" s="25" t="s">
+      <c r="B185" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C185" s="23" t="s">
+      <c r="C185" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D185" s="23" t="s">
+      <c r="D185" s="24" t="s">
         <v>886</v>
       </c>
-      <c r="E185" s="23" t="s">
+      <c r="E185" s="24" t="s">
         <v>887</v>
       </c>
       <c r="F185" s="4"/>
@@ -13452,19 +13466,19 @@
       <c r="Z185" s="4"/>
     </row>
     <row r="186" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="25" t="s">
+      <c r="A186" s="26" t="s">
         <v>888</v>
       </c>
-      <c r="B186" s="25" t="s">
+      <c r="B186" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C186" s="23" t="s">
+      <c r="C186" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D186" s="23" t="s">
+      <c r="D186" s="24" t="s">
         <v>889</v>
       </c>
-      <c r="E186" s="23" t="s">
+      <c r="E186" s="24" t="s">
         <v>890</v>
       </c>
       <c r="F186" s="4"/>
@@ -13510,19 +13524,19 @@
       <c r="Z186" s="4"/>
     </row>
     <row r="187" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="25" t="s">
+      <c r="A187" s="26" t="s">
         <v>891</v>
       </c>
-      <c r="B187" s="25" t="s">
+      <c r="B187" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C187" s="23" t="s">
+      <c r="C187" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D187" s="23" t="s">
+      <c r="D187" s="24" t="s">
         <v>892</v>
       </c>
-      <c r="E187" s="23" t="s">
+      <c r="E187" s="24" t="s">
         <v>893</v>
       </c>
       <c r="F187" s="4"/>
@@ -13568,19 +13582,19 @@
       <c r="Z187" s="4"/>
     </row>
     <row r="188" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="25" t="s">
+      <c r="A188" s="26" t="s">
         <v>894</v>
       </c>
-      <c r="B188" s="25" t="s">
+      <c r="B188" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C188" s="23" t="s">
+      <c r="C188" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D188" s="23" t="s">
+      <c r="D188" s="24" t="s">
         <v>895</v>
       </c>
-      <c r="E188" s="23" t="s">
+      <c r="E188" s="24" t="s">
         <v>896</v>
       </c>
       <c r="F188" s="4"/>
@@ -13626,19 +13640,19 @@
       <c r="Z188" s="4"/>
     </row>
     <row r="189" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="25" t="s">
+      <c r="A189" s="26" t="s">
         <v>897</v>
       </c>
-      <c r="B189" s="25" t="s">
+      <c r="B189" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C189" s="23" t="s">
+      <c r="C189" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D189" s="23" t="s">
+      <c r="D189" s="24" t="s">
         <v>898</v>
       </c>
-      <c r="E189" s="23" t="s">
+      <c r="E189" s="24" t="s">
         <v>899</v>
       </c>
       <c r="F189" s="4"/>
@@ -13684,19 +13698,19 @@
       <c r="Z189" s="4"/>
     </row>
     <row r="190" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="25" t="s">
+      <c r="A190" s="26" t="s">
         <v>900</v>
       </c>
-      <c r="B190" s="25" t="s">
+      <c r="B190" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C190" s="23" t="s">
+      <c r="C190" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D190" s="23" t="s">
+      <c r="D190" s="24" t="s">
         <v>901</v>
       </c>
-      <c r="E190" s="23" t="s">
+      <c r="E190" s="24" t="s">
         <v>902</v>
       </c>
       <c r="F190" s="4"/>
@@ -13742,19 +13756,19 @@
       <c r="Z190" s="4"/>
     </row>
     <row r="191" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="25" t="s">
+      <c r="A191" s="26" t="s">
         <v>903</v>
       </c>
-      <c r="B191" s="25" t="s">
+      <c r="B191" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C191" s="23" t="s">
+      <c r="C191" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D191" s="23" t="s">
+      <c r="D191" s="24" t="s">
         <v>904</v>
       </c>
-      <c r="E191" s="23" t="s">
+      <c r="E191" s="24" t="s">
         <v>905</v>
       </c>
       <c r="F191" s="4"/>
@@ -13800,19 +13814,19 @@
       <c r="Z191" s="4"/>
     </row>
     <row r="192" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="25" t="s">
+      <c r="A192" s="26" t="s">
         <v>906</v>
       </c>
-      <c r="B192" s="25" t="s">
+      <c r="B192" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C192" s="23" t="s">
+      <c r="C192" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D192" s="23" t="s">
+      <c r="D192" s="24" t="s">
         <v>907</v>
       </c>
-      <c r="E192" s="23" t="s">
+      <c r="E192" s="24" t="s">
         <v>908</v>
       </c>
       <c r="F192" s="4"/>
@@ -13858,19 +13872,19 @@
       <c r="Z192" s="4"/>
     </row>
     <row r="193" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="25" t="s">
+      <c r="A193" s="26" t="s">
         <v>909</v>
       </c>
-      <c r="B193" s="25" t="s">
+      <c r="B193" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C193" s="23" t="s">
+      <c r="C193" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D193" s="23" t="s">
+      <c r="D193" s="24" t="s">
         <v>910</v>
       </c>
-      <c r="E193" s="23" t="s">
+      <c r="E193" s="24" t="s">
         <v>911</v>
       </c>
       <c r="F193" s="4"/>
@@ -13916,19 +13930,19 @@
       <c r="Z193" s="4"/>
     </row>
     <row r="194" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="25" t="s">
+      <c r="A194" s="26" t="s">
         <v>912</v>
       </c>
-      <c r="B194" s="25" t="s">
+      <c r="B194" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C194" s="23" t="s">
+      <c r="C194" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D194" s="23" t="s">
+      <c r="D194" s="24" t="s">
         <v>913</v>
       </c>
-      <c r="E194" s="23" t="s">
+      <c r="E194" s="24" t="s">
         <v>914</v>
       </c>
       <c r="F194" s="4"/>
@@ -13974,17 +13988,17 @@
       <c r="Z194" s="4"/>
     </row>
     <row r="195" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="25" t="s">
+      <c r="A195" s="26" t="s">
         <v>915</v>
       </c>
-      <c r="B195" s="25" t="s">
+      <c r="B195" s="26" t="s">
         <v>856</v>
       </c>
       <c r="C195" s="4"/>
-      <c r="D195" s="23" t="s">
+      <c r="D195" s="24" t="s">
         <v>916</v>
       </c>
-      <c r="E195" s="23" t="s">
+      <c r="E195" s="24" t="s">
         <v>917</v>
       </c>
       <c r="F195" s="4"/>
@@ -14010,7 +14024,7 @@
       <c r="P195" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q195" s="23" t="s">
+      <c r="Q195" s="24" t="s">
         <v>446</v>
       </c>
       <c r="R195" s="11" t="s">
@@ -14026,19 +14040,19 @@
       <c r="Z195" s="4"/>
     </row>
     <row r="196" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="25" t="s">
+      <c r="A196" s="26" t="s">
         <v>919</v>
       </c>
-      <c r="B196" s="25" t="s">
+      <c r="B196" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C196" s="23" t="s">
+      <c r="C196" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D196" s="23" t="s">
+      <c r="D196" s="24" t="s">
         <v>920</v>
       </c>
-      <c r="E196" s="23" t="s">
+      <c r="E196" s="24" t="s">
         <v>917</v>
       </c>
       <c r="F196" s="4"/>
@@ -14082,17 +14096,17 @@
       <c r="Z196" s="4"/>
     </row>
     <row r="197" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="25" t="s">
+      <c r="A197" s="26" t="s">
         <v>921</v>
       </c>
-      <c r="B197" s="25" t="s">
+      <c r="B197" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C197" s="23"/>
-      <c r="D197" s="23" t="s">
+      <c r="C197" s="24"/>
+      <c r="D197" s="24" t="s">
         <v>922</v>
       </c>
-      <c r="E197" s="23" t="s">
+      <c r="E197" s="24" t="s">
         <v>923</v>
       </c>
       <c r="F197" s="4"/>
@@ -14115,10 +14129,10 @@
         <v>54</v>
       </c>
       <c r="O197" s="4"/>
-      <c r="P197" s="23" t="s">
+      <c r="P197" s="24" t="s">
         <v>924</v>
       </c>
-      <c r="Q197" s="23"/>
+      <c r="Q197" s="24"/>
       <c r="R197" s="11" t="s">
         <v>925</v>
       </c>
@@ -14132,17 +14146,17 @@
       <c r="Z197" s="4"/>
     </row>
     <row r="198" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="25" t="s">
+      <c r="A198" s="26" t="s">
         <v>926</v>
       </c>
-      <c r="B198" s="25" t="s">
+      <c r="B198" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C198" s="23"/>
-      <c r="D198" s="23" t="s">
+      <c r="C198" s="24"/>
+      <c r="D198" s="24" t="s">
         <v>927</v>
       </c>
-      <c r="E198" s="23" t="s">
+      <c r="E198" s="24" t="s">
         <v>928</v>
       </c>
       <c r="F198" s="4"/>
@@ -14165,10 +14179,10 @@
         <v>54</v>
       </c>
       <c r="O198" s="4"/>
-      <c r="P198" s="23" t="s">
+      <c r="P198" s="24" t="s">
         <v>929</v>
       </c>
-      <c r="Q198" s="23"/>
+      <c r="Q198" s="24"/>
       <c r="R198" s="11" t="s">
         <v>930</v>
       </c>
@@ -14182,19 +14196,19 @@
       <c r="Z198" s="4"/>
     </row>
     <row r="199" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="25" t="s">
+      <c r="A199" s="26" t="s">
         <v>931</v>
       </c>
-      <c r="B199" s="25" t="s">
+      <c r="B199" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C199" s="23" t="s">
+      <c r="C199" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D199" s="23" t="s">
+      <c r="D199" s="24" t="s">
         <v>932</v>
       </c>
-      <c r="E199" s="23" t="s">
+      <c r="E199" s="24" t="s">
         <v>908</v>
       </c>
       <c r="F199" s="4"/>
@@ -14238,17 +14252,17 @@
       <c r="Z199" s="4"/>
     </row>
     <row r="200" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="25" t="s">
+      <c r="A200" s="26" t="s">
         <v>933</v>
       </c>
-      <c r="B200" s="25" t="s">
+      <c r="B200" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C200" s="23"/>
-      <c r="D200" s="23" t="s">
+      <c r="C200" s="24"/>
+      <c r="D200" s="24" t="s">
         <v>934</v>
       </c>
-      <c r="E200" s="23" t="s">
+      <c r="E200" s="24" t="s">
         <v>935</v>
       </c>
       <c r="F200" s="4"/>
@@ -14269,10 +14283,10 @@
         <v>54</v>
       </c>
       <c r="O200" s="4"/>
-      <c r="P200" s="23" t="s">
+      <c r="P200" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="Q200" s="23" t="s">
+      <c r="Q200" s="24" t="s">
         <v>936</v>
       </c>
       <c r="R200" s="11" t="s">
@@ -14288,19 +14302,19 @@
       <c r="Z200" s="4"/>
     </row>
     <row r="201" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="25" t="s">
+      <c r="A201" s="26" t="s">
         <v>938</v>
       </c>
-      <c r="B201" s="25" t="s">
+      <c r="B201" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C201" s="23" t="s">
+      <c r="C201" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D201" s="23" t="s">
+      <c r="D201" s="24" t="s">
         <v>939</v>
       </c>
-      <c r="E201" s="23" t="s">
+      <c r="E201" s="24" t="s">
         <v>940</v>
       </c>
       <c r="F201" s="4"/>
@@ -14344,19 +14358,19 @@
       <c r="Z201" s="4"/>
     </row>
     <row r="202" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="25" t="s">
+      <c r="A202" s="26" t="s">
         <v>941</v>
       </c>
-      <c r="B202" s="25" t="s">
+      <c r="B202" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C202" s="23" t="s">
+      <c r="C202" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D202" s="23" t="s">
+      <c r="D202" s="24" t="s">
         <v>942</v>
       </c>
-      <c r="E202" s="23" t="s">
+      <c r="E202" s="24" t="s">
         <v>908</v>
       </c>
       <c r="F202" s="4"/>
@@ -14400,17 +14414,17 @@
       <c r="Z202" s="4"/>
     </row>
     <row r="203" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="25" t="s">
+      <c r="A203" s="26" t="s">
         <v>943</v>
       </c>
-      <c r="B203" s="25" t="s">
+      <c r="B203" s="26" t="s">
         <v>856</v>
       </c>
       <c r="C203" s="4"/>
-      <c r="D203" s="23" t="s">
+      <c r="D203" s="24" t="s">
         <v>944</v>
       </c>
-      <c r="E203" s="23" t="s">
+      <c r="E203" s="24" t="s">
         <v>945</v>
       </c>
       <c r="F203" s="4"/>
@@ -14436,7 +14450,7 @@
       <c r="P203" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="Q203" s="23" t="s">
+      <c r="Q203" s="24" t="s">
         <v>167</v>
       </c>
       <c r="R203" s="11" t="s">
@@ -14452,17 +14466,17 @@
       <c r="Z203" s="4"/>
     </row>
     <row r="204" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A204" s="25" t="s">
+      <c r="A204" s="26" t="s">
         <v>947</v>
       </c>
-      <c r="B204" s="25" t="s">
+      <c r="B204" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C204" s="23"/>
-      <c r="D204" s="23" t="s">
+      <c r="C204" s="24"/>
+      <c r="D204" s="24" t="s">
         <v>948</v>
       </c>
-      <c r="E204" s="23" t="s">
+      <c r="E204" s="24" t="s">
         <v>949</v>
       </c>
       <c r="F204" s="4"/>
@@ -14488,7 +14502,7 @@
       <c r="P204" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q204" s="23" t="s">
+      <c r="Q204" s="24" t="s">
         <v>936</v>
       </c>
       <c r="R204" s="11" t="s">
@@ -14504,17 +14518,17 @@
       <c r="Z204" s="4"/>
     </row>
     <row r="205" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="25" t="s">
+      <c r="A205" s="26" t="s">
         <v>952</v>
       </c>
-      <c r="B205" s="25" t="s">
+      <c r="B205" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C205" s="23"/>
-      <c r="D205" s="26" t="s">
+      <c r="C205" s="24"/>
+      <c r="D205" s="27" t="s">
         <v>953</v>
       </c>
-      <c r="E205" s="23" t="s">
+      <c r="E205" s="24" t="s">
         <v>954</v>
       </c>
       <c r="F205" s="4"/>
@@ -14542,7 +14556,7 @@
       <c r="P205" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="Q205" s="23" t="s">
+      <c r="Q205" s="24" t="s">
         <v>46</v>
       </c>
       <c r="R205" s="11" t="s">
@@ -14558,17 +14572,17 @@
       <c r="Z205" s="4"/>
     </row>
     <row r="206" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="25" t="s">
+      <c r="A206" s="26" t="s">
         <v>956</v>
       </c>
-      <c r="B206" s="25" t="s">
+      <c r="B206" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C206" s="23"/>
-      <c r="D206" s="23" t="s">
+      <c r="C206" s="24"/>
+      <c r="D206" s="24" t="s">
         <v>957</v>
       </c>
-      <c r="E206" s="23" t="s">
+      <c r="E206" s="24" t="s">
         <v>958</v>
       </c>
       <c r="F206" s="4"/>
@@ -14594,7 +14608,7 @@
       <c r="P206" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q206" s="23" t="s">
+      <c r="Q206" s="24" t="s">
         <v>936</v>
       </c>
       <c r="R206" s="11" t="s">
@@ -14610,19 +14624,19 @@
       <c r="Z206" s="4"/>
     </row>
     <row r="207" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="25" t="s">
+      <c r="A207" s="26" t="s">
         <v>960</v>
       </c>
-      <c r="B207" s="25" t="s">
+      <c r="B207" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C207" s="23" t="s">
+      <c r="C207" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D207" s="26" t="s">
+      <c r="D207" s="27" t="s">
         <v>961</v>
       </c>
-      <c r="E207" s="23" t="s">
+      <c r="E207" s="24" t="s">
         <v>962</v>
       </c>
       <c r="F207" s="4"/>
@@ -14666,19 +14680,19 @@
       <c r="Z207" s="4"/>
     </row>
     <row r="208" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="25" t="s">
+      <c r="A208" s="26" t="s">
         <v>963</v>
       </c>
-      <c r="B208" s="25" t="s">
+      <c r="B208" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C208" s="23" t="s">
+      <c r="C208" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D208" s="26" t="s">
+      <c r="D208" s="27" t="s">
         <v>964</v>
       </c>
-      <c r="E208" s="23" t="s">
+      <c r="E208" s="24" t="s">
         <v>965</v>
       </c>
       <c r="F208" s="4"/>
@@ -14722,19 +14736,19 @@
       <c r="Z208" s="4"/>
     </row>
     <row r="209" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="25" t="s">
+      <c r="A209" s="26" t="s">
         <v>966</v>
       </c>
-      <c r="B209" s="25" t="s">
+      <c r="B209" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C209" s="23" t="s">
+      <c r="C209" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D209" s="23" t="s">
+      <c r="D209" s="24" t="s">
         <v>967</v>
       </c>
-      <c r="E209" s="23" t="s">
+      <c r="E209" s="24" t="s">
         <v>968</v>
       </c>
       <c r="F209" s="4"/>
@@ -14778,19 +14792,19 @@
       <c r="Z209" s="4"/>
     </row>
     <row r="210" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="25" t="s">
+      <c r="A210" s="26" t="s">
         <v>969</v>
       </c>
-      <c r="B210" s="25" t="s">
+      <c r="B210" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C210" s="23" t="s">
+      <c r="C210" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D210" s="23" t="s">
+      <c r="D210" s="24" t="s">
         <v>970</v>
       </c>
-      <c r="E210" s="23" t="s">
+      <c r="E210" s="24" t="s">
         <v>971</v>
       </c>
       <c r="F210" s="4"/>
@@ -14834,19 +14848,19 @@
       <c r="Z210" s="4"/>
     </row>
     <row r="211" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="25" t="s">
+      <c r="A211" s="26" t="s">
         <v>972</v>
       </c>
-      <c r="B211" s="25" t="s">
+      <c r="B211" s="26" t="s">
         <v>856</v>
       </c>
-      <c r="C211" s="23" t="s">
+      <c r="C211" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D211" s="23" t="s">
+      <c r="D211" s="24" t="s">
         <v>973</v>
       </c>
-      <c r="E211" s="23" t="s">
+      <c r="E211" s="24" t="s">
         <v>974</v>
       </c>
       <c r="F211" s="4"/>

</xml_diff>